<commit_message>
wp and act cut down to bare min
</commit_message>
<xml_diff>
--- a/src/data/activity_data.xlsx
+++ b/src/data/activity_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Activities"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2555" uniqueCount="786">
   <si>
     <t>ID</t>
   </si>
@@ -2104,9 +2104,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -2164,61 +2161,43 @@
     <t>wp1</t>
   </si>
   <si>
-    <t>Micro-hydro power</t>
-  </si>
-  <si>
     <t>Technology platfroms</t>
   </si>
   <si>
     <t>wp2</t>
   </si>
   <si>
-    <t>Drain Water Heat Recovery</t>
-  </si>
-  <si>
     <t>wp3</t>
   </si>
   <si>
-    <t xml:space="preserve">Smart Network Control </t>
-  </si>
-  <si>
     <t>wp4</t>
   </si>
   <si>
-    <t>Economic and Environmental Impact Assessment</t>
-  </si>
-  <si>
     <t>Policy Support and Guidance</t>
   </si>
   <si>
     <t>wp5</t>
   </si>
   <si>
-    <t>Benchmarking of Energy Efficiency Measures</t>
-  </si>
-  <si>
     <t>wp6</t>
   </si>
   <si>
-    <t>Energy Auditing and Rating</t>
-  </si>
-  <si>
     <t>wp7</t>
   </si>
   <si>
-    <t>Climate Change Impacts and Adaptation</t>
-  </si>
-  <si>
     <t>wp8</t>
   </si>
   <si>
-    <t xml:space="preserve">Smart Specialisation Cluster </t>
-  </si>
-  <si>
     <t>Dissemination and Collaboration</t>
   </si>
   <si>
+    <t>heyo</t>
+  </si>
+  <si>
     <t>WP</t>
+  </si>
+  <si>
+    <t>activity name</t>
   </si>
   <si>
     <t>End Month/ Planned End Date</t>
@@ -2470,6 +2449,9 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2480,22 +2462,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2801,1948 +2780,1948 @@
   </sheetPr>
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>733</v>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="12" t="s">
+        <v>724</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>725</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="10" t="s">
+        <v>726</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>734</v>
+      <c r="E1" s="12" t="s">
+        <v>727</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10">
+        <v>728</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12">
         <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="73.5">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
         <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="154.5">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>737</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
+        <v>730</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
         <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="60">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>739</v>
-      </c>
-      <c r="D5" s="10">
+        <v>732</v>
+      </c>
+      <c r="D5" s="12">
         <v>57</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="114">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10">
+        <v>733</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
         <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="46.5">
+      <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>54</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="12">
         <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="10">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="181.5">
+      <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="12">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>742</v>
-      </c>
-      <c r="D8" s="10">
+        <v>735</v>
+      </c>
+      <c r="D8" s="12">
         <v>38</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="12">
         <v>62</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="10">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="114">
+      <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="12">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="D9" s="10">
+        <v>736</v>
+      </c>
+      <c r="D9" s="12">
         <v>33</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="12">
         <v>78</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="154.5">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="12">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10">
+        <v>737</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12">
         <v>29</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="10">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="127.5">
+      <c r="A11" s="12">
         <v>10</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="12">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>745</v>
-      </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10">
+        <v>738</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12">
         <v>35</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="10">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="114">
+      <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="12">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>746</v>
-      </c>
-      <c r="D12" s="10">
-        <v>1</v>
-      </c>
-      <c r="E12" s="10">
+        <v>739</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12">
         <v>40</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="10">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="87">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="12">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="10">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12">
         <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="114">
+      <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="12">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="D14" s="10">
+        <v>740</v>
+      </c>
+      <c r="D14" s="12">
         <v>42</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="12">
         <v>78</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="181.5">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="10">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10">
+      <c r="D15" s="12">
+        <v>55</v>
+      </c>
+      <c r="E15" s="12">
+        <v>55</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12">
         <v>4</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>748</v>
-      </c>
-      <c r="D15" s="10">
+      <c r="C16" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="D16" s="12">
+        <v>31</v>
+      </c>
+      <c r="E16" s="12">
         <v>55</v>
       </c>
-      <c r="E15" s="10">
-        <v>55</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="10">
-        <v>15</v>
-      </c>
-      <c r="B16" s="10">
+      <c r="F16" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="37.5">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12">
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>749</v>
-      </c>
-      <c r="D16" s="10">
+      <c r="C17" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="D17" s="12">
+        <v>23</v>
+      </c>
+      <c r="E17" s="12">
+        <v>47</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="100.5">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="D18" s="12">
+        <v>35</v>
+      </c>
+      <c r="E18" s="12">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="37.5">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="D19" s="12">
         <v>31</v>
       </c>
-      <c r="E16" s="10">
-        <v>55</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="10">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>750</v>
-      </c>
-      <c r="D17" s="10">
-        <v>23</v>
-      </c>
-      <c r="E17" s="10">
-        <v>47</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="10">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="D18" s="10">
-        <v>35</v>
-      </c>
-      <c r="E18" s="10">
-        <v>64</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="10">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10">
-        <v>4</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>752</v>
-      </c>
-      <c r="D19" s="10">
-        <v>31</v>
-      </c>
-      <c r="E19" s="10">
+      <c r="E19" s="12">
         <v>74</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="10">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="141">
+      <c r="A20" s="12">
         <v>20</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="12">
         <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="12">
         <v>62</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="12">
         <v>62</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="114">
+      <c r="A21" s="12">
         <v>21</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="12">
         <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>753</v>
-      </c>
-      <c r="D21" s="10">
+        <v>746</v>
+      </c>
+      <c r="D21" s="12">
         <v>53</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="12">
         <v>78</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="100.5">
+      <c r="A22" s="12">
         <v>22</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="12">
         <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>754</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="10">
+        <v>747</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" s="12">
         <v>18</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="127.5">
+      <c r="A23" s="12">
         <v>23</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="12">
         <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>755</v>
-      </c>
-      <c r="D23" s="10">
+        <v>748</v>
+      </c>
+      <c r="D23" s="12">
         <v>19</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="12">
         <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="168">
+      <c r="A24" s="12">
         <v>24</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="12">
         <v>7</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D24" s="10">
+        <v>749</v>
+      </c>
+      <c r="D24" s="12">
         <v>18</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="12">
         <v>47</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="60">
+      <c r="A25" s="12">
         <v>25</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="12">
         <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="12">
         <v>57</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="12">
         <v>64</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="168">
+      <c r="A26" s="12">
         <v>26</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="12">
         <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="D26" s="10">
-        <v>1</v>
-      </c>
-      <c r="E26" s="10">
+        <v>750</v>
+      </c>
+      <c r="D26" s="12">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12">
         <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="87">
+      <c r="A27" s="12">
         <v>27</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="12">
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>758</v>
-      </c>
-      <c r="D27" s="10">
+        <v>751</v>
+      </c>
+      <c r="D27" s="12">
         <v>39</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="12">
         <v>39</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="87">
+      <c r="A28" s="12">
         <v>28</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="12">
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>759</v>
-      </c>
-      <c r="D28" s="10">
-        <v>1</v>
-      </c>
-      <c r="E28" s="10">
+        <v>752</v>
+      </c>
+      <c r="D28" s="12">
+        <v>1</v>
+      </c>
+      <c r="E28" s="12">
         <v>78</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="10">
+        <v>729</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="114">
+      <c r="A29" s="12">
         <v>29</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="12">
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="D29" s="10">
-        <v>1</v>
-      </c>
-      <c r="E29" s="10">
+        <v>753</v>
+      </c>
+      <c r="D29" s="12">
+        <v>1</v>
+      </c>
+      <c r="E29" s="12">
         <v>78</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="10">
+      <c r="A30" s="12">
         <v>30</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="12">
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>761</v>
-      </c>
-      <c r="D30" s="10">
+        <v>754</v>
+      </c>
+      <c r="D30" s="12">
         <v>54</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="12">
         <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="10">
+      <c r="A31" s="12">
         <v>31</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="12">
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="12">
         <v>33</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="12">
         <v>33</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="10">
+      <c r="A32" s="12">
         <v>32</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="12">
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="D32" s="10">
+        <v>755</v>
+      </c>
+      <c r="D32" s="12">
         <v>62</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="12">
         <v>78</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="10">
+      <c r="A33" s="12">
         <v>33</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="12">
         <v>8</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D33" s="10">
+        <v>756</v>
+      </c>
+      <c r="D33" s="12">
         <v>62</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="12">
         <v>78</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="10">
+      <c r="A34" s="12">
         <v>34</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="12">
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10">
+        <v>757</v>
+      </c>
+      <c r="D34" s="12">
+        <v>1</v>
+      </c>
+      <c r="E34" s="12">
         <v>52</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="10">
+      <c r="A35" s="12">
         <v>35</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="12">
         <v>3</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="D35" s="10">
+        <v>758</v>
+      </c>
+      <c r="D35" s="12">
         <v>63</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="12">
         <v>63</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="10">
+      <c r="A36" s="12">
         <v>36</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="12">
         <v>6</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="12">
         <v>30</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="12">
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="10">
+      <c r="A37" s="12">
         <v>37</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="12">
         <v>6</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="D37" s="10">
+        <v>759</v>
+      </c>
+      <c r="D37" s="12">
         <v>54</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="12">
         <v>54</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="10">
+      <c r="A38" s="12">
         <v>38</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="12">
         <v>6</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="12">
         <v>43</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="12">
         <v>78</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="10">
+      <c r="A39" s="12">
         <v>39</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="12">
         <v>6</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="12">
         <v>43</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="12">
         <v>70</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="10">
+      <c r="A40" s="12">
         <v>40</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="12">
         <v>6</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="12">
         <v>43</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="12">
         <v>49</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="10">
+      <c r="A41" s="12">
         <v>41</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="12">
         <v>6</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="12">
         <v>55</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="12">
         <v>78</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="10">
+      <c r="A42" s="12">
         <v>42</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="12">
         <v>8</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="12">
         <v>67</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="12">
         <v>78</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="10">
+      <c r="A43" s="12">
         <v>43</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="12">
         <v>2</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="12">
         <v>55</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="12">
         <v>55</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="10">
+      <c r="A44" s="12">
         <v>44</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="12">
         <v>2</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="D44" s="10">
+        <v>760</v>
+      </c>
+      <c r="D44" s="12">
         <v>61</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="12">
         <v>78</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="10">
+      <c r="A45" s="12">
         <v>45</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="12">
         <v>2</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="12">
         <v>21</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="12">
         <v>78</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="10">
+      <c r="A46" s="12">
         <v>46</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="12">
         <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="12">
         <v>41</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="12">
         <v>78</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="10">
+      <c r="A47" s="12">
         <v>47</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="12">
         <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="12">
         <v>56</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="12">
         <v>56</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="10">
+      <c r="A48" s="12">
         <v>48</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="12">
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="12">
         <v>65</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="12">
         <v>78</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="10">
+      <c r="A49" s="12">
         <v>49</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="12">
         <v>2</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="12">
         <v>64</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="12">
         <v>64</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="10">
+      <c r="A50" s="12">
         <v>50</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="12">
         <v>4</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="D50" s="10">
+        <v>761</v>
+      </c>
+      <c r="D50" s="12">
         <v>68</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="12">
         <v>68</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="10">
+      <c r="A51" s="12">
         <v>51</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="12">
         <v>8</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="12">
         <v>2</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="12">
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="10">
+      <c r="A52" s="12">
         <v>52</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="12">
         <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="12">
         <v>14</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="12">
         <v>14</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="10">
+      <c r="A53" s="12">
         <v>53</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="12">
         <v>8</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="12">
         <v>18</v>
       </c>
-      <c r="E53" s="10">
+      <c r="E53" s="12">
         <v>18</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="10">
+      <c r="A54" s="12">
         <v>54</v>
       </c>
-      <c r="B54" s="10">
+      <c r="B54" s="12">
         <v>8</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="12">
         <v>20</v>
       </c>
-      <c r="E54" s="10">
+      <c r="E54" s="12">
         <v>20</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="10">
+      <c r="A55" s="12">
         <v>55</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="12">
         <v>8</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="12">
         <v>26</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55" s="12">
         <v>26</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="10">
+      <c r="A56" s="12">
         <v>56</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="12">
         <v>6</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="D56" s="10">
+        <v>762</v>
+      </c>
+      <c r="D56" s="12">
         <v>65</v>
       </c>
-      <c r="E56" s="10">
+      <c r="E56" s="12">
         <v>78</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="10">
+      <c r="A57" s="12">
         <v>57</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="12">
         <v>6</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>770</v>
-      </c>
-      <c r="D57" s="10">
+        <v>763</v>
+      </c>
+      <c r="D57" s="12">
         <v>60</v>
       </c>
-      <c r="E57" s="10">
+      <c r="E57" s="12">
         <v>78</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="10">
+      <c r="A58" s="12">
         <v>58</v>
       </c>
-      <c r="B58" s="10">
+      <c r="B58" s="12">
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="12">
         <v>58</v>
       </c>
-      <c r="E58" s="10">
+      <c r="E58" s="12">
         <v>60</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="10">
+      <c r="A59" s="12">
         <v>59</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B59" s="12">
         <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="12">
         <v>56</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59" s="12">
         <v>58</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="10">
+      <c r="A60" s="12">
         <v>60</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="12">
         <v>2</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>771</v>
-      </c>
-      <c r="D60" s="10">
+        <v>764</v>
+      </c>
+      <c r="D60" s="12">
         <v>53</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="12">
         <v>78</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="10">
+      <c r="A61" s="12">
         <v>61</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="12">
         <v>6</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="12">
         <v>30</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E61" s="12">
         <v>42</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="10">
+      <c r="A62" s="12">
         <v>62</v>
       </c>
-      <c r="B62" s="10">
+      <c r="B62" s="12">
         <v>6</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>772</v>
-      </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
+        <v>765</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
       <c r="F62" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="10">
+      <c r="A63" s="12">
         <v>63</v>
       </c>
-      <c r="B63" s="10">
+      <c r="B63" s="12">
         <v>7</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>753</v>
-      </c>
-      <c r="D63" s="10">
+        <v>746</v>
+      </c>
+      <c r="D63" s="12">
         <v>19</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63" s="12">
         <v>52</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="10">
+      <c r="A64" s="12">
         <v>64</v>
       </c>
-      <c r="B64" s="10">
+      <c r="B64" s="12">
         <v>8</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>773</v>
-      </c>
-      <c r="D64" s="10">
+        <v>766</v>
+      </c>
+      <c r="D64" s="12">
         <v>46</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="12">
         <v>66</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="10">
+      <c r="A65" s="12">
         <v>65</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B65" s="12">
         <v>4</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="D65" s="10">
+        <v>767</v>
+      </c>
+      <c r="D65" s="12">
         <v>50</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="12">
         <v>62</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="10">
+      <c r="A66" s="12">
         <v>66</v>
       </c>
-      <c r="B66" s="10">
+      <c r="B66" s="12">
         <v>8</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="12">
         <v>67</v>
       </c>
-      <c r="E66" s="10">
+      <c r="E66" s="12">
         <v>68</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="10">
+      <c r="A67" s="12">
         <v>67</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="12">
         <v>5</v>
       </c>
       <c r="C67" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="D67" s="12">
+        <v>14</v>
+      </c>
+      <c r="E67" s="12">
+        <v>35</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="A68" s="12">
+        <v>68</v>
+      </c>
+      <c r="B68" s="12">
+        <v>5</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="D68" s="12">
+        <v>36</v>
+      </c>
+      <c r="E68" s="12">
+        <v>49</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+      <c r="A69" s="12">
+        <v>69</v>
+      </c>
+      <c r="B69" s="12">
+        <v>5</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="D69" s="12">
+        <v>50</v>
+      </c>
+      <c r="E69" s="12">
+        <v>58</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+      <c r="A70" s="12">
+        <v>70</v>
+      </c>
+      <c r="B70" s="12">
+        <v>5</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="D70" s="12">
+        <v>59</v>
+      </c>
+      <c r="E70" s="12">
+        <v>64</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+      <c r="A71" s="12">
+        <v>71</v>
+      </c>
+      <c r="B71" s="12">
+        <v>5</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="D71" s="12">
+        <v>65</v>
+      </c>
+      <c r="E71" s="12">
+        <v>74</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="37.5">
+      <c r="A72" s="12">
+        <v>72</v>
+      </c>
+      <c r="B72" s="12">
+        <v>1</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="D72" s="12">
+        <v>6</v>
+      </c>
+      <c r="E72" s="12">
+        <v>9</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="37.5">
+      <c r="A73" s="12">
+        <v>73</v>
+      </c>
+      <c r="B73" s="12">
+        <v>1</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="D73" s="12">
+        <v>6</v>
+      </c>
+      <c r="E73" s="12">
+        <v>9</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="37.5">
+      <c r="A74" s="12">
+        <v>74</v>
+      </c>
+      <c r="B74" s="12">
+        <v>1</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>775</v>
       </c>
-      <c r="D67" s="10">
-        <v>14</v>
-      </c>
-      <c r="E67" s="10">
-        <v>35</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
-      <c r="A68" s="10">
-        <v>68</v>
-      </c>
-      <c r="B68" s="10">
-        <v>5</v>
-      </c>
-      <c r="C68" s="3" t="s">
+      <c r="D74" s="12">
+        <v>6</v>
+      </c>
+      <c r="E74" s="12">
+        <v>9</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="37.5">
+      <c r="A75" s="12">
+        <v>75</v>
+      </c>
+      <c r="B75" s="12">
+        <v>1</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="D68" s="10">
-        <v>36</v>
-      </c>
-      <c r="E68" s="10">
-        <v>49</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="10">
-        <v>69</v>
-      </c>
-      <c r="B69" s="10">
-        <v>5</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>777</v>
-      </c>
-      <c r="D69" s="10">
-        <v>50</v>
-      </c>
-      <c r="E69" s="10">
-        <v>58</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
-      <c r="A70" s="10">
-        <v>70</v>
-      </c>
-      <c r="B70" s="10">
-        <v>5</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>778</v>
-      </c>
-      <c r="D70" s="10">
-        <v>59</v>
-      </c>
-      <c r="E70" s="10">
-        <v>64</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="10">
-        <v>71</v>
-      </c>
-      <c r="B71" s="10">
-        <v>5</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="D71" s="10">
-        <v>65</v>
-      </c>
-      <c r="E71" s="10">
-        <v>74</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="10">
-        <v>72</v>
-      </c>
-      <c r="B72" s="10">
-        <v>1</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>780</v>
-      </c>
-      <c r="D72" s="10">
+      <c r="D75" s="12">
         <v>6</v>
       </c>
-      <c r="E72" s="10">
+      <c r="E75" s="12">
         <v>9</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
-      <c r="A73" s="10">
-        <v>73</v>
-      </c>
-      <c r="B73" s="10">
-        <v>1</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>781</v>
-      </c>
-      <c r="D73" s="10">
-        <v>6</v>
-      </c>
-      <c r="E73" s="10">
-        <v>9</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="10">
-        <v>74</v>
-      </c>
-      <c r="B74" s="10">
-        <v>1</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>782</v>
-      </c>
-      <c r="D74" s="10">
-        <v>6</v>
-      </c>
-      <c r="E74" s="10">
-        <v>9</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
-      <c r="A75" s="10">
-        <v>75</v>
-      </c>
-      <c r="B75" s="10">
-        <v>1</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="D75" s="10">
-        <v>6</v>
-      </c>
-      <c r="E75" s="10">
-        <v>9</v>
-      </c>
       <c r="F75" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="10">
+      <c r="A76" s="12">
         <v>76</v>
       </c>
-      <c r="B76" s="10">
+      <c r="B76" s="12">
         <v>1</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D76" s="12">
         <v>9</v>
       </c>
-      <c r="E76" s="10">
+      <c r="E76" s="12">
         <v>11</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="37.5">
+      <c r="A77" s="12">
         <v>77</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" s="12">
         <v>1</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>784</v>
-      </c>
-      <c r="D77" s="10">
+        <v>777</v>
+      </c>
+      <c r="D77" s="12">
         <v>12</v>
       </c>
-      <c r="E77" s="10">
+      <c r="E77" s="12">
         <v>13</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="10">
+      <c r="A78" s="12">
         <v>78</v>
       </c>
-      <c r="B78" s="10">
+      <c r="B78" s="12">
         <v>1</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D78" s="10">
-        <v>1</v>
-      </c>
-      <c r="E78" s="10">
+      <c r="D78" s="12">
+        <v>1</v>
+      </c>
+      <c r="E78" s="12">
         <v>3</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="10">
+      <c r="A79" s="12">
         <v>79</v>
       </c>
-      <c r="B79" s="10">
+      <c r="B79" s="12">
         <v>1</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D79" s="10">
+      <c r="D79" s="12">
         <v>21</v>
       </c>
-      <c r="E79" s="10">
+      <c r="E79" s="12">
         <v>22</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
-      <c r="A80" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="37.5">
+      <c r="A80" s="12">
         <v>80</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" s="12">
         <v>1</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>785</v>
-      </c>
-      <c r="D80" s="10">
+        <v>778</v>
+      </c>
+      <c r="D80" s="12">
         <v>12</v>
       </c>
-      <c r="E80" s="10">
+      <c r="E80" s="12">
         <v>14</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
-      <c r="A81" s="10">
+      <c r="A81" s="12">
         <v>81</v>
       </c>
-      <c r="B81" s="10">
+      <c r="B81" s="12">
         <v>1</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D81" s="10">
+      <c r="D81" s="12">
         <v>45</v>
       </c>
-      <c r="E81" s="10">
+      <c r="E81" s="12">
         <v>47</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
-      <c r="A82" s="10">
+      <c r="A82" s="12">
         <v>82</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" s="12">
         <v>1</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D82" s="10">
+      <c r="D82" s="12">
         <v>41</v>
       </c>
-      <c r="E82" s="10">
+      <c r="E82" s="12">
         <v>43</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
-      <c r="A83" s="10">
+      <c r="A83" s="12">
         <v>83</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="12">
         <v>1</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D83" s="10">
+      <c r="D83" s="12">
         <v>43</v>
       </c>
-      <c r="E83" s="10">
+      <c r="E83" s="12">
         <v>44</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
-      <c r="A84" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="37.5">
+      <c r="A84" s="12">
         <v>84</v>
       </c>
-      <c r="B84" s="10">
+      <c r="B84" s="12">
         <v>4</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="D84" s="10">
+        <v>779</v>
+      </c>
+      <c r="D84" s="12">
         <v>31</v>
       </c>
-      <c r="E84" s="10">
+      <c r="E84" s="12">
         <v>64</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
-      <c r="A85" s="10">
+      <c r="A85" s="12">
         <v>85</v>
       </c>
-      <c r="B85" s="10">
+      <c r="B85" s="12">
         <v>2</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D85" s="10">
+      <c r="D85" s="12">
         <v>65</v>
       </c>
-      <c r="E85" s="10">
+      <c r="E85" s="12">
         <v>78</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
-      <c r="A86" s="10">
+      <c r="A86" s="12">
         <v>86</v>
       </c>
-      <c r="B86" s="10">
+      <c r="B86" s="12">
         <v>7</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="D86" s="10">
+        <v>780</v>
+      </c>
+      <c r="D86" s="12">
         <v>65</v>
       </c>
-      <c r="E86" s="10">
+      <c r="E86" s="12">
         <v>78</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
-      <c r="A87" s="10">
+      <c r="A87" s="12">
         <v>87</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B87" s="12">
         <v>7</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D87" s="10">
+      <c r="D87" s="12">
         <v>56</v>
       </c>
-      <c r="E87" s="10">
+      <c r="E87" s="12">
         <v>57</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="10">
+      <c r="A88" s="12">
         <v>88</v>
       </c>
-      <c r="B88" s="10">
+      <c r="B88" s="12">
         <v>4</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D88" s="10">
+      <c r="D88" s="12">
         <v>69</v>
       </c>
-      <c r="E88" s="10">
+      <c r="E88" s="12">
         <v>71</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
-      <c r="A89" s="10">
+      <c r="A89" s="12">
         <v>89</v>
       </c>
-      <c r="B89" s="10">
+      <c r="B89" s="12">
         <v>8</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D89" s="10">
+      <c r="D89" s="12">
         <v>74</v>
       </c>
-      <c r="E89" s="10">
+      <c r="E89" s="12">
         <v>74</v>
       </c>
       <c r="F89" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
-      <c r="A90" s="10">
+      <c r="A90" s="12">
         <v>90</v>
       </c>
-      <c r="B90" s="10">
+      <c r="B90" s="12">
         <v>8</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D90" s="10">
+      <c r="D90" s="12">
         <v>74</v>
       </c>
-      <c r="E90" s="10">
+      <c r="E90" s="12">
         <v>74</v>
       </c>
       <c r="F90" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
-      <c r="A91" s="10">
+      <c r="A91" s="12">
         <v>91</v>
       </c>
-      <c r="B91" s="10">
+      <c r="B91" s="12">
         <v>8</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>788</v>
-      </c>
-      <c r="D91" s="10">
+        <v>781</v>
+      </c>
+      <c r="D91" s="12">
         <v>68</v>
       </c>
-      <c r="E91" s="10"/>
+      <c r="E91" s="12"/>
       <c r="F91" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
-      <c r="A92" s="10">
+      <c r="A92" s="12">
         <v>92</v>
       </c>
-      <c r="B92" s="10">
+      <c r="B92" s="12">
         <v>2</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D92" s="10">
+      <c r="D92" s="12">
         <v>16</v>
       </c>
-      <c r="E92" s="10">
+      <c r="E92" s="12">
         <v>44</v>
       </c>
       <c r="F92" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
-      <c r="A93" s="10">
+      <c r="A93" s="12">
         <v>93</v>
       </c>
-      <c r="B93" s="10">
+      <c r="B93" s="12">
         <v>5</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D93" s="10">
+      <c r="D93" s="12">
         <v>25</v>
       </c>
-      <c r="E93" s="10">
+      <c r="E93" s="12">
         <v>25</v>
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
-      <c r="A94" s="10">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="37.5">
+      <c r="A94" s="12">
         <v>94</v>
       </c>
-      <c r="B94" s="10">
+      <c r="B94" s="12">
         <v>1</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>789</v>
-      </c>
-      <c r="D94" s="10">
+        <v>782</v>
+      </c>
+      <c r="D94" s="12">
         <v>15</v>
       </c>
-      <c r="E94" s="10">
+      <c r="E94" s="12">
         <v>20</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
-      <c r="A95" s="10">
+        <v>731</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="37.5">
+      <c r="A95" s="12">
         <v>95</v>
       </c>
-      <c r="B95" s="10">
+      <c r="B95" s="12">
         <v>1</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>790</v>
-      </c>
-      <c r="D95" s="10">
+        <v>783</v>
+      </c>
+      <c r="D95" s="12">
         <v>25</v>
       </c>
-      <c r="E95" s="10">
+      <c r="E95" s="12">
         <v>25</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
-      <c r="A96" s="10">
+      <c r="A96" s="12">
         <v>96</v>
       </c>
-      <c r="B96" s="10">
+      <c r="B96" s="12">
         <v>8</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D96" s="12">
         <v>75</v>
       </c>
-      <c r="E96" s="10">
+      <c r="E96" s="12">
         <v>78</v>
       </c>
       <c r="F96" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="10">
+      <c r="A97" s="12">
         <v>97</v>
       </c>
-      <c r="B97" s="10">
+      <c r="B97" s="12">
         <v>4</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D97" s="10">
+      <c r="D97" s="12">
         <v>25</v>
       </c>
-      <c r="E97" s="10">
+      <c r="E97" s="12">
         <v>75</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="10">
+      <c r="A98" s="12">
         <v>98</v>
       </c>
-      <c r="B98" s="10">
+      <c r="B98" s="12">
         <v>7</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D98" s="10">
+      <c r="D98" s="12">
         <v>22</v>
       </c>
-      <c r="E98" s="10">
+      <c r="E98" s="12">
         <v>22</v>
       </c>
       <c r="F98" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
-      <c r="A99" s="10">
+      <c r="A99" s="12">
         <v>99</v>
       </c>
-      <c r="B99" s="10">
+      <c r="B99" s="12">
         <v>1</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>792</v>
-      </c>
-      <c r="D99" s="10">
+        <v>785</v>
+      </c>
+      <c r="D99" s="12">
         <v>10</v>
       </c>
-      <c r="E99" s="10">
+      <c r="E99" s="12">
         <v>10</v>
       </c>
       <c r="F99" s="1"/>
@@ -4757,9 +4736,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4768,21 +4747,20 @@
     <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -4801,367 +4779,340 @@
       <c r="E1" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>699</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="12" t="s">
         <v>701</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="12" t="s">
         <v>702</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="12" t="s">
         <v>705</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="12" t="s">
         <v>708</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="12" t="s">
         <v>709</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="12" t="s">
         <v>710</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="12" t="s">
         <v>712</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>713</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>716</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="10">
-        <v>1</v>
-      </c>
-      <c r="J2" s="10">
-        <v>1</v>
-      </c>
-      <c r="K2" s="10">
-        <v>1</v>
-      </c>
-      <c r="L2" s="10">
-        <v>1</v>
-      </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10">
-        <v>1</v>
-      </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="10">
+      <c r="F2" s="12"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="12">
+        <v>1</v>
+      </c>
+      <c r="I2" s="12">
+        <v>1</v>
+      </c>
+      <c r="J2" s="12">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12">
+        <v>1</v>
+      </c>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12">
+        <v>1</v>
+      </c>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="12">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>716</v>
-      </c>
+        <v>714</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="10">
-        <v>1</v>
-      </c>
-      <c r="J3" s="10">
-        <v>1</v>
-      </c>
-      <c r="K3" s="10">
-        <v>1</v>
-      </c>
-      <c r="L3" s="10">
-        <v>1</v>
-      </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10">
-        <v>1</v>
-      </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="10">
+      <c r="F3" s="12"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1</v>
+      </c>
+      <c r="J3" s="12">
+        <v>1</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12">
+        <v>1</v>
+      </c>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="12">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>716</v>
-      </c>
+        <v>714</v>
+      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="10">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10">
-        <v>1</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10">
-        <v>1</v>
-      </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10">
-        <v>1</v>
-      </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="10"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="12">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12">
+        <v>1</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>723</v>
-      </c>
+        <v>718</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="10">
-        <v>1</v>
-      </c>
-      <c r="J5" s="10">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10">
-        <v>1</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1</v>
-      </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10">
-        <v>1</v>
-      </c>
-      <c r="O5" s="10">
-        <v>1</v>
-      </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10">
-        <v>1</v>
-      </c>
-      <c r="R5" s="10">
-        <v>1</v>
-      </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="10">
+      <c r="F5" s="12"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="12">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1</v>
+      </c>
+      <c r="J5" s="12">
+        <v>1</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12">
+        <v>1</v>
+      </c>
+      <c r="N5" s="12">
+        <v>1</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="12">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>723</v>
-      </c>
+        <v>718</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="10">
-        <v>1</v>
-      </c>
-      <c r="J6" s="10">
-        <v>1</v>
-      </c>
-      <c r="K6" s="10">
-        <v>1</v>
-      </c>
-      <c r="L6" s="10">
-        <v>1</v>
-      </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="10"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>723</v>
-      </c>
+        <v>718</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="10">
-        <v>1</v>
-      </c>
-      <c r="J7" s="10">
-        <v>1</v>
-      </c>
-      <c r="K7" s="10">
-        <v>1</v>
-      </c>
-      <c r="L7" s="10">
-        <v>1</v>
-      </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10">
-        <v>1</v>
-      </c>
-      <c r="O7" s="10">
-        <v>1</v>
-      </c>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="10">
+      <c r="F7" s="12"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="12">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12">
+        <v>1</v>
+      </c>
+      <c r="N7" s="12">
+        <v>1</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="12">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>723</v>
-      </c>
+        <v>718</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="10">
-        <v>1</v>
-      </c>
-      <c r="J8" s="10">
-        <v>1</v>
-      </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="10"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="12">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>732</v>
-      </c>
+        <v>723</v>
+      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="10">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10">
-        <v>1</v>
-      </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10">
-        <v>1</v>
-      </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>1</v>
-      </c>
-      <c r="R9" s="10">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1"/>
-      <c r="T9" s="10">
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="12">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12">
+        <v>1</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12">
+        <v>1</v>
+      </c>
+      <c r="P9" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="12">
         <v>1</v>
       </c>
     </row>
@@ -5181,67 +5132,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="51" max="51" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="52" max="52" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="53" max="53" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="54" max="54" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="55" max="55" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="56" max="56" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="57" max="57" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="58" max="58" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="59" max="59" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="60" max="60" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="61" max="61" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -5323,7 +5274,7 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -5436,7 +5387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="370.5" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="370.5" customFormat="1" s="7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>104</v>
@@ -5446,7 +5397,7 @@
       <c r="E3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>106</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -5627,7 +5578,7 @@
       <c r="E4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -6035,7 +5986,7 @@
         <v>176</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="4"/>
@@ -6114,7 +6065,7 @@
       <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="4"/>
@@ -6333,7 +6284,7 @@
         <v>187</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="4"/>
@@ -7231,7 +7182,7 @@
         <v>219</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G24" s="4"/>
@@ -8115,7 +8066,7 @@
         <v>223</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -8774,7 +8725,7 @@
         <v>268</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G45" s="4"/>
@@ -8849,7 +8800,7 @@
         <v>268</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G46" s="4"/>
@@ -9729,7 +9680,7 @@
         <v>268</v>
       </c>
       <c r="E58" s="4"/>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -9810,7 +9761,7 @@
         <v>219</v>
       </c>
       <c r="E59" s="4"/>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G59" s="4"/>
@@ -10337,7 +10288,7 @@
         <v>176</v>
       </c>
       <c r="E66" s="4"/>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G66" s="4"/>
@@ -10708,7 +10659,7 @@
       <c r="E71" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G71" s="4"/>
@@ -10858,7 +10809,7 @@
       <c r="E73" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -15377,7 +15328,7 @@
       <c r="E134" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F134" s="5" t="s">
+      <c r="F134" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G134" s="4"/>
@@ -15624,7 +15575,7 @@
       <c r="E137" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F137" s="5" t="s">
+      <c r="F137" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G137" s="4"/>
@@ -16149,7 +16100,7 @@
         <v>223</v>
       </c>
       <c r="E144" s="4"/>
-      <c r="F144" s="5" t="s">
+      <c r="F144" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G144" s="4"/>
@@ -16295,7 +16246,7 @@
         <v>176</v>
       </c>
       <c r="E146" s="4"/>
-      <c r="F146" s="5" t="s">
+      <c r="F146" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G146" s="4"/>
@@ -18000,7 +17951,7 @@
         <v>263</v>
       </c>
       <c r="E169" s="4"/>
-      <c r="F169" s="5" t="s">
+      <c r="F169" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G169" s="4"/>
@@ -19180,7 +19131,7 @@
         <v>223</v>
       </c>
       <c r="E185" s="4"/>
-      <c r="F185" s="5" t="s">
+      <c r="F185" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G185" s="4"/>
@@ -19776,7 +19727,7 @@
       <c r="E193" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F193" s="5" t="s">
+      <c r="F193" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G193" s="4"/>
@@ -20216,7 +20167,7 @@
       <c r="E199" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F199" s="5" t="s">
+      <c r="F199" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G199" s="4"/>
@@ -20362,7 +20313,7 @@
         <v>176</v>
       </c>
       <c r="E201" s="4"/>
-      <c r="F201" s="5" t="s">
+      <c r="F201" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G201" s="4"/>
@@ -20437,7 +20388,7 @@
       <c r="E202" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F202" s="5" t="s">
+      <c r="F202" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G202" s="4"/>
@@ -20729,7 +20680,7 @@
         <v>314</v>
       </c>
       <c r="E206" s="4"/>
-      <c r="F206" s="5" t="s">
+      <c r="F206" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G206" s="4"/>
@@ -21623,7 +21574,7 @@
         <v>176</v>
       </c>
       <c r="E218" s="4"/>
-      <c r="F218" s="5" t="s">
+      <c r="F218" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G218" s="4"/>

</xml_diff>

<commit_message>
added meta to config
</commit_message>
<xml_diff>
--- a/src/data/activity_data.xlsx
+++ b/src/data/activity_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Activities"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2555" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2622" uniqueCount="810">
   <si>
     <t>ID</t>
   </si>
@@ -2104,288 +2104,353 @@
     <t>id</t>
   </si>
   <si>
+    <t>WP_1</t>
+  </si>
+  <si>
+    <t>WP_2</t>
+  </si>
+  <si>
+    <t>WP_3</t>
+  </si>
+  <si>
+    <t>WP_4</t>
+  </si>
+  <si>
+    <t>WP_5</t>
+  </si>
+  <si>
+    <t>WP_6</t>
+  </si>
+  <si>
+    <t>WP_7</t>
+  </si>
+  <si>
+    <t>WP_8</t>
+  </si>
+  <si>
+    <t>heyo</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>End Month/ Planned End Date</t>
+  </si>
+  <si>
+    <t>Activity description</t>
+  </si>
+  <si>
     <t>category</t>
   </si>
   <si>
-    <t>SDG_1</t>
-  </si>
-  <si>
-    <t>SDG_2</t>
-  </si>
-  <si>
-    <t>SDG_3</t>
-  </si>
-  <si>
-    <t>SDG_4</t>
-  </si>
-  <si>
-    <t>SDG_5</t>
-  </si>
-  <si>
-    <t>SDG_6</t>
-  </si>
-  <si>
-    <t>SDG_7</t>
-  </si>
-  <si>
-    <t>SDG_8</t>
-  </si>
-  <si>
-    <t>SDG_9</t>
-  </si>
-  <si>
-    <t>SDG_10</t>
-  </si>
-  <si>
-    <t>SDG_11</t>
-  </si>
-  <si>
-    <t>SDG_12</t>
-  </si>
-  <si>
-    <t>SDG_13</t>
-  </si>
-  <si>
-    <t>SDG_14</t>
-  </si>
-  <si>
-    <t>SDG_15</t>
-  </si>
-  <si>
-    <t>SDG_16</t>
-  </si>
-  <si>
-    <t>SDG_17</t>
-  </si>
-  <si>
-    <t>wp1</t>
-  </si>
-  <si>
-    <t>Technology platfroms</t>
-  </si>
-  <si>
-    <t>wp2</t>
-  </si>
-  <si>
-    <t>wp3</t>
-  </si>
-  <si>
-    <t>wp4</t>
-  </si>
-  <si>
-    <t>Policy Support and Guidance</t>
-  </si>
-  <si>
-    <t>wp5</t>
-  </si>
-  <si>
-    <t>wp6</t>
-  </si>
-  <si>
-    <t>wp7</t>
-  </si>
-  <si>
-    <t>wp8</t>
-  </si>
-  <si>
-    <t>Dissemination and Collaboration</t>
-  </si>
-  <si>
-    <t>heyo</t>
-  </si>
-  <si>
-    <t>WP</t>
-  </si>
-  <si>
-    <t>activity name</t>
-  </si>
-  <si>
-    <t>End Month/ Planned End Date</t>
-  </si>
-  <si>
     <t>Single/Inter/Trans-disciplinary</t>
   </si>
   <si>
+    <t xml:space="preserve">Design, procurement, installation supervision, commissioning of a 3.3 kW hydro pilot plant at the Blackstairs Water Treatment Plant in Co. Wexford (Ireland) </t>
+  </si>
+  <si>
+    <t>Installation/Demo site</t>
+  </si>
+  <si>
     <t>Transdisciplinary</t>
   </si>
   <si>
-    <t>A model for the extrapolation of the characteristic curves of Pumps as Turbines from a datum Best Efficiency Point</t>
+    <t>Design, procurement, installation supervision, commissioning of a 3.6 kW hydro pilot plant on a site owned by National Trust Wales (UK)</t>
+  </si>
+  <si>
+    <t>Journal publication</t>
+  </si>
+  <si>
+    <t>Publication</t>
   </si>
   <si>
     <t>Single Discipline</t>
   </si>
   <si>
-    <t>BGWS Primary School Webinars</t>
-  </si>
-  <si>
-    <t>Cost model for pumps as turbines in run-of-river and in-pipe microhydropower applications</t>
+    <t>The webinar is a place-based 45 minute on-line workshop for primary school pupils in 4th to 6th class. Topics: it covers the natural and man made water cycle; the Blackstairs GWS scheme details; the MHP system details. The workshop is interactive and engaging with a number of hands-on activities, including a group activity to design and plan for climate action in their schools or communities.</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>A 1 hour long webinar about Low-cost and modular hydro turbines: opportunity, design and results from pilot installations .Since 2011 the research team Trinity College Dublin has been working  on a novel type of low-cost and modular water turbine, consisting of using regular water pumps in reverse as turbines. The webinar will introduce the technology and provide an overview of the locations where it could be beneficial. Also, the results from the various installed pilot plants operating since 2019 will be presented.</t>
   </si>
   <si>
     <t>Interdisciplinary</t>
   </si>
   <si>
-    <t>Design and Year-Long Performance Evaluation of a Pump as Turbine (PAT) Pico-Hydropower Energy Recovery Device in a Water Network</t>
-  </si>
-  <si>
-    <t>Monitoring and maintaining of the Demonstration sites in Ty Mawr and Blackstairs</t>
-  </si>
-  <si>
-    <t>Decentralized drain water heat recovery: A probabilistic method for prediction of wastewater and heating system interaction</t>
-  </si>
-  <si>
-    <t>Decentralized drain water heat recovery from commercial kitchens in the hospitality sector.</t>
-  </si>
-  <si>
-    <t>Spatial and temporal considerations in the performance of wastewater heat recovery systems</t>
-  </si>
-  <si>
-    <t>Ongoing functioning and monitoring of Penrhyn Castle heat recovery system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Webinar: Don't flush money down the kitchen drain! How to recover heat from drain water in commercial kitchens and save costs and emissions. </t>
-  </si>
-  <si>
-    <t>Heat recovery toolkit</t>
-  </si>
-  <si>
-    <t>Emissions down the drain: Balancing life cycle energy and greenhouse gas
-savings with resource use for heat recovery from kitchen drains</t>
-  </si>
-  <si>
-    <t>Circular use of feed by-products from alcohol production mitigates water scarcity</t>
-  </si>
-  <si>
-    <t>Heat recovery and water reuse in micro-distilleries improves eco-efficiency of alcohol
-production</t>
-  </si>
-  <si>
-    <t>Climate change impact assessment for UK and Irish hydropower production</t>
-  </si>
-  <si>
-    <t>Historical climate and streamflow characterisation study for Wales, with publication</t>
-  </si>
-  <si>
-    <t>Climate change impact study for future streamflow and water quality in Wales, with publication</t>
-  </si>
-  <si>
-    <t>Climate change impact assessment study of water resources for hydropower and public water supply in Wales, with publication</t>
-  </si>
-  <si>
-    <t>Implementation of demonstration sites: Blackstairs GWS (IRL); Ty Mwr Wybrant (Wales, UK); Penrhyn Castle (Wales, UK) and ABP Foods (IRL)</t>
-  </si>
-  <si>
-    <t>Tŷ Mawr Wybrnant Pico Hydropower Demonstration  Site Launch</t>
-  </si>
-  <si>
-    <t>Establishment of a Smart Specialisation Cluster and Water-Energy Network</t>
-  </si>
-  <si>
-    <t>Communication activities:  project website; newsletters; Social media: Twitter;Youtube; LinkedIn</t>
-  </si>
-  <si>
-    <t>Sustainability Webinar Series</t>
-  </si>
-  <si>
-    <t>NTW staff engagement and training about the heat recovery system and Penrhyn</t>
-  </si>
-  <si>
-    <t>Visitors engagement with Penrhyn Castle Heat recovery system</t>
-  </si>
-  <si>
-    <t>All DU activities: technological solutions; energy and environmental audits and assessments; climate change impact assessment; action learning activities and communication methods</t>
-  </si>
-  <si>
-    <t>EPANET workshop for NFGWS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expert panel discussion on heat recovery potential of leisure centres.  </t>
-  </si>
-  <si>
-    <t>Grease Trap Heat recovery device development</t>
-  </si>
-  <si>
-    <t>Webinar: Don't flush money down the kitchen drain! How to recover heat from drain water in commercial kitchens and save costs and emissions. Heat Recovery Tool Webinar- 2</t>
-  </si>
-  <si>
-    <t>Climate action hackathon programme in Welsh secondary schools</t>
-  </si>
-  <si>
-    <t>Citizen science project in Irish homes</t>
-  </si>
-  <si>
-    <t>Decentralized vs centralized WWHR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Improving water-related energy efficiency in Denbighshire (DCC) Primary schools. </t>
-  </si>
-  <si>
-    <t>Developing green process innovation through network action learning journal article submission to Creativity &amp; Innovation Management</t>
-  </si>
-  <si>
-    <t>Reducing household greenhouse gas emissions from space and water heating through low-carbon technology: Identifying cost-effective approaches</t>
-  </si>
-  <si>
-    <t>Economic and environmental efficiency of UK and Ireland water companies: Influence of exogenous factors and rurality</t>
-  </si>
-  <si>
-    <t>Key performance indicators to explain energy &amp; economic efficiency across water utilities, and identifying suitable proxies</t>
-  </si>
-  <si>
-    <t>Aligning efficiency benchmarking with sustainable outcomes in the United Kingdom water sector</t>
-  </si>
-  <si>
-    <t>Pitfalls in international benchmarking of energy intensity across wastewater treatment utilities</t>
-  </si>
-  <si>
-    <t>Cross-sector sustainability benchmarking of major utilities in the United Kingdom</t>
-  </si>
-  <si>
-    <t>Feasibility of MHP generation in community-owned rural water supply networks in Ireland
-Case study: Ballacolla network</t>
-  </si>
-  <si>
-    <t>Feasibility of MHP generation in community-owned rural water supply networks in Ireland
-Case study: Blackstairs network</t>
-  </si>
-  <si>
-    <t>Feasibility of MHP generation in community-owned rural water supply networks in Ireland
-Case study: Ballinabrannagh network</t>
-  </si>
-  <si>
-    <t>Feasibility of MHP generation in community-owned rural water supply networks in Ireland
-Case study: Kilanerin network</t>
-  </si>
-  <si>
-    <t>Hydro Project Blaenau Gwent
-Pre feasibility study</t>
-  </si>
-  <si>
-    <t>Preliminary design of a hydropower energy recovery scheme
-Case study: Rathnure tank inlet</t>
-  </si>
-  <si>
-    <t>Introducing a Calculator for the Environmental and Financial
-Potential of DrainWater Heat Recovery in Commercial Kitchens</t>
-  </si>
-  <si>
-    <t>Study on the impact of variation in abstraction licence conditions between England, Wales, Scotland, Northern Ireland, and Ireland on water abstraction for run-of-river hydropower</t>
-  </si>
-  <si>
-    <t>3D tours of demonstration sites</t>
-  </si>
-  <si>
-    <t>Feasibility of MHP generation in community-owned rural water supply networks in Ireland
-Case studies: Ballinguiroe Tankardstown GWS, Coolagh Caherleske GWS, Kilcredan GWS, Killally Ballinrush GWS and Kilriffith Kilmore GWS and Walterstown (plus Moyne and Patrickswell GWSs - unfinished)</t>
-  </si>
-  <si>
-    <t>Mullins Mill, Kells, County Kilkenny
-Hydropower potential assessment</t>
+    <t>This part of the project is related to the ongoing monitoring and maintainance of the two micro-hydropower demonstration sites</t>
+  </si>
+  <si>
+    <t>Journal publication to present the results of spatial and temporal influences in the performance of wastewater heat recovery systems at residence scale in Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal publication assessing the impact of introducing direct drain water heat recovery systems in commercial kitchens in the UK, based on a commercially available heat exchangers. </t>
+  </si>
+  <si>
+    <t>This study illustrates a method to include both the spatial and temporal aspects in the assessment of the operation and feasibility of an effluent heat recovery system at a WWTP. This leads to a more detailed and comprehensive prediction of the actual recovered heat, and thus allows for a more precise prediction of the feasibility of such projects. The application on a case study in Ireland indicated the general practicability of the suggested method as well as the promising potential of wastewater heat recovery, and the role it can play to reach renewable energy and greenhouse gas reduction
+targets.</t>
+  </si>
+  <si>
+    <t>This project concerns the design, planning and installation of the DWHR system at Penrhyn Castle in N Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data recorded at Penrhyn Castle is monitored to assess how much heat is recovered from the system installed in the café </t>
+  </si>
+  <si>
+    <t>Webinar to introduce heat recovery toolkit to public.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development of a heat recovery toolkit for commercial kitchen owners (pubs, restaurants, cafes, canteens etc.) to get an estimate on their individual heat recovery potential from drain water, environmental and cost savings (or trade-offs); to support and facilitate uptake of heat recovery from drain water in commercial kitchens. </t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Exploring the environmental footprint of heat recovery installations for drain water heat recovery from commercial kitchens (Penrhyn castle and in general, kitchens in the UK).</t>
+  </si>
+  <si>
+    <t>Publication: Life Cycle Assessment of whisky (Scotch Single Malt whisky) production and by-product use. Focus on water footprint and carbon emissions.</t>
+  </si>
+  <si>
+    <t>Exploring the environmental and financial benefits (and trade-offs) of recovering heat in a distillery from process and waste flows. Focus on the impact categories climate change (GHG emissions) and water scarcity impacts.</t>
+  </si>
+  <si>
+    <t>A webinar chaired by Sopan Patil, with Richard Dallison as speaker, presenting the results of WP7 work on the impacts of future climate change on water resources in Wales, and the implications for hydropower production. Results for Wales were put in the context of the wider UK, and for other water abstractors.</t>
+  </si>
+  <si>
+    <t>Study investigating how future worst-case scenario climate change will impact on the timing and quantity of streamflow at 585 catchments across the UK and Ireland, and the knock-on implications of such changes for water abstraction at 531 hydropower locations in 178 catchments in England, Wales, Scotland, Ireland &amp; Northern Ireland.</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Study investigating the historical trends in mean and extreme streamflow, temperatures, and precipitation, in five catchments in Wales.</t>
+  </si>
+  <si>
+    <t>Study investigating future trends in mean and extreme streamflow, as well as water quality, for five catchments in Wales, in worst-case scenario future climate change.</t>
+  </si>
+  <si>
+    <t>Study investigating the impacts of future climate change induced streamflow alterations on water available for public water supply and hydropower, using two catchments in Wales as case studies.</t>
+  </si>
+  <si>
+    <t>The webinar is place-based 45 minute on-line workshop for primary school pupils in 4th to 6th class in school served by BGWS. Topics: it covers the natural and man made water cycle; the Blackstairs GWS scheme details; the MHP system details. The workshop is interactive and engaging with a number of hands-on activities, including a group activity to design and plan for climate action in their schools or communities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Four demonstration sites to showcase the techological solutions were planned and implemented as part of Dwr Uisce with the aim of bringing outside of the lab the technology and to demonstrate in practice how they work and how they can benefit the users. Each of the installation at the different demonstration sites underwent a process of lab testing, prototyping, implementation, feedback from other stakeholders involved. The four fall in two main categories: micro-hydropower installations and heat recovery systems. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Official opening of the demonstration site in Tŷ Mawr Wybrnant, Wales (UK) on 21/11/19. The event was about demonstrating a novel technology such as the application of a pump-as-turbine to produce energy from a small stream running along the land, property of the National Trust Wales. The energy produced is used within Ty Mwr to power a dehumidifying system that preserves the first Welsh-translated bible from beign damaged by the dampness. Associated information board remains as a legacy of the project communicting key features to visitors. </t>
+  </si>
+  <si>
+    <t>The SSC and Water-Energy Network aim to facilitate dissemination of information and technology, and collaboration within the network of participating enterprises. The smart specialisation cluster comprises key actors in the sector in Ireland and Wales, supplemented by outside expertise where appropriate. In the context of the Dŵr Uisce project, the smart specialisation cluster can be seen as a learning network of enterprises.</t>
+  </si>
+  <si>
+    <t>Tools for dissemination and for translating research into ordinary speak.</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A series of free sustainability webinars to present the findings, challenges and practical solutions to improving energy efficiency in the water sector. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Official opening of the demonstration site in Blackstairs (Co. Wexford, Ireland) on 02/05/19. The event was about demonstrating a novel technology such as the application of a pump-as-turbine to recover energy in a water supply network managed by a Group water Scheme. The event was used as an intervention to elict knowledge sharing, feedback and dissemination of the idea, in order to accelerate adoption of the technological solution by other suitable water network operators. Associated information board remains as a legacy of the project communicting key features to visitors. </t>
+  </si>
+  <si>
+    <t>We are planning to deliver a short training to staff from NTW to raise awarenss of the installed heat recovery system</t>
+  </si>
+  <si>
+    <t>We developed information boards to share the details of the DWHR system as well as raising awareness of the climate action potential of the system</t>
+  </si>
+  <si>
+    <t>The project aims to improve the long-term sustainability of water supply, treatment and end-use in Ireland and Wales. This improvement is to be achieved through the development of new innovative technology platforms, undertaking economic and environmental impact assessments, and developing policy and best practice guidelines to facilitate the implementation of integrated low-carbon and smart energy solutions. The scope of Dŵr Uisce covers three themes: Technology Platforms; Policy Support and Guidance; and, Dissemination and Collaboration.</t>
+  </si>
+  <si>
+    <t>In person workshop to present the software EPANET to members of the Group Water Schemes and to illustrate the features, possibilities and some potential applications to manage their networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assessing the water-energy efficiency of wet leisure centre stock of a local authority in North Wales. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A panel discussion of experts working in different areas of leisure centre design, development, operation, and management that discussed the potential for existing leisure centres to adopt heat recovery as a means of emissions reductions and costs savings, particularly with respect to Covid-19 and net-zero targets and ambitions. </t>
+  </si>
+  <si>
+    <t>Assessing and quantifying the whole building potential (NZEB) of a community-run rural leisure centre in mid-Wales: case study.</t>
+  </si>
+  <si>
+    <t>Monitoring, assessment and quantification of the water-energy use efficiency and management on resource use, carbon footprint, and water quality of existing swimming pools in North Wales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assessing the water-energy efficiency potential of office water use in a new-build science park on Anglesey, Wales. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assessing and quantifying the water-energy efficiency of a historic pub/ restaurant in Dublin. Case study for heat recovery potential of commercial pub kitchen. </t>
+  </si>
+  <si>
+    <t>The workshop, based on the content and activities developed for BGWS, has been adapted to be used by other GWSs in collaboration with NFGWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-hour long webinar to present the concept and applications of DWHR </t>
+  </si>
+  <si>
+    <t>Development of thermal recovery unit for enhanced heat recaptre from the kitchens wastewater. Furthermore, analyse the impact of heat recovery on grease trap removal efficiency. In near future, new heat exchanger material design in our portfolio to explore with an objective to develop cost-effective and thermally competent system design.</t>
+  </si>
+  <si>
+    <t>This project concerns the design, planning and installation of the DWHR system at ABP in Tipperary, Ireland</t>
+  </si>
+  <si>
+    <t>Data recorded at ABP is monitored to assess how much heat is recovered from the system installed in meat factory</t>
+  </si>
+  <si>
+    <t>1- hour long webinar to present to the general public and SSC memmebrs the output of the benchmarking work</t>
+  </si>
+  <si>
+    <t>The student accommodation has been monitored using tiny tags to assess the heat recovery potential</t>
+  </si>
+  <si>
+    <t>The grease trap has been nmonitored for three weeks in December 2021 to evaluate the temperature of the drainwater leaving the kitchen of the on-site café to assess the heat recovery potential</t>
+  </si>
+  <si>
+    <t>A 1 hour long webinar targeted to the hospitality sector to present DWHR from commercial kitchens in theory and practice by illustrating the demo site at Penrhyn Castle.Also the Heat recovery Tool was presented and participants were given the time to explore the tool and test the feasibility of applying the system in their kitchens using their data.</t>
+  </si>
+  <si>
+    <t>The kick-off event took place in 2016 and included presentations by principal investigators from Trinity College and Bangor University; a structured group discussion in the morning. In the afternoon, two 10-mins presentations were delivered by two demonstrators  Welsh Water and National Trust Wales. Those were followed by a breakout session which included all participants. Three pre-formed goups were assigned as follows: 1 WW representative and 2 NTW representatives. DU team mebers  placed themselves strategically according to individual project responsibility and interests among the three groups to prompt, observe and note the questioning. At the end each participant was given a one-page questionnaire in order to record specific details about each of them in terms of personal and organizational motivation, contribution, interest, and expectations.</t>
+  </si>
+  <si>
+    <t>The first annual Dwr Uisce Conference was hosted by Bangor University in Wales. The theme of the conference aimed to address the challenges we face in relation to water and energy demands in our region. The event included guest speakers on technical, social and governance perspectives on the importance of valuing our water and energy resources, and discussed how we can ensure water and energy security in the future. There was also an opportunity for conference participants to give their own 2-minute perspective on an energy efficiency water sector.</t>
+  </si>
+  <si>
+    <t>This event presented case studies and discussions as to how and why achieving savings, offsetting your demands and identify opportunities for recycling/recovery of energy and water is so important to Wales. The programme had three sections: Savings; Innovation and Offsets. Presentations from stakeholders such as Cadiff University, Centre for Alternative Technologies, Waterwise, Dulas, Bangor University Sustainability Lab, Adnams Southwold Brewery, Aberyswith University as well as two interventions from Dwr Uisce team members were featured.</t>
+  </si>
+  <si>
+    <t>Delivered in collaboration with the National Federation of Group Water Schemes (Ireland). The workshop's objective were:                                                                                                             - To present, discuss and learn from some of actual case-studies in the area of energy recovery from water distribution systems and wastewater systems, using hydropower turbines, pump optimisation and leakage reduction.
+- To build on the research connections between members of Group Water Schemes in Ireland and the Dŵr Uisce project team, legislators and technology providers.
+- To explore opportunities for energy recovery within the member schemes and implementation challenges.
+- To create new learning opportunities and connections for workshop participants.</t>
+  </si>
+  <si>
+    <t>The second annual Dwr Uisce conference was hosted by Trinity College Dublin in Ireland. The theme was 'Water–Energy Innovation' and it addressed the challenges we face in relation to water and energy demands in our region. The programme included three sessions: "Innovation Opportunities", "Innovation Practice" and "Demonstrating Learning".  The event featured a variety of guest speakers from industry, HEI and government sectors in Ireland and Wales. Participants were offered the opportunity to present two-minutes pitches of their water-energy related business or research.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competition programme for key stage 4 and 5 students in Welsh secondary schools. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploring and quantifying the climate action potential from household water-related energy efficiency and contributions from emissions savings on Irish net-zero ambitions and targets. </t>
+  </si>
+  <si>
+    <t>An in person event to launch our Citizen Science project and gather feedback from a community.</t>
+  </si>
+  <si>
+    <t>The Climate Action Hackathon was a 2 -day online event to engaged teenagers aged 15-17 in ideating solutions for water-energy inefficiency. The event was led by Dwr Uisce team members and organised in collaboration with ECO-UNESCO in Dublin. During the 1 hr long pre-hackathon, participants had an opportunity to ask questions to Dwr Uisce team members about their work, the water-energy nexus and the project overall. The hackathon took place on the second day and the participants had 3 hours to work in teams to plan, design and present to the organisers and the other teams an idea that could improve the efficiency of water-related energy use in their schools, cmmunities or on a broader scale. Dwr Uisce team members acted as mentors, providing support and suggesitons throughout the event.</t>
+  </si>
+  <si>
+    <t>Analyzing the difference in available wastewater heating resource across the different scales of an urban wastewater system i.e. how much heat is loss to the environment and does it build a case for decentralized wastewater heat recovery?</t>
+  </si>
+  <si>
+    <t>Assessment and quantification of the water use efficiency and management on resource use in participating schools</t>
+  </si>
+  <si>
+    <t>Study investigating how future worst-case scenario climate change will impact on the timing and quantity of streamflow at 130 catchment accross the UK and Ireland (currently England, Wales, Ireland &amp; Northern Ireland), and the knock-on implications of such changes for water abstraction at 420 hydropower locations.</t>
+  </si>
+  <si>
+    <t>Journal article based upon a conference paper presented at IPDMC 2020.  Describe and reflect on the actions undertaken by a network of stakeholders to co-generate learning from green process innovation.</t>
+  </si>
+  <si>
+    <t>Study investigating cost-effectiveness and emissions savings from replacing conventional heating systems (gas, oil, electricity, LPG and coal) to low-carbon heating systems (ASHP, GSHP, biomass boilers solar PV)</t>
+  </si>
+  <si>
+    <t>We carried out a focus group with a gropu of transition year students to develop the materials for the hackathon porgamme</t>
+  </si>
+  <si>
+    <t>Journal article investigating economic and environmental efficiency of water and sewage companes, with a focus on appropriate methodologies and the factors affecting performance</t>
+  </si>
+  <si>
+    <t>Journal article investigating energy and economic efficiency across water and sewage and water-only companies. Additional focus on assessing how common proxy indicators performed vs. best available</t>
+  </si>
+  <si>
+    <t>Journal article investigating the productivity of the UK water sector over a 6 year period using metrics based on a wider sustainability perspective.</t>
+  </si>
+  <si>
+    <t>Journal article evaluating the energy consumption of wastewater utilities across the globe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal article investigating the efficiency of water and sewage, communication, and energy utilties </t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Ballacolla GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Blackstairs GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Ballinabrannagh GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Kilanerin GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Analysis of three water networks operated by EPS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Analysis of a series of water networks and roadside culverts owned by the Blaenau Gwent municipality to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Analysis of the outfall of the Five Fords WWTP operated by Welsh Water to assess the potential for hydro energy recovery and produce a preliminary design of the hydro site</t>
+  </si>
+  <si>
+    <t>Analysis of the Dodder water supply line operated by Dublin City Council on behalf of Irish Water to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Preliminary design of a picoturbine at the inlet of a storage tank in the Blackstairs GWS</t>
+  </si>
+  <si>
+    <t>Analysis of a pressure reducing station at Boliden Tara Mines to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Analysis of the outfall of the Dairygold WWTP to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Analysis of the inlet of the Fethard WTP to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Publication of the research on the development of a heat recovery toolkit for commercial kitchen owners (pubs, restaurants, cafes, canteens etc.) whcich enables them to get an estimate on their individual heat recovery potential from drain water, environmental and cost savings (or trade-offs).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assess the feasibility of installaing a DWHR system at the Imperial Hotel, Llandudno </t>
+  </si>
+  <si>
+    <t>Study investigating the impact of variation in abstraction licence conditions between England, Wales, Scotland, Northern Ireland, and Ireland on water abstraction for run-of-river hydropower. Study looks at the lost abstraction, and therefore power generation both historically (1985-2015) and for future worst-cast scenario climate change (RCP8.5) affected flows (2021-2080)</t>
+  </si>
+  <si>
+    <t>Hydrological modelling work completed for the Talybont Community Flood Group to identify sub-catchments upstream of the village that are contributing the most to peak flows. Also studied was the impact of tree planting on reducing these peak flood flows.</t>
+  </si>
+  <si>
+    <t>Consultation work for Aber Falls distillery on how to lower their environmental footprint with focus on energy, water use and by-product use.</t>
+  </si>
+  <si>
+    <t>"Feaibility studies for DWHR at the following sites: National Trust, Coolmore Park GWS,Talbot Hotel Stillorgan,Druids Glen Hotel, Ashlawn Nursing Home, Nenagh Swimming Pool, Cooleney Cheese, ABP Food Group,	Noel Lawlor Consulting Engineers"</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Ballinguiroe Tankardstown GWS and Coolagh Caherleske GWS, Kilcredan GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Hydropower potential assessment of the Mullins Mill on the River Kings in Co. Kilkenny</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>Delivery of the Hackathon Programme in Irish Secondary Schools</t>
+  </si>
+  <si>
+    <t>Data collection for the whole production life cycle of whisky at Arbikie distillery, calculation of an environmental footprint and elaboration of suitable measures to reduce the carbon and water footprint by: using by-products or recovering heat from waste and process streams.</t>
   </si>
   <si>
     <t>Inter- and Transdisciplinary</t>
-  </si>
-  <si>
-    <t>Preliminary design of a 4KWh pico hydro scheme powered by a pump-as-turbine for Ogwen Hydro</t>
   </si>
 </sst>
 </file>
@@ -2435,7 +2500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -2472,6 +2537,18 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2778,78 +2855,88 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="1" max="1" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="12" t="s">
-        <v>724</v>
+        <v>703</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>725</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="D1" s="12" t="s">
+        <v>704</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>727</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>728</v>
+      <c r="D1" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>706</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>707</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>708</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>121</v>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
       </c>
       <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>729</v>
+      <c r="E2" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>710</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="73.5">
-      <c r="A3" s="12">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
         <v>39</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>729</v>
+      <c r="E3" s="12" t="s">
+        <v>712</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>710</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="154.5">
@@ -2859,57 +2946,66 @@
       <c r="B4" s="12">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>730</v>
+      <c r="C4" s="15">
+        <v>1</v>
       </c>
       <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
         <v>26</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>731</v>
+      <c r="E4" s="12" t="s">
+        <v>713</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>714</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="60">
       <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>732</v>
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>57</v>
       </c>
       <c r="D5" s="12">
-        <v>57</v>
-      </c>
-      <c r="E5" s="12">
         <v>64</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>729</v>
+      <c r="E5" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="114">
-      <c r="A6" s="12">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
         <v>33</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>731</v>
+      <c r="E6" s="12" t="s">
+        <v>713</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="46.5">
@@ -2919,54 +3015,63 @@
       <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>115</v>
+      <c r="C7" s="13">
+        <v>54</v>
       </c>
       <c r="D7" s="12">
         <v>54</v>
       </c>
-      <c r="E7" s="12">
-        <v>54</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>734</v>
+      <c r="E7" s="12" t="s">
+        <v>718</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="181.5">
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="12">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>735</v>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12">
+        <v>38</v>
       </c>
       <c r="D8" s="12">
-        <v>38</v>
-      </c>
-      <c r="E8" s="12">
         <v>62</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G8" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="114">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="12">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="C9" s="12">
         <v>33</v>
       </c>
-      <c r="E9" s="12">
+      <c r="D9" s="16">
         <v>78</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="E9" s="12" t="s">
+        <v>720</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>710</v>
+      </c>
+      <c r="G9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="154.5">
       <c r="A10" s="12">
@@ -2975,52 +3080,61 @@
       <c r="B10" s="12">
         <v>2</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>737</v>
+      <c r="C10" s="15">
+        <v>1</v>
       </c>
       <c r="D10" s="12">
-        <v>1</v>
-      </c>
-      <c r="E10" s="12">
         <v>29</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="E10" s="12" t="s">
+        <v>721</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>714</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="127.5">
       <c r="A11" s="12">
         <v>10</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>738</v>
+      <c r="C11" s="12">
+        <v>1</v>
       </c>
       <c r="D11" s="12">
-        <v>1</v>
-      </c>
-      <c r="E11" s="12">
         <v>35</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="114">
-      <c r="A12" s="12">
+      <c r="E11" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G11" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="37.5">
+      <c r="A12" s="15">
         <v>11</v>
       </c>
       <c r="B12" s="12">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>739</v>
-      </c>
-      <c r="D12" s="12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="C12" s="12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13">
         <v>40</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="E12" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="87">
       <c r="A13" s="12">
@@ -3029,57 +3143,66 @@
       <c r="B13" s="12">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>125</v>
+      <c r="C13" s="13">
+        <v>1</v>
       </c>
       <c r="D13" s="12">
-        <v>1</v>
-      </c>
-      <c r="E13" s="12">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>729</v>
+      <c r="E13" s="12" t="s">
+        <v>724</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>710</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="114">
       <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="13">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>740</v>
+      <c r="C14" s="12">
+        <v>42</v>
       </c>
       <c r="D14" s="12">
-        <v>42</v>
-      </c>
-      <c r="E14" s="12">
         <v>78</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>734</v>
+      <c r="E14" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>710</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="181.5">
-      <c r="A15" s="12">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="12">
         <v>4</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="D15" s="12">
+      <c r="C15" s="12">
         <v>55</v>
       </c>
-      <c r="E15" s="12">
+      <c r="D15" s="16">
         <v>55</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>734</v>
+      <c r="E15" s="12" t="s">
+        <v>726</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33">
@@ -3089,57 +3212,66 @@
       <c r="B16" s="12">
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>742</v>
+      <c r="C16" s="15">
+        <v>31</v>
       </c>
       <c r="D16" s="12">
-        <v>31</v>
-      </c>
-      <c r="E16" s="12">
         <v>55</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>734</v>
+      <c r="E16" s="12" t="s">
+        <v>727</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>728</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="37.5">
       <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="15">
         <v>4</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>743</v>
+      <c r="C17" s="12">
+        <v>23</v>
       </c>
       <c r="D17" s="12">
-        <v>23</v>
-      </c>
-      <c r="E17" s="12">
         <v>47</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>734</v>
+      <c r="E17" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="100.5">
-      <c r="A18" s="12">
+      <c r="A18" s="15">
         <v>17</v>
       </c>
       <c r="B18" s="12">
         <v>4</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="D18" s="12">
+      <c r="C18" s="12">
         <v>35</v>
       </c>
-      <c r="E18" s="12">
+      <c r="D18" s="13">
         <v>64</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>731</v>
+      <c r="E18" s="12" t="s">
+        <v>730</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="37.5">
@@ -3149,57 +3281,66 @@
       <c r="B19" s="12">
         <v>4</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>745</v>
+      <c r="C19" s="13">
+        <v>31</v>
       </c>
       <c r="D19" s="12">
-        <v>31</v>
-      </c>
-      <c r="E19" s="12">
         <v>74</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>734</v>
+      <c r="E19" s="12" t="s">
+        <v>731</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>714</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="141">
       <c r="A20" s="12">
         <v>20</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="13">
         <v>7</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>119</v>
+      <c r="C20" s="12">
+        <v>62</v>
       </c>
       <c r="D20" s="12">
         <v>62</v>
       </c>
-      <c r="E20" s="12">
-        <v>62</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>729</v>
+      <c r="E20" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="114">
-      <c r="A21" s="12">
+      <c r="A21" s="13">
         <v>21</v>
       </c>
       <c r="B21" s="12">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>746</v>
-      </c>
-      <c r="D21" s="12">
+      <c r="C21" s="12">
         <v>53</v>
       </c>
-      <c r="E21" s="12">
+      <c r="D21" s="16">
         <v>78</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>731</v>
+      <c r="E21" s="12" t="s">
+        <v>733</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="100.5">
@@ -3209,57 +3350,66 @@
       <c r="B22" s="12">
         <v>7</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>747</v>
+      <c r="C22" s="15">
+        <v>1</v>
       </c>
       <c r="D22" s="12">
-        <v>1</v>
-      </c>
-      <c r="E22" s="12">
         <v>18</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>731</v>
+      <c r="E22" s="12" t="s">
+        <v>735</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>734</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="127.5">
       <c r="A23" s="12">
         <v>23</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="15">
         <v>7</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>748</v>
+      <c r="C23" s="12">
+        <v>19</v>
       </c>
       <c r="D23" s="12">
-        <v>19</v>
-      </c>
-      <c r="E23" s="12">
         <v>52</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>731</v>
+      <c r="E23" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="168">
-      <c r="A24" s="12">
+      <c r="A24" s="15">
         <v>24</v>
       </c>
       <c r="B24" s="12">
         <v>7</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>749</v>
-      </c>
-      <c r="D24" s="12">
+      <c r="C24" s="12">
         <v>18</v>
       </c>
-      <c r="E24" s="12">
+      <c r="D24" s="13">
         <v>47</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>731</v>
+      <c r="E24" s="12" t="s">
+        <v>737</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="60">
@@ -3269,57 +3419,66 @@
       <c r="B25" s="12">
         <v>8</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>127</v>
+      <c r="C25" s="13">
+        <v>57</v>
       </c>
       <c r="D25" s="12">
-        <v>57</v>
-      </c>
-      <c r="E25" s="12">
         <v>64</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>729</v>
+      <c r="E25" s="12" t="s">
+        <v>738</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="168">
       <c r="A26" s="12">
         <v>26</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="13">
         <v>8</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>750</v>
+      <c r="C26" s="12">
+        <v>1</v>
       </c>
       <c r="D26" s="12">
-        <v>1</v>
-      </c>
-      <c r="E26" s="12">
         <v>78</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>729</v>
+      <c r="E26" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>710</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="87">
-      <c r="A27" s="12">
+      <c r="A27" s="13">
         <v>27</v>
       </c>
       <c r="B27" s="12">
         <v>8</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="D27" s="12">
+      <c r="C27" s="12">
         <v>39</v>
       </c>
-      <c r="E27" s="12">
+      <c r="D27" s="16">
         <v>39</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>729</v>
+      <c r="E27" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="87">
@@ -3329,57 +3488,66 @@
       <c r="B28" s="12">
         <v>8</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>752</v>
+      <c r="C28" s="15">
+        <v>1</v>
       </c>
       <c r="D28" s="12">
-        <v>1</v>
-      </c>
-      <c r="E28" s="12">
         <v>78</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>729</v>
+      <c r="E28" s="12" t="s">
+        <v>741</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>734</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="114">
       <c r="A29" s="12">
         <v>29</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="15">
         <v>8</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>753</v>
+      <c r="C29" s="12">
+        <v>1</v>
       </c>
       <c r="D29" s="12">
-        <v>1</v>
-      </c>
-      <c r="E29" s="12">
         <v>78</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>734</v>
+      <c r="E29" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>743</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="12">
+      <c r="A30" s="15">
         <v>30</v>
       </c>
       <c r="B30" s="12">
         <v>8</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>754</v>
-      </c>
-      <c r="D30" s="12">
+      <c r="C30" s="12">
         <v>54</v>
       </c>
-      <c r="E30" s="12">
+      <c r="D30" s="13">
         <v>78</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>734</v>
+      <c r="E30" s="12" t="s">
+        <v>744</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -3389,54 +3557,63 @@
       <c r="B31" s="12">
         <v>8</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>110</v>
+      <c r="C31" s="13">
+        <v>33</v>
       </c>
       <c r="D31" s="12">
         <v>33</v>
       </c>
-      <c r="E31" s="12">
-        <v>33</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>729</v>
+      <c r="E31" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="12">
         <v>32</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="13">
         <v>8</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>755</v>
+      <c r="C32" s="12">
+        <v>62</v>
       </c>
       <c r="D32" s="12">
-        <v>62</v>
-      </c>
-      <c r="E32" s="12">
         <v>78</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>743</v>
+      </c>
+      <c r="G32" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="12">
+      <c r="A33" s="13">
         <v>33</v>
       </c>
       <c r="B33" s="12">
         <v>8</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="D33" s="12">
+      <c r="C33" s="12">
         <v>62</v>
       </c>
-      <c r="E33" s="12">
+      <c r="D33" s="16">
         <v>78</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="E33" s="12" t="s">
+        <v>747</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>743</v>
+      </c>
+      <c r="G33" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="12">
@@ -3445,55 +3622,64 @@
       <c r="B34" s="12">
         <v>8</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>757</v>
+      <c r="C34" s="15">
+        <v>1</v>
       </c>
       <c r="D34" s="12">
-        <v>1</v>
-      </c>
-      <c r="E34" s="12">
         <v>52</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>734</v>
+      <c r="E34" s="12" t="s">
+        <v>748</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>714</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="12">
         <v>35</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="15">
         <v>3</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>758</v>
+      <c r="C35" s="12">
+        <v>63</v>
       </c>
       <c r="D35" s="12">
         <v>63</v>
       </c>
-      <c r="E35" s="12">
-        <v>63</v>
-      </c>
-      <c r="F35" s="1"/>
+      <c r="E35" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G35" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="12">
+      <c r="A36" s="15">
         <v>36</v>
       </c>
       <c r="B36" s="12">
         <v>6</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D36" s="12">
+      <c r="C36" s="12">
         <v>30</v>
       </c>
-      <c r="E36" s="12">
+      <c r="D36" s="13">
         <v>42</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="E36" s="12" t="s">
+        <v>750</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>734</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
@@ -3503,57 +3689,66 @@
       <c r="B37" s="12">
         <v>6</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>759</v>
+      <c r="C37" s="13">
+        <v>54</v>
       </c>
       <c r="D37" s="12">
         <v>54</v>
       </c>
-      <c r="E37" s="12">
-        <v>54</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>729</v>
+      <c r="E37" s="12" t="s">
+        <v>751</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="12">
         <v>38</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="13">
         <v>6</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>146</v>
+      <c r="C38" s="12">
+        <v>43</v>
       </c>
       <c r="D38" s="12">
-        <v>43</v>
-      </c>
-      <c r="E38" s="12">
         <v>78</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="E38" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>734</v>
       </c>
+      <c r="G38" s="12" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="12">
+      <c r="A39" s="13">
         <v>39</v>
       </c>
       <c r="B39" s="12">
         <v>6</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="12">
+      <c r="C39" s="12">
         <v>43</v>
       </c>
-      <c r="E39" s="12">
+      <c r="D39" s="16">
         <v>70</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>729</v>
+      <c r="E39" s="12" t="s">
+        <v>753</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
@@ -3563,57 +3758,66 @@
       <c r="B40" s="12">
         <v>6</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>148</v>
+      <c r="C40" s="15">
+        <v>43</v>
       </c>
       <c r="D40" s="12">
-        <v>43</v>
-      </c>
-      <c r="E40" s="12">
         <v>49</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="E40" s="12" t="s">
+        <v>754</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>734</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="12">
         <v>41</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="15">
         <v>6</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>149</v>
+      <c r="C41" s="12">
+        <v>55</v>
       </c>
       <c r="D41" s="12">
-        <v>55</v>
-      </c>
-      <c r="E41" s="12">
         <v>78</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="E41" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="F41" s="12" t="s">
         <v>734</v>
       </c>
+      <c r="G41" s="12" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="12">
+      <c r="A42" s="15">
         <v>42</v>
       </c>
       <c r="B42" s="12">
         <v>8</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="12">
+      <c r="C42" s="12">
         <v>67</v>
       </c>
-      <c r="E42" s="12">
+      <c r="D42" s="13">
         <v>78</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>729</v>
+      <c r="E42" s="12" t="s">
+        <v>756</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
@@ -3623,57 +3827,66 @@
       <c r="B43" s="12">
         <v>2</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>116</v>
+      <c r="C43" s="13">
+        <v>55</v>
       </c>
       <c r="D43" s="12">
         <v>55</v>
       </c>
-      <c r="E43" s="12">
-        <v>55</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>729</v>
+      <c r="E43" s="12" t="s">
+        <v>757</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="12">
         <v>44</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="13">
         <v>2</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>760</v>
+      <c r="C44" s="12">
+        <v>61</v>
       </c>
       <c r="D44" s="12">
-        <v>61</v>
-      </c>
-      <c r="E44" s="12">
         <v>78</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>731</v>
+      <c r="E44" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="12">
+      <c r="A45" s="13">
         <v>45</v>
       </c>
       <c r="B45" s="12">
         <v>2</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" s="12">
+      <c r="C45" s="12">
         <v>21</v>
       </c>
-      <c r="E45" s="12">
+      <c r="D45" s="16">
         <v>78</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>729</v>
+      <c r="E45" s="12" t="s">
+        <v>759</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>710</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -3683,57 +3896,66 @@
       <c r="B46" s="12">
         <v>2</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>123</v>
+      <c r="C46" s="15">
+        <v>41</v>
       </c>
       <c r="D46" s="12">
-        <v>41</v>
-      </c>
-      <c r="E46" s="12">
         <v>78</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>729</v>
+      <c r="E46" s="12" t="s">
+        <v>760</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>710</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="12">
         <v>47</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47" s="15">
         <v>5</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>118</v>
+      <c r="C47" s="12">
+        <v>56</v>
       </c>
       <c r="D47" s="12">
         <v>56</v>
       </c>
-      <c r="E47" s="12">
-        <v>56</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>734</v>
+      <c r="E47" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="12">
+      <c r="A48" s="15">
         <v>48</v>
       </c>
       <c r="B48" s="12">
         <v>2</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D48" s="12">
+      <c r="C48" s="12">
         <v>65</v>
       </c>
-      <c r="E48" s="12">
+      <c r="D48" s="13">
         <v>78</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>729</v>
+      <c r="E48" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -3743,57 +3965,66 @@
       <c r="B49" s="12">
         <v>2</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>144</v>
+      <c r="C49" s="13">
+        <v>64</v>
       </c>
       <c r="D49" s="12">
         <v>64</v>
       </c>
-      <c r="E49" s="12">
-        <v>64</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>729</v>
+      <c r="E49" s="12" t="s">
+        <v>763</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="12">
         <v>50</v>
       </c>
-      <c r="B50" s="12">
+      <c r="B50" s="13">
         <v>4</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>761</v>
+      <c r="C50" s="12">
+        <v>68</v>
       </c>
       <c r="D50" s="12">
         <v>68</v>
       </c>
-      <c r="E50" s="12">
-        <v>68</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>734</v>
+      <c r="E50" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="12">
+      <c r="A51" s="13">
         <v>51</v>
       </c>
       <c r="B51" s="12">
         <v>8</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="12">
+      <c r="C51" s="12">
         <v>2</v>
       </c>
-      <c r="E51" s="12">
+      <c r="D51" s="16">
         <v>2</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>729</v>
+      <c r="E51" s="12" t="s">
+        <v>765</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
@@ -3803,57 +4034,66 @@
       <c r="B52" s="12">
         <v>8</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>106</v>
+      <c r="C52" s="15">
+        <v>14</v>
       </c>
       <c r="D52" s="12">
         <v>14</v>
       </c>
-      <c r="E52" s="12">
-        <v>14</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>729</v>
+      <c r="E52" s="12" t="s">
+        <v>766</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>717</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="12">
         <v>53</v>
       </c>
-      <c r="B53" s="12">
+      <c r="B53" s="15">
         <v>8</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>107</v>
+      <c r="C53" s="12">
+        <v>18</v>
       </c>
       <c r="D53" s="12">
         <v>18</v>
       </c>
-      <c r="E53" s="12">
-        <v>18</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="12">
+      <c r="E53" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="131.25">
+      <c r="A54" s="15">
         <v>54</v>
       </c>
       <c r="B54" s="12">
         <v>8</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="12">
+      <c r="C54" s="12">
         <v>20</v>
       </c>
-      <c r="E54" s="12">
+      <c r="D54" s="13">
         <v>20</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>729</v>
+      <c r="E54" s="12" t="s">
+        <v>768</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
@@ -3863,57 +4103,66 @@
       <c r="B55" s="12">
         <v>8</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>109</v>
+      <c r="C55" s="13">
+        <v>26</v>
       </c>
       <c r="D55" s="12">
         <v>26</v>
       </c>
-      <c r="E55" s="12">
-        <v>26</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>729</v>
+      <c r="E55" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="12">
         <v>56</v>
       </c>
-      <c r="B56" s="12">
+      <c r="B56" s="13">
         <v>6</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>762</v>
+      <c r="C56" s="12">
+        <v>65</v>
       </c>
       <c r="D56" s="12">
-        <v>65</v>
-      </c>
-      <c r="E56" s="12">
         <v>78</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="E56" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="F56" s="12" t="s">
         <v>734</v>
       </c>
+      <c r="G56" s="12" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="12">
+      <c r="A57" s="13">
         <v>57</v>
       </c>
       <c r="B57" s="12">
         <v>6</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D57" s="12">
+      <c r="C57" s="12">
         <v>60</v>
       </c>
-      <c r="E57" s="12">
+      <c r="D57" s="16">
         <v>78</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="E57" s="12" t="s">
+        <v>771</v>
+      </c>
+      <c r="F57" s="12" t="s">
         <v>734</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
@@ -3923,57 +4172,66 @@
       <c r="B58" s="12">
         <v>8</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>113</v>
+      <c r="C58" s="15">
+        <v>58</v>
       </c>
       <c r="D58" s="12">
-        <v>58</v>
-      </c>
-      <c r="E58" s="12">
         <v>60</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>734</v>
+      <c r="E58" s="12" t="s">
+        <v>772</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>717</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="12">
         <v>59</v>
       </c>
-      <c r="B59" s="12">
+      <c r="B59" s="15">
         <v>8</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>129</v>
+      <c r="C59" s="12">
+        <v>56</v>
       </c>
       <c r="D59" s="12">
-        <v>56</v>
-      </c>
-      <c r="E59" s="12">
         <v>58</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>734</v>
+      <c r="E59" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="12">
+      <c r="A60" s="15">
         <v>60</v>
       </c>
       <c r="B60" s="12">
         <v>2</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="D60" s="12">
+      <c r="C60" s="12">
         <v>53</v>
       </c>
-      <c r="E60" s="12">
+      <c r="D60" s="13">
         <v>78</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>731</v>
+      <c r="E60" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
@@ -3983,48 +4241,57 @@
       <c r="B61" s="12">
         <v>6</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>145</v>
+      <c r="C61" s="13">
+        <v>30</v>
       </c>
       <c r="D61" s="12">
-        <v>30</v>
-      </c>
-      <c r="E61" s="12">
         <v>42</v>
       </c>
-      <c r="F61" s="1"/>
+      <c r="E61" s="12" t="s">
+        <v>750</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G61" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="12">
         <v>62</v>
       </c>
-      <c r="B62" s="12">
+      <c r="B62" s="13">
         <v>6</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>765</v>
-      </c>
+      <c r="C62" s="12"/>
       <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G62" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="12">
+      <c r="A63" s="13">
         <v>63</v>
       </c>
       <c r="B63" s="12">
         <v>7</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>746</v>
-      </c>
-      <c r="D63" s="12">
+      <c r="C63" s="12">
         <v>19</v>
       </c>
-      <c r="E63" s="12">
+      <c r="D63" s="16">
         <v>52</v>
       </c>
-      <c r="F63" s="1"/>
+      <c r="E63" s="12" t="s">
+        <v>776</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G63" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="12">
@@ -4033,55 +4300,64 @@
       <c r="B64" s="12">
         <v>8</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>766</v>
+      <c r="C64" s="15">
+        <v>46</v>
       </c>
       <c r="D64" s="12">
-        <v>46</v>
-      </c>
-      <c r="E64" s="12">
         <v>66</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>734</v>
+      <c r="E64" s="12" t="s">
+        <v>777</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>714</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="12">
         <v>65</v>
       </c>
-      <c r="B65" s="12">
+      <c r="B65" s="15">
         <v>4</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>767</v>
+      <c r="C65" s="12">
+        <v>50</v>
       </c>
       <c r="D65" s="12">
-        <v>50</v>
-      </c>
-      <c r="E65" s="12">
         <v>62</v>
       </c>
-      <c r="F65" s="1"/>
+      <c r="E65" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G65" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="12">
+      <c r="A66" s="15">
         <v>66</v>
       </c>
       <c r="B66" s="12">
         <v>8</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D66" s="12">
+      <c r="C66" s="12">
         <v>67</v>
       </c>
-      <c r="E66" s="12">
+      <c r="D66" s="13">
         <v>68</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>729</v>
+      <c r="E66" s="12" t="s">
+        <v>779</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
@@ -4091,57 +4367,66 @@
       <c r="B67" s="12">
         <v>5</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>768</v>
+      <c r="C67" s="13">
+        <v>14</v>
       </c>
       <c r="D67" s="12">
-        <v>14</v>
-      </c>
-      <c r="E67" s="12">
         <v>35</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>734</v>
+      <c r="E67" s="12" t="s">
+        <v>780</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>714</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="12">
         <v>68</v>
       </c>
-      <c r="B68" s="12">
+      <c r="B68" s="13">
         <v>5</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>769</v>
+      <c r="C68" s="12">
+        <v>36</v>
       </c>
       <c r="D68" s="12">
-        <v>36</v>
-      </c>
-      <c r="E68" s="12">
         <v>49</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>734</v>
+      <c r="E68" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="12">
+      <c r="A69" s="13">
         <v>69</v>
       </c>
       <c r="B69" s="12">
         <v>5</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>770</v>
-      </c>
-      <c r="D69" s="12">
+      <c r="C69" s="12">
         <v>50</v>
       </c>
-      <c r="E69" s="12">
+      <c r="D69" s="16">
         <v>58</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>734</v>
+      <c r="E69" s="12" t="s">
+        <v>782</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
@@ -4151,57 +4436,66 @@
       <c r="B70" s="12">
         <v>5</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>771</v>
+      <c r="C70" s="15">
+        <v>59</v>
       </c>
       <c r="D70" s="12">
-        <v>59</v>
-      </c>
-      <c r="E70" s="12">
         <v>64</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>731</v>
+      <c r="E70" s="12" t="s">
+        <v>783</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>714</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="12">
         <v>71</v>
       </c>
-      <c r="B71" s="12">
+      <c r="B71" s="15">
         <v>5</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>772</v>
+      <c r="C71" s="12">
+        <v>65</v>
       </c>
       <c r="D71" s="12">
-        <v>65</v>
-      </c>
-      <c r="E71" s="12">
         <v>74</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>734</v>
+      <c r="E71" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="37.5">
-      <c r="A72" s="12">
+      <c r="A72" s="15">
         <v>72</v>
       </c>
       <c r="B72" s="12">
         <v>1</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>773</v>
-      </c>
-      <c r="D72" s="12">
+      <c r="C72" s="12">
         <v>6</v>
       </c>
-      <c r="E72" s="12">
+      <c r="D72" s="13">
         <v>9</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>731</v>
+      <c r="E72" s="12" t="s">
+        <v>785</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="37.5">
@@ -4211,57 +4505,66 @@
       <c r="B73" s="12">
         <v>1</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>774</v>
+      <c r="C73" s="13">
+        <v>6</v>
       </c>
       <c r="D73" s="12">
-        <v>6</v>
-      </c>
-      <c r="E73" s="12">
         <v>9</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>731</v>
+      <c r="E73" s="12" t="s">
+        <v>787</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="37.5">
       <c r="A74" s="12">
         <v>74</v>
       </c>
-      <c r="B74" s="12">
-        <v>1</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>775</v>
+      <c r="B74" s="13">
+        <v>1</v>
+      </c>
+      <c r="C74" s="12">
+        <v>6</v>
       </c>
       <c r="D74" s="12">
+        <v>9</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="37.5">
+      <c r="A75" s="13">
+        <v>75</v>
+      </c>
+      <c r="B75" s="12">
+        <v>1</v>
+      </c>
+      <c r="C75" s="12">
         <v>6</v>
       </c>
-      <c r="E74" s="12">
+      <c r="D75" s="16">
         <v>9</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="37.5">
-      <c r="A75" s="12">
-        <v>75</v>
-      </c>
-      <c r="B75" s="12">
-        <v>1</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>776</v>
-      </c>
-      <c r="D75" s="12">
-        <v>6</v>
-      </c>
-      <c r="E75" s="12">
-        <v>9</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>731</v>
+      <c r="E75" s="12" t="s">
+        <v>789</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
@@ -4271,57 +4574,66 @@
       <c r="B76" s="12">
         <v>1</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>135</v>
+      <c r="C76" s="15">
+        <v>9</v>
       </c>
       <c r="D76" s="12">
-        <v>9</v>
-      </c>
-      <c r="E76" s="12">
         <v>11</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>731</v>
+      <c r="E76" s="12" t="s">
+        <v>790</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>786</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="37.5">
       <c r="A77" s="12">
         <v>77</v>
       </c>
-      <c r="B77" s="12">
-        <v>1</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>777</v>
+      <c r="B77" s="15">
+        <v>1</v>
+      </c>
+      <c r="C77" s="12">
+        <v>12</v>
       </c>
       <c r="D77" s="12">
-        <v>12</v>
-      </c>
-      <c r="E77" s="12">
         <v>13</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>731</v>
+      <c r="E77" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="12">
+      <c r="A78" s="15">
         <v>78</v>
       </c>
       <c r="B78" s="12">
         <v>1</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D78" s="12">
-        <v>1</v>
-      </c>
-      <c r="E78" s="12">
+      <c r="C78" s="12">
+        <v>1</v>
+      </c>
+      <c r="D78" s="13">
         <v>3</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>731</v>
+      <c r="E78" s="12" t="s">
+        <v>792</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
@@ -4331,57 +4643,66 @@
       <c r="B79" s="12">
         <v>1</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>138</v>
+      <c r="C79" s="13">
+        <v>21</v>
       </c>
       <c r="D79" s="12">
-        <v>21</v>
-      </c>
-      <c r="E79" s="12">
         <v>22</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>731</v>
+      <c r="E79" s="12" t="s">
+        <v>793</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="37.5">
       <c r="A80" s="12">
         <v>80</v>
       </c>
-      <c r="B80" s="12">
-        <v>1</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>778</v>
+      <c r="B80" s="13">
+        <v>1</v>
+      </c>
+      <c r="C80" s="12">
+        <v>12</v>
       </c>
       <c r="D80" s="12">
-        <v>12</v>
-      </c>
-      <c r="E80" s="12">
         <v>14</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>731</v>
+      <c r="E80" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
-      <c r="A81" s="12">
+      <c r="A81" s="13">
         <v>81</v>
       </c>
       <c r="B81" s="12">
         <v>1</v>
       </c>
-      <c r="C81" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D81" s="12">
+      <c r="C81" s="12">
         <v>45</v>
       </c>
-      <c r="E81" s="12">
+      <c r="D81" s="16">
         <v>47</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>731</v>
+      <c r="E81" s="12" t="s">
+        <v>795</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
@@ -4391,57 +4712,66 @@
       <c r="B82" s="12">
         <v>1</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>141</v>
+      <c r="C82" s="15">
+        <v>41</v>
       </c>
       <c r="D82" s="12">
-        <v>41</v>
-      </c>
-      <c r="E82" s="12">
         <v>43</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>731</v>
+      <c r="E82" s="12" t="s">
+        <v>796</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>786</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="12">
         <v>83</v>
       </c>
-      <c r="B83" s="12">
-        <v>1</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>142</v>
+      <c r="B83" s="15">
+        <v>1</v>
+      </c>
+      <c r="C83" s="12">
+        <v>43</v>
       </c>
       <c r="D83" s="12">
-        <v>43</v>
-      </c>
-      <c r="E83" s="12">
         <v>44</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>731</v>
+      <c r="E83" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="F83" s="12" t="s">
+        <v>786</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="37.5">
-      <c r="A84" s="12">
+      <c r="A84" s="15">
         <v>84</v>
       </c>
       <c r="B84" s="12">
         <v>4</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="D84" s="12">
+      <c r="C84" s="12">
         <v>31</v>
       </c>
-      <c r="E84" s="12">
+      <c r="D84" s="13">
         <v>64</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>734</v>
+      <c r="E84" s="12" t="s">
+        <v>798</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
@@ -4451,280 +4781,313 @@
       <c r="B85" s="12">
         <v>2</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>143</v>
+      <c r="C85" s="13">
+        <v>65</v>
       </c>
       <c r="D85" s="12">
+        <v>78</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>799</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+      <c r="A86" s="15">
+        <v>86</v>
+      </c>
+      <c r="B86" s="15">
+        <v>7</v>
+      </c>
+      <c r="C86" s="15">
         <v>65</v>
       </c>
-      <c r="E85" s="12">
+      <c r="D86" s="16">
         <v>78</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
-      <c r="A86" s="12">
-        <v>86</v>
-      </c>
-      <c r="B86" s="12">
+      <c r="E86" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="F86" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+      <c r="A87" s="15">
+        <v>87</v>
+      </c>
+      <c r="B87" s="15">
         <v>7</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>780</v>
-      </c>
-      <c r="D86" s="12">
-        <v>65</v>
-      </c>
-      <c r="E86" s="12">
+      <c r="C87" s="15">
+        <v>56</v>
+      </c>
+      <c r="D87" s="16">
+        <v>57</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+      <c r="A88" s="15">
+        <v>88</v>
+      </c>
+      <c r="B88" s="15">
+        <v>4</v>
+      </c>
+      <c r="C88" s="15">
+        <v>69</v>
+      </c>
+      <c r="D88" s="16">
+        <v>71</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+      <c r="A89" s="15">
+        <v>89</v>
+      </c>
+      <c r="B89" s="15">
+        <v>8</v>
+      </c>
+      <c r="C89" s="15">
+        <v>74</v>
+      </c>
+      <c r="D89" s="16">
+        <v>74</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G89" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+      <c r="A90" s="15">
+        <v>90</v>
+      </c>
+      <c r="B90" s="15">
+        <v>8</v>
+      </c>
+      <c r="C90" s="15">
+        <v>74</v>
+      </c>
+      <c r="D90" s="16">
+        <v>74</v>
+      </c>
+      <c r="E90" s="1"/>
+      <c r="F90" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="G90" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+      <c r="A91" s="15">
+        <v>91</v>
+      </c>
+      <c r="B91" s="15">
+        <v>8</v>
+      </c>
+      <c r="C91" s="15">
+        <v>68</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G91" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+      <c r="A92" s="15">
+        <v>92</v>
+      </c>
+      <c r="B92" s="15">
+        <v>2</v>
+      </c>
+      <c r="C92" s="15">
+        <v>16</v>
+      </c>
+      <c r="D92" s="16">
+        <v>44</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G92" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+      <c r="A93" s="15">
+        <v>93</v>
+      </c>
+      <c r="B93" s="15">
+        <v>5</v>
+      </c>
+      <c r="C93" s="15">
+        <v>25</v>
+      </c>
+      <c r="D93" s="16">
+        <v>25</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G93" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="37.5">
+      <c r="A94" s="15">
+        <v>94</v>
+      </c>
+      <c r="B94" s="15">
+        <v>1</v>
+      </c>
+      <c r="C94" s="15">
+        <v>15</v>
+      </c>
+      <c r="D94" s="16">
+        <v>20</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="37.5">
+      <c r="A95" s="15">
+        <v>95</v>
+      </c>
+      <c r="B95" s="15">
+        <v>1</v>
+      </c>
+      <c r="C95" s="15">
+        <v>25</v>
+      </c>
+      <c r="D95" s="16">
+        <v>25</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>806</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+      <c r="A96" s="15">
+        <v>96</v>
+      </c>
+      <c r="B96" s="15">
+        <v>8</v>
+      </c>
+      <c r="C96" s="15">
+        <v>75</v>
+      </c>
+      <c r="D96" s="16">
         <v>78</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
-      <c r="A87" s="12">
-        <v>87</v>
-      </c>
-      <c r="B87" s="12">
+      <c r="E96" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G96" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+      <c r="A97" s="15">
+        <v>97</v>
+      </c>
+      <c r="B97" s="15">
+        <v>4</v>
+      </c>
+      <c r="C97" s="15">
+        <v>25</v>
+      </c>
+      <c r="D97" s="16">
+        <v>75</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+      <c r="A98" s="15">
+        <v>98</v>
+      </c>
+      <c r="B98" s="15">
         <v>7</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D87" s="12">
-        <v>56</v>
-      </c>
-      <c r="E87" s="12">
-        <v>57</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="12">
-        <v>88</v>
-      </c>
-      <c r="B88" s="12">
-        <v>4</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D88" s="12">
-        <v>69</v>
-      </c>
-      <c r="E88" s="12">
-        <v>71</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
-      <c r="A89" s="12">
-        <v>89</v>
-      </c>
-      <c r="B89" s="12">
-        <v>8</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D89" s="12">
-        <v>74</v>
-      </c>
-      <c r="E89" s="12">
-        <v>74</v>
-      </c>
-      <c r="F89" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
-      <c r="A90" s="12">
-        <v>90</v>
-      </c>
-      <c r="B90" s="12">
-        <v>8</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D90" s="12">
-        <v>74</v>
-      </c>
-      <c r="E90" s="12">
-        <v>74</v>
-      </c>
-      <c r="F90" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
-      <c r="A91" s="12">
-        <v>91</v>
-      </c>
-      <c r="B91" s="12">
-        <v>8</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>781</v>
-      </c>
-      <c r="D91" s="12">
-        <v>68</v>
-      </c>
-      <c r="E91" s="12"/>
-      <c r="F91" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
-      <c r="A92" s="12">
-        <v>92</v>
-      </c>
-      <c r="B92" s="12">
-        <v>2</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D92" s="12">
-        <v>16</v>
-      </c>
-      <c r="E92" s="12">
-        <v>44</v>
-      </c>
-      <c r="F92" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
-      <c r="A93" s="12">
-        <v>93</v>
-      </c>
-      <c r="B93" s="12">
-        <v>5</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D93" s="12">
-        <v>25</v>
-      </c>
-      <c r="E93" s="12">
-        <v>25</v>
-      </c>
-      <c r="F93" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="37.5">
-      <c r="A94" s="12">
-        <v>94</v>
-      </c>
-      <c r="B94" s="12">
-        <v>1</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>782</v>
-      </c>
-      <c r="D94" s="12">
-        <v>15</v>
-      </c>
-      <c r="E94" s="12">
-        <v>20</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="37.5">
-      <c r="A95" s="12">
-        <v>95</v>
-      </c>
-      <c r="B95" s="12">
-        <v>1</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="D95" s="12">
-        <v>25</v>
-      </c>
-      <c r="E95" s="12">
-        <v>25</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
-      <c r="A96" s="12">
-        <v>96</v>
-      </c>
-      <c r="B96" s="12">
-        <v>8</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D96" s="12">
-        <v>75</v>
-      </c>
-      <c r="E96" s="12">
-        <v>78</v>
-      </c>
-      <c r="F96" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="12">
-        <v>97</v>
-      </c>
-      <c r="B97" s="12">
-        <v>4</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D97" s="12">
-        <v>25</v>
-      </c>
-      <c r="E97" s="12">
-        <v>75</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="12">
-        <v>98</v>
-      </c>
-      <c r="B98" s="12">
-        <v>7</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D98" s="12">
+      <c r="C98" s="15">
         <v>22</v>
       </c>
-      <c r="E98" s="12">
+      <c r="D98" s="16">
         <v>22</v>
       </c>
-      <c r="F98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G98" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
-      <c r="A99" s="12">
+      <c r="A99" s="15">
         <v>99</v>
       </c>
-      <c r="B99" s="12">
-        <v>1</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>785</v>
-      </c>
-      <c r="D99" s="12">
+      <c r="B99" s="15">
+        <v>1</v>
+      </c>
+      <c r="C99" s="15">
         <v>10</v>
       </c>
-      <c r="E99" s="12">
+      <c r="D99" s="16">
         <v>10</v>
       </c>
-      <c r="F99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="G99" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4736,384 +5099,58 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>699</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>701</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>702</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>703</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>704</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>705</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>706</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>707</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>708</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>709</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>710</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>712</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="12">
-        <v>1</v>
-      </c>
-      <c r="I2" s="12">
-        <v>1</v>
-      </c>
-      <c r="J2" s="12">
-        <v>1</v>
-      </c>
-      <c r="K2" s="12">
-        <v>1</v>
-      </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12">
-        <v>1</v>
-      </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="12">
-        <v>1</v>
+        <v>695</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="12">
-        <v>1</v>
-      </c>
-      <c r="J3" s="12">
-        <v>1</v>
-      </c>
-      <c r="K3" s="12">
-        <v>1</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12">
-        <v>1</v>
-      </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="12">
-        <v>1</v>
+        <v>696</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="12">
-        <v>1</v>
-      </c>
-      <c r="I4" s="12">
-        <v>1</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12">
-        <v>1</v>
-      </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12">
-        <v>1</v>
-      </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="12"/>
+        <v>697</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="12">
-        <v>1</v>
-      </c>
-      <c r="I5" s="12">
-        <v>1</v>
-      </c>
-      <c r="J5" s="12">
-        <v>1</v>
-      </c>
-      <c r="K5" s="12">
-        <v>1</v>
-      </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12">
-        <v>1</v>
-      </c>
-      <c r="N5" s="12">
-        <v>1</v>
-      </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="12">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="12">
-        <v>1</v>
+        <v>698</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="12">
-        <v>1</v>
-      </c>
-      <c r="I6" s="12">
-        <v>1</v>
-      </c>
-      <c r="J6" s="12">
-        <v>1</v>
-      </c>
-      <c r="K6" s="12">
-        <v>1</v>
-      </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="12"/>
+        <v>699</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="12">
-        <v>1</v>
-      </c>
-      <c r="I7" s="12">
-        <v>1</v>
-      </c>
-      <c r="J7" s="12">
-        <v>1</v>
-      </c>
-      <c r="K7" s="12">
-        <v>1</v>
-      </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12">
-        <v>1</v>
-      </c>
-      <c r="N7" s="12">
-        <v>1</v>
-      </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="12">
-        <v>1</v>
+        <v>700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="12">
-        <v>1</v>
-      </c>
-      <c r="I8" s="12">
-        <v>1</v>
-      </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12">
-        <v>1</v>
-      </c>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="12"/>
+        <v>701</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="12">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="12">
-        <v>1</v>
-      </c>
-      <c r="I9" s="12">
-        <v>1</v>
-      </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12">
-        <v>1</v>
-      </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12">
-        <v>1</v>
-      </c>
-      <c r="P9" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="12">
-        <v>1</v>
-      </c>
-      <c r="R9" s="1"/>
-      <c r="S9" s="12">
-        <v>1</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hide options of no dates are provided
</commit_message>
<xml_diff>
--- a/src/data/activity_data.xlsx
+++ b/src/data/activity_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Activities"/>
@@ -2911,7 +2911,7 @@
   </sheetPr>
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2947,7 +2947,7 @@
         <v>722</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>725</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="73.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>725</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="154.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>729</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="60">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="465">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>725</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="114">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>729</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="46.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>733</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="181.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -5155,7 +5155,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
change how colors work
</commit_message>
<xml_diff>
--- a/src/data/activity_data.xlsx
+++ b/src/data/activity_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4077" uniqueCount="830">
   <si>
     <t>S_ID</t>
   </si>
@@ -2175,6 +2175,15 @@
     <t>england</t>
   </si>
   <si>
+    <t>WP_9</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>testland</t>
+  </si>
+  <si>
     <t>actividad</t>
   </si>
   <si>
@@ -2187,10 +2196,16 @@
     <t>Activity description</t>
   </si>
   <si>
+    <t xml:space="preserve">test </t>
+  </si>
+  <si>
     <t>Single/Inter/Trans-disciplinary</t>
   </si>
   <si>
     <t xml:space="preserve">Design, procurement, installation supervision, commissioning of a 3.3 kW hydro pilot plant at the Blackstairs Water Treatment Plant in Co. Wexford (Ireland) </t>
+  </si>
+  <si>
+    <t>testing data</t>
   </si>
   <si>
     <t>Installation/Demo site</t>
@@ -2495,6 +2510,9 @@
   </si>
   <si>
     <t>Inter- and Transdisciplinary</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -2909,7 +2927,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -2920,31 +2938,35 @@
     <col min="3" max="3" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="14" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>411</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>721</v>
-      </c>
-      <c r="F1" s="16" t="s">
+        <v>724</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>697</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>722</v>
+      <c r="H1" s="16" t="s">
+        <v>726</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
@@ -2961,13 +2983,16 @@
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>723</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>724</v>
+        <v>727</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>725</v>
+        <v>729</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -2984,13 +3009,16 @@
         <v>39</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>726</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>724</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>725</v>
+        <v>731</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>729</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -3007,13 +3035,16 @@
         <v>26</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>727</v>
-      </c>
-      <c r="F4" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>729</v>
+      <c r="G4" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="465">
@@ -3030,13 +3061,16 @@
         <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>730</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>725</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -3053,13 +3087,16 @@
         <v>33</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>727</v>
-      </c>
-      <c r="F6" s="16" t="s">
+        <v>732</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>729</v>
+      <c r="G6" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -3076,13 +3113,16 @@
         <v>54</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>732</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>731</v>
+        <v>737</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>733</v>
+        <v>736</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -3099,12 +3139,15 @@
         <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="F8" s="16" t="s">
+        <v>732</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="H8" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="114">
       <c r="A9" s="15">
@@ -3120,12 +3163,15 @@
         <v>78</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>734</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>724</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>739</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>729</v>
+      </c>
+      <c r="H9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="154.5">
       <c r="A10" s="14">
@@ -3141,12 +3187,15 @@
         <v>29</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>735</v>
-      </c>
-      <c r="F10" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="H10" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="127.5">
       <c r="A11" s="14">
@@ -3162,12 +3211,15 @@
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="F11" s="16" t="s">
+        <v>741</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="H11" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="37.5">
       <c r="A12" s="14">
@@ -3183,12 +3235,15 @@
         <v>40</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>737</v>
-      </c>
-      <c r="F12" s="16" t="s">
+        <v>742</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="H12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="87">
       <c r="A13" s="14">
@@ -3204,13 +3259,16 @@
         <v>42</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>738</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>724</v>
+        <v>743</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>725</v>
+        <v>729</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="114">
@@ -3227,13 +3285,16 @@
         <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>739</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>724</v>
+        <v>744</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>733</v>
+        <v>729</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="181.5">
@@ -3250,13 +3311,16 @@
         <v>55</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>740</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>733</v>
+        <v>745</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33">
@@ -3273,13 +3337,16 @@
         <v>55</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>742</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>733</v>
+        <v>746</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="37.5">
@@ -3296,13 +3363,16 @@
         <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="F17" s="16" t="s">
+        <v>748</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>728</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>733</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="100.5">
@@ -3319,13 +3389,16 @@
         <v>64</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>744</v>
-      </c>
-      <c r="F18" s="16" t="s">
+        <v>749</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>729</v>
+      <c r="G18" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="37.5">
@@ -3342,13 +3415,16 @@
         <v>74</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="F19" s="16" t="s">
+        <v>750</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>728</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>733</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="141">
@@ -3365,13 +3441,16 @@
         <v>62</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>731</v>
+        <v>751</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>725</v>
+        <v>736</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="114">
@@ -3388,13 +3467,16 @@
         <v>78</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>747</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>729</v>
+        <v>752</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="100.5">
@@ -3411,13 +3493,16 @@
         <v>18</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>749</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>729</v>
+        <v>754</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="127.5">
@@ -3434,13 +3519,16 @@
         <v>52</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>748</v>
+        <v>755</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>729</v>
+        <v>753</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="168">
@@ -3457,13 +3545,16 @@
         <v>47</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>751</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>729</v>
+        <v>756</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="60">
@@ -3480,13 +3571,16 @@
         <v>64</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>752</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>731</v>
+        <v>757</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>725</v>
+        <v>736</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="168">
@@ -3503,13 +3597,16 @@
         <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>724</v>
+        <v>758</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>725</v>
+        <v>729</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="87">
@@ -3526,13 +3623,16 @@
         <v>39</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>754</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>725</v>
+        <v>759</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="87">
@@ -3549,13 +3649,16 @@
         <v>78</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>755</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>725</v>
+        <v>760</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="114">
@@ -3572,13 +3675,16 @@
         <v>78</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>757</v>
+        <v>761</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>733</v>
+        <v>762</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
@@ -3595,13 +3701,16 @@
         <v>78</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>758</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>733</v>
+        <v>763</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -3618,13 +3727,16 @@
         <v>33</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>759</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>731</v>
+        <v>764</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>725</v>
+        <v>736</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
@@ -3641,12 +3753,15 @@
         <v>78</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>760</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>757</v>
-      </c>
-      <c r="G32" s="14"/>
+        <v>765</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>762</v>
+      </c>
+      <c r="H32" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="15">
@@ -3662,12 +3777,15 @@
         <v>78</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>761</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>757</v>
-      </c>
-      <c r="G33" s="1"/>
+        <v>766</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>762</v>
+      </c>
+      <c r="H33" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="14">
@@ -3683,13 +3801,16 @@
         <v>52</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>762</v>
-      </c>
-      <c r="F34" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="1" t="s">
         <v>733</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
@@ -3706,12 +3827,15 @@
         <v>63</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G35" s="14"/>
+        <v>768</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H35" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="14">
@@ -3727,13 +3851,16 @@
         <v>42</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>764</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>733</v>
+        <v>769</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
@@ -3750,13 +3877,16 @@
         <v>54</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>765</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>731</v>
+        <v>770</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>725</v>
+        <v>736</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
@@ -3773,13 +3903,16 @@
         <v>78</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>748</v>
+        <v>771</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>733</v>
+        <v>753</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
@@ -3796,13 +3929,16 @@
         <v>70</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>767</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>725</v>
+        <v>772</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
@@ -3819,13 +3955,16 @@
         <v>49</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>768</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>733</v>
+        <v>773</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
@@ -3842,13 +3981,16 @@
         <v>78</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>748</v>
+        <v>774</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>733</v>
+        <v>753</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
@@ -3865,13 +4007,16 @@
         <v>78</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>725</v>
+        <v>775</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
@@ -3888,13 +4033,16 @@
         <v>55</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>771</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>731</v>
+        <v>776</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>725</v>
+        <v>736</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
@@ -3911,13 +4059,16 @@
         <v>78</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>772</v>
-      </c>
-      <c r="F44" s="16" t="s">
+        <v>777</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G44" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="G44" s="16" t="s">
-        <v>729</v>
+      <c r="H44" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
@@ -3934,13 +4085,16 @@
         <v>78</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>773</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>724</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>725</v>
+        <v>778</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>729</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -3957,13 +4111,16 @@
         <v>78</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>774</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>725</v>
+        <v>779</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
@@ -3980,13 +4137,16 @@
         <v>56</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>731</v>
+        <v>780</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>733</v>
+        <v>736</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -4003,13 +4163,16 @@
         <v>78</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>776</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>725</v>
+        <v>781</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -4026,13 +4189,16 @@
         <v>64</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>777</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>748</v>
+        <v>782</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>725</v>
+        <v>753</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -4049,13 +4215,16 @@
         <v>68</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>731</v>
+        <v>783</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>733</v>
+        <v>736</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
@@ -4072,13 +4241,16 @@
         <v>2</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>779</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>725</v>
+        <v>784</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
@@ -4095,13 +4267,16 @@
         <v>14</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>780</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>725</v>
+        <v>785</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
@@ -4118,13 +4293,16 @@
         <v>18</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>731</v>
+        <v>786</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>725</v>
+        <v>736</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="131.25">
@@ -4141,13 +4319,16 @@
         <v>20</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>782</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>725</v>
+        <v>787</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
@@ -4164,13 +4345,16 @@
         <v>26</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>783</v>
-      </c>
-      <c r="F55" s="16" t="s">
-        <v>731</v>
+        <v>788</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>725</v>
+        <v>736</v>
+      </c>
+      <c r="H55" s="16" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
@@ -4187,13 +4371,16 @@
         <v>78</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>784</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>748</v>
+        <v>789</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>733</v>
+        <v>753</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
@@ -4210,13 +4397,16 @@
         <v>78</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>785</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>733</v>
+        <v>790</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
@@ -4233,13 +4423,16 @@
         <v>60</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>786</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>733</v>
+        <v>791</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="H58" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
@@ -4256,13 +4449,16 @@
         <v>58</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="F59" s="16" t="s">
-        <v>731</v>
+        <v>792</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>733</v>
+        <v>736</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
@@ -4279,13 +4475,16 @@
         <v>78</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>788</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>729</v>
+        <v>793</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G60" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
@@ -4302,12 +4501,15 @@
         <v>42</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>764</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G61" s="14"/>
+        <v>769</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H61" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="14">
@@ -4319,12 +4521,15 @@
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G62" s="14"/>
+        <v>794</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H62" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="15">
@@ -4340,12 +4545,15 @@
         <v>52</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>790</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G63" s="1"/>
+        <v>795</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H63" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="14">
@@ -4361,13 +4569,16 @@
         <v>66</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>791</v>
-      </c>
-      <c r="F64" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G64" s="16" t="s">
+      <c r="G64" s="1" t="s">
         <v>733</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
@@ -4384,12 +4595,15 @@
         <v>62</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>792</v>
-      </c>
-      <c r="F65" s="16" t="s">
+        <v>797</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G65" s="14"/>
+      <c r="G65" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="H65" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="14">
@@ -4405,13 +4619,16 @@
         <v>68</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>793</v>
-      </c>
-      <c r="F66" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>725</v>
+        <v>798</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
@@ -4428,13 +4645,16 @@
         <v>35</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>794</v>
-      </c>
-      <c r="F67" s="16" t="s">
+        <v>799</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>728</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>733</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
@@ -4451,13 +4671,16 @@
         <v>49</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="F68" s="16" t="s">
+        <v>800</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>728</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>733</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
@@ -4474,13 +4697,16 @@
         <v>58</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>796</v>
-      </c>
-      <c r="F69" s="16" t="s">
+        <v>801</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="G69" s="16" t="s">
         <v>733</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
@@ -4497,13 +4723,16 @@
         <v>64</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>797</v>
-      </c>
-      <c r="F70" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G70" s="16" t="s">
-        <v>729</v>
+      <c r="G70" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="H70" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
@@ -4520,13 +4749,16 @@
         <v>74</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="F71" s="16" t="s">
+        <v>803</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>728</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>733</v>
+      </c>
+      <c r="H71" s="16" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="37.5">
@@ -4543,13 +4775,16 @@
         <v>9</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>799</v>
-      </c>
-      <c r="F72" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>729</v>
+        <v>804</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="37.5">
@@ -4566,13 +4801,16 @@
         <v>9</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>801</v>
-      </c>
-      <c r="F73" s="16" t="s">
-        <v>800</v>
+        <v>806</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>729</v>
+        <v>805</v>
+      </c>
+      <c r="H73" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="37.5">
@@ -4589,13 +4827,16 @@
         <v>9</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>802</v>
-      </c>
-      <c r="F74" s="16" t="s">
-        <v>800</v>
+        <v>807</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G74" s="16" t="s">
-        <v>729</v>
+        <v>805</v>
+      </c>
+      <c r="H74" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="37.5">
@@ -4612,13 +4853,16 @@
         <v>9</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>803</v>
-      </c>
-      <c r="F75" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>729</v>
+        <v>808</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
@@ -4635,13 +4879,16 @@
         <v>11</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>804</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="G76" s="16" t="s">
-        <v>729</v>
+        <v>809</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H76" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="37.5">
@@ -4658,13 +4905,16 @@
         <v>13</v>
       </c>
       <c r="E77" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G77" s="16" t="s">
         <v>805</v>
       </c>
-      <c r="F77" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G77" s="16" t="s">
-        <v>729</v>
+      <c r="H77" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
@@ -4681,13 +4931,16 @@
         <v>3</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>806</v>
-      </c>
-      <c r="F78" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>729</v>
+        <v>811</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G78" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
@@ -4704,13 +4957,16 @@
         <v>22</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>807</v>
-      </c>
-      <c r="F79" s="16" t="s">
-        <v>800</v>
+        <v>812</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G79" s="16" t="s">
-        <v>729</v>
+        <v>805</v>
+      </c>
+      <c r="H79" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="37.5">
@@ -4727,13 +4983,16 @@
         <v>14</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>808</v>
-      </c>
-      <c r="F80" s="16" t="s">
-        <v>800</v>
+        <v>813</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>729</v>
+        <v>805</v>
+      </c>
+      <c r="H80" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
@@ -4750,13 +5009,16 @@
         <v>47</v>
       </c>
       <c r="E81" s="16" t="s">
-        <v>809</v>
-      </c>
-      <c r="F81" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>729</v>
+        <v>814</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G81" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
@@ -4773,13 +5035,16 @@
         <v>43</v>
       </c>
       <c r="E82" s="16" t="s">
-        <v>810</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="G82" s="16" t="s">
-        <v>729</v>
+        <v>815</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
@@ -4796,13 +5061,16 @@
         <v>44</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>811</v>
-      </c>
-      <c r="F83" s="16" t="s">
-        <v>800</v>
+        <v>816</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>729</v>
+        <v>805</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="37.5">
@@ -4819,13 +5087,16 @@
         <v>64</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>812</v>
-      </c>
-      <c r="F84" s="16" t="s">
+        <v>817</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G84" s="16" t="s">
         <v>733</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>738</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
@@ -4842,13 +5113,16 @@
         <v>78</v>
       </c>
       <c r="E85" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="F85" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>725</v>
+        <v>818</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G85" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
@@ -4865,13 +5139,16 @@
         <v>78</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="F86" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>729</v>
+        <v>819</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G86" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -4888,13 +5165,16 @@
         <v>57</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>815</v>
-      </c>
-      <c r="F87" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>725</v>
+        <v>820</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G87" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
@@ -4911,13 +5191,16 @@
         <v>71</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>816</v>
-      </c>
-      <c r="F88" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>725</v>
+        <v>821</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G88" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
@@ -4934,10 +5217,13 @@
         <v>74</v>
       </c>
       <c r="E89" s="2"/>
-      <c r="F89" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G89" s="2"/>
+      <c r="F89" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G89" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H89" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="14">
@@ -4953,10 +5239,13 @@
         <v>74</v>
       </c>
       <c r="E90" s="2"/>
-      <c r="F90" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="G90" s="2"/>
+      <c r="F90" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G90" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="H90" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="14">
@@ -4970,10 +5259,13 @@
       </c>
       <c r="D91" s="14"/>
       <c r="E91" s="2"/>
-      <c r="F91" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G91" s="2"/>
+      <c r="F91" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G91" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H91" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="14">
@@ -4989,12 +5281,15 @@
         <v>44</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>817</v>
-      </c>
-      <c r="F92" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G92" s="2"/>
+        <v>822</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G92" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H92" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="14">
@@ -5010,10 +5305,13 @@
         <v>25</v>
       </c>
       <c r="E93" s="2"/>
-      <c r="F93" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G93" s="2"/>
+      <c r="F93" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G93" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H93" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="37.5">
       <c r="A94" s="14">
@@ -5029,13 +5327,16 @@
         <v>20</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>818</v>
-      </c>
-      <c r="F94" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>729</v>
+        <v>823</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G94" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="37.5">
@@ -5052,13 +5353,16 @@
         <v>25</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>819</v>
-      </c>
-      <c r="F95" s="16" t="s">
-        <v>820</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>729</v>
+        <v>824</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G95" s="16" t="s">
+        <v>825</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>734</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
@@ -5075,12 +5379,15 @@
         <v>78</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="F96" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G96" s="2"/>
+        <v>826</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G96" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H96" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="14">
@@ -5096,13 +5403,16 @@
         <v>75</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="F97" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>823</v>
+        <v>827</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G97" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>828</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
@@ -5119,10 +5429,13 @@
         <v>22</v>
       </c>
       <c r="E98" s="2"/>
-      <c r="F98" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G98" s="2"/>
+      <c r="F98" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G98" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H98" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="14">
@@ -5138,10 +5451,37 @@
         <v>10</v>
       </c>
       <c r="E99" s="2"/>
-      <c r="F99" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="G99" s="2"/>
+      <c r="F99" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G99" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="H99" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+      <c r="A100" s="14">
+        <v>100</v>
+      </c>
+      <c r="B100" s="14">
+        <v>9</v>
+      </c>
+      <c r="C100" s="14">
+        <v>3</v>
+      </c>
+      <c r="D100" s="14">
+        <v>6</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="G100" s="16" t="s">
+        <v>829</v>
+      </c>
+      <c r="H100" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5153,7 +5493,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5261,6 +5601,17 @@
       </c>
       <c r="C9" s="2" t="s">
         <v>717</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="15.75">
+      <c r="A10" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle none dates whn data is first parsed
</commit_message>
<xml_diff>
--- a/src/data/activity_data.xlsx
+++ b/src/data/activity_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Activities"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4328" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4326" uniqueCount="837">
   <si>
     <t>S_ID</t>
   </si>
@@ -2961,7 +2961,7 @@
   </sheetPr>
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -51658,7 +51658,7 @@
   </sheetPr>
   <dimension ref="A1:D235"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -54072,7 +54072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
       <c r="A173" s="1" t="s">
         <v>239</v>
       </c>
@@ -54086,7 +54086,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
       <c r="A174" s="1" t="s">
         <v>240</v>
       </c>
@@ -54100,7 +54100,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
       <c r="A175" s="1" t="s">
         <v>241</v>
       </c>
@@ -54114,7 +54114,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5">
       <c r="A176" s="1" t="s">
         <v>242</v>
       </c>
@@ -54128,7 +54128,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5">
       <c r="A177" s="1" t="s">
         <v>243</v>
       </c>
@@ -54142,7 +54142,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="19.5">
       <c r="A178" s="1" t="s">
         <v>244</v>
       </c>
@@ -54156,7 +54156,7 @@
         <v>237</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="19.5">
       <c r="A179" s="1" t="s">
         <v>245</v>
       </c>
@@ -54170,7 +54170,7 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="19.5">
       <c r="A180" s="1" t="s">
         <v>246</v>
       </c>
@@ -54184,7 +54184,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="19.5">
       <c r="A181" s="1" t="s">
         <v>247</v>
       </c>
@@ -54198,7 +54198,7 @@
         <v>235</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="19.5">
       <c r="A182" s="1" t="s">
         <v>248</v>
       </c>
@@ -54212,7 +54212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="19.5">
       <c r="A183" s="1" t="s">
         <v>249</v>
       </c>
@@ -54226,7 +54226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="19.5">
       <c r="A184" s="1" t="s">
         <v>250</v>
       </c>
@@ -54240,7 +54240,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5">
       <c r="A185" s="1" t="s">
         <v>251</v>
       </c>
@@ -54254,7 +54254,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="19.5">
       <c r="A186" s="1" t="s">
         <v>252</v>
       </c>
@@ -54268,7 +54268,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="19.5">
       <c r="A187" s="1" t="s">
         <v>253</v>
       </c>
@@ -54282,7 +54282,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="19.5">
       <c r="A188" s="1" t="s">
         <v>254</v>
       </c>
@@ -54296,7 +54296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="19.5">
       <c r="A189" s="1" t="s">
         <v>255</v>
       </c>
@@ -54310,7 +54310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="19.5">
       <c r="A190" s="1" t="s">
         <v>256</v>
       </c>
@@ -54324,7 +54324,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="19.5">
       <c r="A191" s="1" t="s">
         <v>257</v>
       </c>
@@ -54338,7 +54338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="19.5">
       <c r="A192" s="1" t="s">
         <v>258</v>
       </c>
@@ -54352,7 +54352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="19.5">
       <c r="A193" s="1" t="s">
         <v>259</v>
       </c>
@@ -54366,7 +54366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="19.5">
       <c r="A194" s="1" t="s">
         <v>260</v>
       </c>
@@ -54380,7 +54380,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="19.5">
       <c r="A195" s="1" t="s">
         <v>261</v>
       </c>
@@ -54394,7 +54394,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5">
       <c r="A196" s="1" t="s">
         <v>262</v>
       </c>
@@ -54408,7 +54408,7 @@
         <v>263</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="19.5">
       <c r="A197" s="1" t="s">
         <v>264</v>
       </c>
@@ -54422,7 +54422,7 @@
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="19.5">
       <c r="A198" s="1" t="s">
         <v>265</v>
       </c>
@@ -54436,7 +54436,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="19.5">
       <c r="A199" s="1" t="s">
         <v>266</v>
       </c>
@@ -54450,7 +54450,7 @@
         <v>267</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="19.5">
       <c r="A200" s="1" t="s">
         <v>268</v>
       </c>
@@ -54464,7 +54464,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="19.5">
       <c r="A201" s="1" t="s">
         <v>269</v>
       </c>
@@ -54931,9 +54931,7 @@
         <v>308</v>
       </c>
       <c r="B234" s="2"/>
-      <c r="C234" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C234" s="2"/>
       <c r="D234" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="18.75">
@@ -54941,9 +54939,7 @@
         <v>309</v>
       </c>
       <c r="B235" s="2"/>
-      <c r="C235" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C235" s="2"/>
       <c r="D235" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sdgs as optional extra for activities
</commit_message>
<xml_diff>
--- a/src/data/activity_data.xlsx
+++ b/src/data/activity_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4326" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4426" uniqueCount="936">
   <si>
     <t>S_ID</t>
   </si>
@@ -2220,6 +2220,9 @@
     <t>start date</t>
   </si>
   <si>
+    <t>ODD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Design, procurement, installation supervision, commissioning of a 3.3 kW hydro pilot plant at the Blackstairs Water Treatment Plant in Co. Wexford (Ireland) </t>
   </si>
   <si>
@@ -2235,9 +2238,15 @@
     <t>2019-05-31</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Design, procurement, installation supervision, commissioning of a 3.6 kW hydro pilot plant on a site owned by National Trust Wales (UK)</t>
   </si>
   <si>
+    <t>3,4,6</t>
+  </si>
+  <si>
     <t>Journal publication</t>
   </si>
   <si>
@@ -2247,161 +2256,308 @@
     <t>Single Discipline</t>
   </si>
   <si>
+    <t>2,6,7,8,9</t>
+  </si>
+  <si>
     <t>The webinar is a place-based 45 minute on-line workshop for primary school pupils in 4th to 6th class. Topics: it covers the natural and man made water cycle; the Blackstairs GWS scheme details; the MHP system details. The workshop is interactive and engaging with a number of hands-on activities, including a group activity to design and plan for climate action in their schools or communities.</t>
   </si>
   <si>
     <t>Event</t>
   </si>
   <si>
+    <t>1,3,4,5,6</t>
+  </si>
+  <si>
+    <t>2,1,6</t>
+  </si>
+  <si>
     <t>A 1 hour long webinar about Low-cost and modular hydro turbines: opportunity, design and results from pilot installations .Since 2011 the research team Trinity College Dublin has been working  on a novel type of low-cost and modular water turbine, consisting of using regular water pumps in reverse as turbines. The webinar will introduce the technology and provide an overview of the locations where it could be beneficial. Also, the results from the various installed pilot plants operating since 2019 will be presented.</t>
   </si>
   <si>
     <t>Interdisciplinary</t>
   </si>
   <si>
+    <t>13,5,17</t>
+  </si>
+  <si>
+    <t>2,16,14</t>
+  </si>
+  <si>
     <t>This part of the project is related to the ongoing monitoring and maintainance of the two micro-hydropower demonstration sites</t>
   </si>
   <si>
+    <t>1,2,4</t>
+  </si>
+  <si>
     <t>Journal publication to present the results of spatial and temporal influences in the performance of wastewater heat recovery systems at residence scale in Ireland</t>
   </si>
   <si>
+    <t>3,4,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Journal publication assessing the impact of introducing direct drain water heat recovery systems in commercial kitchens in the UK, based on a commercially available heat exchangers. </t>
+  </si>
+  <si>
+    <t>2,6,7,8,10</t>
   </si>
   <si>
     <t>This study illustrates a method to include both the spatial and temporal aspects in the assessment of the operation and feasibility of an effluent heat recovery system at a WWTP. This leads to a more detailed and comprehensive prediction of the actual recovered heat, and thus allows for a more precise prediction of the feasibility of such projects. The application on a case study in Ireland indicated the general practicability of the suggested method as well as the promising potential of wastewater heat recovery, and the role it can play to reach renewable energy and greenhouse gas reduction
 targets.</t>
   </si>
   <si>
+    <t>1,3,4,5,7</t>
+  </si>
+  <si>
     <t>This project concerns the design, planning and installation of the DWHR system at Penrhyn Castle in N Wales</t>
   </si>
   <si>
+    <t>2,1,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data recorded at Penrhyn Castle is monitored to assess how much heat is recovered from the system installed in the café </t>
   </si>
   <si>
+    <t>13,5,18</t>
+  </si>
+  <si>
     <t>Webinar to introduce heat recovery toolkit to public.</t>
   </si>
   <si>
+    <t>2,16,15</t>
+  </si>
+  <si>
     <t xml:space="preserve">Development of a heat recovery toolkit for commercial kitchen owners (pubs, restaurants, cafes, canteens etc.) to get an estimate on their individual heat recovery potential from drain water, environmental and cost savings (or trade-offs); to support and facilitate uptake of heat recovery from drain water in commercial kitchens. </t>
   </si>
   <si>
     <t>Tool</t>
   </si>
   <si>
+    <t>1,2,5</t>
+  </si>
+  <si>
     <t>Exploring the environmental footprint of heat recovery installations for drain water heat recovery from commercial kitchens (Penrhyn castle and in general, kitchens in the UK).</t>
   </si>
   <si>
+    <t>3,4,8</t>
+  </si>
+  <si>
     <t>Publication: Life Cycle Assessment of whisky (Scotch Single Malt whisky) production and by-product use. Focus on water footprint and carbon emissions.</t>
   </si>
   <si>
+    <t>2,6,7,8,11</t>
+  </si>
+  <si>
     <t>Exploring the environmental and financial benefits (and trade-offs) of recovering heat in a distillery from process and waste flows. Focus on the impact categories climate change (GHG emissions) and water scarcity impacts.</t>
   </si>
   <si>
+    <t>1,3,4,5,8</t>
+  </si>
+  <si>
     <t>A webinar chaired by Sopan Patil, with Richard Dallison as speaker, presenting the results of WP7 work on the impacts of future climate change on water resources in Wales, and the implications for hydropower production. Results for Wales were put in the context of the wider UK, and for other water abstractors.</t>
   </si>
   <si>
+    <t>2,1,8</t>
+  </si>
+  <si>
     <t>Study investigating how future worst-case scenario climate change will impact on the timing and quantity of streamflow at 585 catchments across the UK and Ireland, and the knock-on implications of such changes for water abstraction at 531 hydropower locations in 178 catchments in England, Wales, Scotland, Ireland &amp; Northern Ireland.</t>
   </si>
   <si>
     <t>Project</t>
   </si>
   <si>
+    <t>13,5,19</t>
+  </si>
+  <si>
     <t>Study investigating the historical trends in mean and extreme streamflow, temperatures, and precipitation, in five catchments in Wales.</t>
   </si>
   <si>
+    <t>2,16,16</t>
+  </si>
+  <si>
     <t>Study investigating future trends in mean and extreme streamflow, as well as water quality, for five catchments in Wales, in worst-case scenario future climate change.</t>
   </si>
   <si>
+    <t>1,2,6</t>
+  </si>
+  <si>
     <t>Study investigating the impacts of future climate change induced streamflow alterations on water available for public water supply and hydropower, using two catchments in Wales as case studies.</t>
   </si>
   <si>
+    <t>3,4,9</t>
+  </si>
+  <si>
     <t>The webinar is place-based 45 minute on-line workshop for primary school pupils in 4th to 6th class in school served by BGWS. Topics: it covers the natural and man made water cycle; the Blackstairs GWS scheme details; the MHP system details. The workshop is interactive and engaging with a number of hands-on activities, including a group activity to design and plan for climate action in their schools or communities.</t>
   </si>
   <si>
+    <t>2,6,7,8,12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Four demonstration sites to showcase the techological solutions were planned and implemented as part of Dwr Uisce with the aim of bringing outside of the lab the technology and to demonstrate in practice how they work and how they can benefit the users. Each of the installation at the different demonstration sites underwent a process of lab testing, prototyping, implementation, feedback from other stakeholders involved. The four fall in two main categories: micro-hydropower installations and heat recovery systems. </t>
   </si>
   <si>
+    <t>1,3,4,5,9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Official opening of the demonstration site in Tŷ Mawr Wybrnant, Wales (UK) on 21/11/19. The event was about demonstrating a novel technology such as the application of a pump-as-turbine to produce energy from a small stream running along the land, property of the National Trust Wales. The energy produced is used within Ty Mwr to power a dehumidifying system that preserves the first Welsh-translated bible from beign damaged by the dampness. Associated information board remains as a legacy of the project communicting key features to visitors. </t>
   </si>
   <si>
+    <t>2,1,9</t>
+  </si>
+  <si>
     <t>The SSC and Water-Energy Network aim to facilitate dissemination of information and technology, and collaboration within the network of participating enterprises. The smart specialisation cluster comprises key actors in the sector in Ireland and Wales, supplemented by outside expertise where appropriate. In the context of the Dŵr Uisce project, the smart specialisation cluster can be seen as a learning network of enterprises.</t>
   </si>
   <si>
+    <t>13,5,20</t>
+  </si>
+  <si>
     <t>Tools for dissemination and for translating research into ordinary speak.</t>
   </si>
   <si>
     <t>Communication</t>
   </si>
   <si>
+    <t>2,16,17</t>
+  </si>
+  <si>
     <t xml:space="preserve">A series of free sustainability webinars to present the findings, challenges and practical solutions to improving energy efficiency in the water sector. </t>
   </si>
   <si>
+    <t>1,2,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Official opening of the demonstration site in Blackstairs (Co. Wexford, Ireland) on 02/05/19. The event was about demonstrating a novel technology such as the application of a pump-as-turbine to recover energy in a water supply network managed by a Group water Scheme. The event was used as an intervention to elict knowledge sharing, feedback and dissemination of the idea, in order to accelerate adoption of the technological solution by other suitable water network operators. Associated information board remains as a legacy of the project communicting key features to visitors. </t>
   </si>
   <si>
+    <t>3,4,10</t>
+  </si>
+  <si>
     <t>We are planning to deliver a short training to staff from NTW to raise awarenss of the installed heat recovery system</t>
   </si>
   <si>
+    <t>2,6,7,8,13</t>
+  </si>
+  <si>
     <t>We developed information boards to share the details of the DWHR system as well as raising awareness of the climate action potential of the system</t>
   </si>
   <si>
+    <t>1,3,4,5,10</t>
+  </si>
+  <si>
     <t>The project aims to improve the long-term sustainability of water supply, treatment and end-use in Ireland and Wales. This improvement is to be achieved through the development of new innovative technology platforms, undertaking economic and environmental impact assessments, and developing policy and best practice guidelines to facilitate the implementation of integrated low-carbon and smart energy solutions. The scope of Dŵr Uisce covers three themes: Technology Platforms; Policy Support and Guidance; and, Dissemination and Collaboration.</t>
   </si>
   <si>
     <t>In person workshop to present the software EPANET to members of the Group Water Schemes and to illustrate the features, possibilities and some potential applications to manage their networks</t>
   </si>
   <si>
+    <t>13,5,21</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assessing the water-energy efficiency of wet leisure centre stock of a local authority in North Wales. </t>
   </si>
   <si>
+    <t>2,16,18</t>
+  </si>
+  <si>
     <t xml:space="preserve">A panel discussion of experts working in different areas of leisure centre design, development, operation, and management that discussed the potential for existing leisure centres to adopt heat recovery as a means of emissions reductions and costs savings, particularly with respect to Covid-19 and net-zero targets and ambitions. </t>
   </si>
   <si>
+    <t>1,2,8</t>
+  </si>
+  <si>
     <t>Assessing and quantifying the whole building potential (NZEB) of a community-run rural leisure centre in mid-Wales: case study.</t>
   </si>
   <si>
+    <t>3,4,11</t>
+  </si>
+  <si>
     <t>Monitoring, assessment and quantification of the water-energy use efficiency and management on resource use, carbon footprint, and water quality of existing swimming pools in North Wales.</t>
   </si>
   <si>
+    <t>2,6,7,8,14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assessing the water-energy efficiency potential of office water use in a new-build science park on Anglesey, Wales. </t>
   </si>
   <si>
+    <t>1,3,4,5,11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assessing and quantifying the water-energy efficiency of a historic pub/ restaurant in Dublin. Case study for heat recovery potential of commercial pub kitchen. </t>
   </si>
   <si>
+    <t>2,1,11</t>
+  </si>
+  <si>
     <t>The workshop, based on the content and activities developed for BGWS, has been adapted to be used by other GWSs in collaboration with NFGWS</t>
   </si>
   <si>
+    <t>13,5,22</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-hour long webinar to present the concept and applications of DWHR </t>
   </si>
   <si>
+    <t>2,16,19</t>
+  </si>
+  <si>
     <t>Development of thermal recovery unit for enhanced heat recaptre from the kitchens wastewater. Furthermore, analyse the impact of heat recovery on grease trap removal efficiency. In near future, new heat exchanger material design in our portfolio to explore with an objective to develop cost-effective and thermally competent system design.</t>
   </si>
   <si>
+    <t>1,2,9</t>
+  </si>
+  <si>
     <t>This project concerns the design, planning and installation of the DWHR system at ABP in Tipperary, Ireland</t>
   </si>
   <si>
+    <t>3,4,12</t>
+  </si>
+  <si>
     <t>Data recorded at ABP is monitored to assess how much heat is recovered from the system installed in meat factory</t>
   </si>
   <si>
+    <t>2,6,7,8,15</t>
+  </si>
+  <si>
     <t>1- hour long webinar to present to the general public and SSC memmebrs the output of the benchmarking work</t>
   </si>
   <si>
+    <t>1,3,4,5,12</t>
+  </si>
+  <si>
     <t>The student accommodation has been monitored using tiny tags to assess the heat recovery potential</t>
   </si>
   <si>
+    <t>2,1,12</t>
+  </si>
+  <si>
     <t>The grease trap has been nmonitored for three weeks in December 2021 to evaluate the temperature of the drainwater leaving the kitchen of the on-site café to assess the heat recovery potential</t>
   </si>
   <si>
+    <t>13,5,23</t>
+  </si>
+  <si>
     <t>A 1 hour long webinar targeted to the hospitality sector to present DWHR from commercial kitchens in theory and practice by illustrating the demo site at Penrhyn Castle.Also the Heat recovery Tool was presented and participants were given the time to explore the tool and test the feasibility of applying the system in their kitchens using their data.</t>
   </si>
   <si>
+    <t>2,16,20</t>
+  </si>
+  <si>
     <t>The kick-off event took place in 2016 and included presentations by principal investigators from Trinity College and Bangor University; a structured group discussion in the morning. In the afternoon, two 10-mins presentations were delivered by two demonstrators  Welsh Water and National Trust Wales. Those were followed by a breakout session which included all participants. Three pre-formed goups were assigned as follows: 1 WW representative and 2 NTW representatives. DU team mebers  placed themselves strategically according to individual project responsibility and interests among the three groups to prompt, observe and note the questioning. At the end each participant was given a one-page questionnaire in order to record specific details about each of them in terms of personal and organizational motivation, contribution, interest, and expectations.</t>
   </si>
   <si>
+    <t>1,2,10</t>
+  </si>
+  <si>
     <t>The first annual Dwr Uisce Conference was hosted by Bangor University in Wales. The theme of the conference aimed to address the challenges we face in relation to water and energy demands in our region. The event included guest speakers on technical, social and governance perspectives on the importance of valuing our water and energy resources, and discussed how we can ensure water and energy security in the future. There was also an opportunity for conference participants to give their own 2-minute perspective on an energy efficiency water sector.</t>
   </si>
   <si>
+    <t>3,4,13</t>
+  </si>
+  <si>
     <t>This event presented case studies and discussions as to how and why achieving savings, offsetting your demands and identify opportunities for recycling/recovery of energy and water is so important to Wales. The programme had three sections: Savings; Innovation and Offsets. Presentations from stakeholders such as Cadiff University, Centre for Alternative Technologies, Waterwise, Dulas, Bangor University Sustainability Lab, Adnams Southwold Brewery, Aberyswith University as well as two interventions from Dwr Uisce team members were featured.</t>
+  </si>
+  <si>
+    <t>2,6,7,8,16</t>
   </si>
   <si>
     <t>Delivered in collaboration with the National Federation of Group Water Schemes (Ireland). The workshop's objective were:                                                                                                             - To present, discuss and learn from some of actual case-studies in the area of energy recovery from water distribution systems and wastewater systems, using hydropower turbines, pump optimisation and leakage reduction.
@@ -2410,130 +2566,271 @@
 - To create new learning opportunities and connections for workshop participants.</t>
   </si>
   <si>
+    <t>1,3,4,5,13</t>
+  </si>
+  <si>
     <t>The second annual Dwr Uisce conference was hosted by Trinity College Dublin in Ireland. The theme was 'Water–Energy Innovation' and it addressed the challenges we face in relation to water and energy demands in our region. The programme included three sessions: "Innovation Opportunities", "Innovation Practice" and "Demonstrating Learning".  The event featured a variety of guest speakers from industry, HEI and government sectors in Ireland and Wales. Participants were offered the opportunity to present two-minutes pitches of their water-energy related business or research.</t>
   </si>
   <si>
+    <t>2,1,13</t>
+  </si>
+  <si>
     <t xml:space="preserve">Competition programme for key stage 4 and 5 students in Welsh secondary schools. </t>
   </si>
   <si>
+    <t>13,5,24</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exploring and quantifying the climate action potential from household water-related energy efficiency and contributions from emissions savings on Irish net-zero ambitions and targets. </t>
   </si>
   <si>
+    <t>2,16,21</t>
+  </si>
+  <si>
     <t>An in person event to launch our Citizen Science project and gather feedback from a community.</t>
   </si>
   <si>
+    <t>1,2,11</t>
+  </si>
+  <si>
     <t>The Climate Action Hackathon was a 2 -day online event to engaged teenagers aged 15-17 in ideating solutions for water-energy inefficiency. The event was led by Dwr Uisce team members and organised in collaboration with ECO-UNESCO in Dublin. During the 1 hr long pre-hackathon, participants had an opportunity to ask questions to Dwr Uisce team members about their work, the water-energy nexus and the project overall. The hackathon took place on the second day and the participants had 3 hours to work in teams to plan, design and present to the organisers and the other teams an idea that could improve the efficiency of water-related energy use in their schools, cmmunities or on a broader scale. Dwr Uisce team members acted as mentors, providing support and suggesitons throughout the event.</t>
   </si>
   <si>
+    <t>3,4,14</t>
+  </si>
+  <si>
     <t>Analyzing the difference in available wastewater heating resource across the different scales of an urban wastewater system i.e. how much heat is loss to the environment and does it build a case for decentralized wastewater heat recovery?</t>
   </si>
   <si>
+    <t>2,6,7,8,17</t>
+  </si>
+  <si>
+    <t>1,3,4,5,14</t>
+  </si>
+  <si>
     <t>Assessment and quantification of the water use efficiency and management on resource use in participating schools</t>
   </si>
   <si>
     <t>undefined</t>
   </si>
   <si>
+    <t>2,1,14</t>
+  </si>
+  <si>
     <t>Study investigating how future worst-case scenario climate change will impact on the timing and quantity of streamflow at 130 catchment accross the UK and Ireland (currently England, Wales, Ireland &amp; Northern Ireland), and the knock-on implications of such changes for water abstraction at 420 hydropower locations.</t>
   </si>
   <si>
+    <t>13,5,25</t>
+  </si>
+  <si>
     <t>Journal article based upon a conference paper presented at IPDMC 2020.  Describe and reflect on the actions undertaken by a network of stakeholders to co-generate learning from green process innovation.</t>
   </si>
   <si>
+    <t>2,16,22</t>
+  </si>
+  <si>
     <t>Study investigating cost-effectiveness and emissions savings from replacing conventional heating systems (gas, oil, electricity, LPG and coal) to low-carbon heating systems (ASHP, GSHP, biomass boilers solar PV)</t>
   </si>
   <si>
+    <t>1,2,12</t>
+  </si>
+  <si>
     <t>We carried out a focus group with a gropu of transition year students to develop the materials for the hackathon porgamme</t>
   </si>
   <si>
+    <t>3,4,15</t>
+  </si>
+  <si>
     <t>Journal article investigating economic and environmental efficiency of water and sewage companes, with a focus on appropriate methodologies and the factors affecting performance</t>
   </si>
   <si>
+    <t>2,6,7,8,18</t>
+  </si>
+  <si>
     <t>Journal article investigating energy and economic efficiency across water and sewage and water-only companies. Additional focus on assessing how common proxy indicators performed vs. best available</t>
   </si>
   <si>
+    <t>1,3,4,5,15</t>
+  </si>
+  <si>
     <t>Journal article investigating the productivity of the UK water sector over a 6 year period using metrics based on a wider sustainability perspective.</t>
   </si>
   <si>
+    <t>2,1,15</t>
+  </si>
+  <si>
     <t>Journal article evaluating the energy consumption of wastewater utilities across the globe</t>
   </si>
   <si>
+    <t>13,5,26</t>
+  </si>
+  <si>
     <t xml:space="preserve">Journal article investigating the efficiency of water and sewage, communication, and energy utilties </t>
   </si>
   <si>
+    <t>2,16,23</t>
+  </si>
+  <si>
     <t>Analysis of the water network operated by the Ballacolla GWS to assess the potential for hydro energy recovery</t>
   </si>
   <si>
     <t>Study</t>
   </si>
   <si>
+    <t>1,2,13</t>
+  </si>
+  <si>
     <t>Analysis of the water network operated by the Blackstairs GWS to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>3,4,16</t>
+  </si>
+  <si>
     <t>Analysis of the water network operated by the Ballinabrannagh GWS to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>2,6,7,8,19</t>
+  </si>
+  <si>
     <t>Analysis of the water network operated by the Kilanerin GWS to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>1,3,4,5,16</t>
+  </si>
+  <si>
     <t>Analysis of three water networks operated by EPS to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>2,1,16</t>
+  </si>
+  <si>
     <t>Analysis of a series of water networks and roadside culverts owned by the Blaenau Gwent municipality to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>13,5,27</t>
+  </si>
+  <si>
     <t>Analysis of the outfall of the Five Fords WWTP operated by Welsh Water to assess the potential for hydro energy recovery and produce a preliminary design of the hydro site</t>
   </si>
   <si>
+    <t>2,16,24</t>
+  </si>
+  <si>
     <t>Analysis of the Dodder water supply line operated by Dublin City Council on behalf of Irish Water to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>1,2,14</t>
+  </si>
+  <si>
     <t>Preliminary design of a picoturbine at the inlet of a storage tank in the Blackstairs GWS</t>
   </si>
   <si>
+    <t>3,4,17</t>
+  </si>
+  <si>
     <t>Analysis of a pressure reducing station at Boliden Tara Mines to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>2,6,7,8,20</t>
+  </si>
+  <si>
     <t>Analysis of the outfall of the Dairygold WWTP to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>1,3,4,5,17</t>
+  </si>
+  <si>
     <t>Analysis of the inlet of the Fethard WTP to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>2,1,17</t>
+  </si>
+  <si>
     <t>Publication of the research on the development of a heat recovery toolkit for commercial kitchen owners (pubs, restaurants, cafes, canteens etc.) whcich enables them to get an estimate on their individual heat recovery potential from drain water, environmental and cost savings (or trade-offs).</t>
   </si>
   <si>
+    <t>13,5,28</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assess the feasibility of installaing a DWHR system at the Imperial Hotel, Llandudno </t>
   </si>
   <si>
+    <t>2,16,25</t>
+  </si>
+  <si>
     <t>Study investigating the impact of variation in abstraction licence conditions between England, Wales, Scotland, Northern Ireland, and Ireland on water abstraction for run-of-river hydropower. Study looks at the lost abstraction, and therefore power generation both historically (1985-2015) and for future worst-cast scenario climate change (RCP8.5) affected flows (2021-2080)</t>
   </si>
   <si>
+    <t>1,2,15</t>
+  </si>
+  <si>
     <t>Hydrological modelling work completed for the Talybont Community Flood Group to identify sub-catchments upstream of the village that are contributing the most to peak flows. Also studied was the impact of tree planting on reducing these peak flood flows.</t>
   </si>
   <si>
+    <t>3,4,18</t>
+  </si>
+  <si>
     <t>Consultation work for Aber Falls distillery on how to lower their environmental footprint with focus on energy, water use and by-product use.</t>
   </si>
   <si>
+    <t>2,6,7,8,21</t>
+  </si>
+  <si>
+    <t>1,3,4,5,18</t>
+  </si>
+  <si>
+    <t>2,1,18</t>
+  </si>
+  <si>
+    <t>13,5,29</t>
+  </si>
+  <si>
     <t>"Feaibility studies for DWHR at the following sites: National Trust, Coolmore Park GWS,Talbot Hotel Stillorgan,Druids Glen Hotel, Ashlawn Nursing Home, Nenagh Swimming Pool, Cooleney Cheese, ABP Food Group,	Noel Lawlor Consulting Engineers"</t>
   </si>
   <si>
+    <t>2,16,26</t>
+  </si>
+  <si>
+    <t>1,2,16</t>
+  </si>
+  <si>
     <t>Analysis of the water network operated by the Ballinguiroe Tankardstown GWS and Coolagh Caherleske GWS, Kilcredan GWS to assess the potential for hydro energy recovery</t>
   </si>
   <si>
+    <t>3,4,19</t>
+  </si>
+  <si>
     <t>Hydropower potential assessment of the Mullins Mill on the River Kings in Co. Kilkenny</t>
   </si>
   <si>
     <t>study</t>
   </si>
   <si>
+    <t>2,6,7,8,22</t>
+  </si>
+  <si>
     <t>Delivery of the Hackathon Programme in Irish Secondary Schools</t>
   </si>
   <si>
+    <t>1,3,4,5,19</t>
+  </si>
+  <si>
     <t>Data collection for the whole production life cycle of whisky at Arbikie distillery, calculation of an environmental footprint and elaboration of suitable measures to reduce the carbon and water footprint by: using by-products or recovering heat from waste and process streams.</t>
   </si>
   <si>
     <t>Inter- and Transdisciplinary</t>
+  </si>
+  <si>
+    <t>2,1,19</t>
+  </si>
+  <si>
+    <t>13,5,30</t>
+  </si>
+  <si>
+    <t>2,16,27</t>
+  </si>
+  <si>
+    <t>1,2,17</t>
   </si>
 </sst>
 </file>
@@ -2636,9 +2933,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2646,6 +2940,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2959,7 +3256,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -2975,6 +3272,7 @@
     <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
     <col min="9" max="9" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2984,36 +3282,39 @@
       <c r="B1" s="14" t="s">
         <v>726</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="8" t="s">
         <v>413</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>727</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>728</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>729</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>699</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>730</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>731</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>732</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>733</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
       <c r="C2" s="14">
@@ -3023,26 +3324,29 @@
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G2" s="16" t="s">
         <v>735</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="J2" s="18">
+      <c r="I2" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="J2" s="17">
         <v>42614</v>
       </c>
+      <c r="K2" s="18" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="15">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="14">
@@ -3054,23 +3358,26 @@
       <c r="D3" s="14">
         <v>39</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>738</v>
+      <c r="E3" s="15" t="s">
+        <v>740</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G3" s="16" t="s">
         <v>735</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="I3" s="18">
+      <c r="H3" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="I3" s="17">
         <v>43799</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="17">
         <v>42614</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>741</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -3086,26 +3393,29 @@
       <c r="D4" s="14">
         <v>26</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>739</v>
+      <c r="E4" s="15" t="s">
+        <v>742</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I4" s="18">
+        <v>735</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I4" s="17">
         <v>43404</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="17">
         <v>42614</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="465">
+      <c r="K4" s="3" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -3118,23 +3428,26 @@
       <c r="D5" s="14">
         <v>64</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>742</v>
+      <c r="E5" s="3" t="s">
+        <v>746</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I5" s="18">
+        <v>735</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I5" s="17">
         <v>44561</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="17">
         <v>44317</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>748</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -3147,26 +3460,29 @@
       <c r="C6" s="14">
         <v>1</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="8">
         <v>33</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>739</v>
+      <c r="E6" s="15" t="s">
+        <v>742</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>743</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I6" s="18">
+        <v>744</v>
+      </c>
+      <c r="I6" s="17">
         <v>43616</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>42614</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>749</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -3176,36 +3492,39 @@
       <c r="B7" s="14">
         <v>1</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="8">
         <v>54</v>
       </c>
       <c r="D7" s="14">
         <v>54</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>744</v>
+      <c r="E7" s="15" t="s">
+        <v>750</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I7" s="18">
+        <v>735</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I7" s="17">
         <v>44255</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="17">
         <v>44228</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>752</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
       <c r="C8" s="14">
@@ -3215,24 +3534,27 @@
         <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>743</v>
       </c>
       <c r="H8" s="14"/>
-      <c r="I8" s="18">
+      <c r="I8" s="17">
         <v>44500</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="17">
         <v>43739</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="114">
-      <c r="A9" s="15">
+      <c r="K8" s="3" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="14">
@@ -3244,24 +3566,27 @@
       <c r="D9" s="14">
         <v>78</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>746</v>
+      <c r="E9" s="15" t="s">
+        <v>754</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G9" s="16" t="s">
         <v>735</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="18">
+      <c r="G9" s="15" t="s">
+        <v>736</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="17">
         <v>44985</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="17">
         <v>43586</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="154.5">
+      <c r="K9" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -3274,24 +3599,27 @@
       <c r="D10" s="14">
         <v>29</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>747</v>
+      <c r="E10" s="15" t="s">
+        <v>756</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>743</v>
       </c>
       <c r="H10" s="14"/>
-      <c r="I10" s="18">
+      <c r="I10" s="17">
         <v>43496</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="17">
         <v>42614</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="127.5">
+      <c r="K10" s="3" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -3304,21 +3632,24 @@
       <c r="D11" s="14">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>748</v>
+      <c r="E11" s="3" t="s">
+        <v>758</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>743</v>
       </c>
       <c r="H11" s="14"/>
-      <c r="I11" s="18">
+      <c r="I11" s="17">
         <v>43677</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="17">
         <v>42614</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>759</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="37.5">
@@ -3331,24 +3662,27 @@
       <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="8">
         <v>40</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>749</v>
+      <c r="E12" s="15" t="s">
+        <v>760</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>743</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="18">
+      <c r="I12" s="17">
         <v>43830</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="17">
         <v>42614</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>761</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="87">
@@ -3358,36 +3692,39 @@
       <c r="B13" s="14">
         <v>2</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="8">
         <v>1</v>
       </c>
       <c r="D13" s="14">
         <v>42</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>750</v>
+      <c r="E13" s="15" t="s">
+        <v>762</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G13" s="16" t="s">
         <v>735</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="I13" s="18">
+      <c r="H13" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I13" s="17">
         <v>43890</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="17">
         <v>42614</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>763</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="114">
       <c r="A14" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="8">
         <v>2</v>
       </c>
       <c r="C14" s="14">
@@ -3397,26 +3734,29 @@
         <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>736</v>
+      </c>
+      <c r="H14" s="15" t="s">
         <v>751</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>735</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I14" s="18">
+      <c r="I14" s="17">
         <v>44985</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="17">
         <v>43862</v>
       </c>
+      <c r="K14" s="3" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="181.5">
-      <c r="A15" s="15">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="14">
@@ -3428,23 +3768,26 @@
       <c r="D15" s="14">
         <v>55</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>752</v>
+      <c r="E15" s="15" t="s">
+        <v>766</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="I15" s="18">
+        <v>735</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="I15" s="17">
         <v>44286</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="17">
         <v>44256</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>767</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33">
@@ -3460,23 +3803,26 @@
       <c r="D16" s="14">
         <v>55</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>753</v>
+      <c r="E16" s="15" t="s">
+        <v>768</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I16" s="18">
+        <v>735</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I16" s="17">
         <v>44286</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="17">
         <v>43525</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>770</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="37.5">
@@ -3492,23 +3838,26 @@
       <c r="D17" s="14">
         <v>47</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>755</v>
+      <c r="E17" s="3" t="s">
+        <v>771</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>740</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I17" s="18">
+        <v>735</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I17" s="17">
         <v>44043</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="17">
         <v>43282</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>772</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="100.5">
@@ -3521,26 +3870,29 @@
       <c r="C18" s="14">
         <v>35</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="8">
         <v>64</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>756</v>
+      <c r="E18" s="15" t="s">
+        <v>773</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>743</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I18" s="18">
+        <v>744</v>
+      </c>
+      <c r="I18" s="17">
         <v>44561</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="17">
         <v>43647</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>774</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="37.5">
@@ -3550,36 +3902,39 @@
       <c r="B19" s="14">
         <v>4</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="8">
         <v>31</v>
       </c>
       <c r="D19" s="14">
         <v>74</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>757</v>
+      <c r="E19" s="15" t="s">
+        <v>775</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>740</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I19" s="18">
+        <v>735</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I19" s="17">
         <v>44865</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="17">
         <v>43525</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>776</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="141">
       <c r="A20" s="14">
         <v>20</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="8">
         <v>7</v>
       </c>
       <c r="C20" s="14">
@@ -3589,26 +3944,29 @@
         <v>62</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>758</v>
+        <v>777</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I20" s="18">
+        <v>735</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I20" s="17">
         <v>44500</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="17">
         <v>44470</v>
       </c>
+      <c r="K20" s="3" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="114">
-      <c r="A21" s="15">
+      <c r="A21" s="8">
         <v>21</v>
       </c>
       <c r="B21" s="14">
@@ -3620,23 +3978,26 @@
       <c r="D21" s="14">
         <v>78</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>759</v>
+      <c r="E21" s="15" t="s">
+        <v>779</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="I21" s="18">
+        <v>735</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="I21" s="17">
         <v>44985</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="17">
         <v>44197</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>781</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="100.5">
@@ -3652,23 +4013,26 @@
       <c r="D22" s="14">
         <v>18</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>761</v>
+      <c r="E22" s="15" t="s">
+        <v>782</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I22" s="18">
+        <v>735</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I22" s="17">
         <v>43159</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="17">
         <v>42614</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>783</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="127.5">
@@ -3684,23 +4048,26 @@
       <c r="D23" s="14">
         <v>52</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>762</v>
+      <c r="E23" s="3" t="s">
+        <v>784</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I23" s="18">
+        <v>735</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I23" s="17">
         <v>44196</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J23" s="17">
         <v>43160</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>785</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="168">
@@ -3713,26 +4080,29 @@
       <c r="C24" s="14">
         <v>18</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="8">
         <v>47</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>763</v>
+      <c r="E24" s="15" t="s">
+        <v>786</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I24" s="18">
+        <v>744</v>
+      </c>
+      <c r="I24" s="17">
         <v>44043</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="17">
         <v>43132</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>787</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="60">
@@ -3742,36 +4112,39 @@
       <c r="B25" s="14">
         <v>8</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="8">
         <v>57</v>
       </c>
       <c r="D25" s="14">
         <v>64</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>764</v>
+      <c r="E25" s="15" t="s">
+        <v>788</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I25" s="18">
+        <v>735</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I25" s="17">
         <v>44561</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="17">
         <v>44317</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>789</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="168">
       <c r="A26" s="14">
         <v>26</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="8">
         <v>8</v>
       </c>
       <c r="C26" s="14">
@@ -3781,26 +4154,29 @@
         <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>765</v>
+        <v>790</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G26" s="16" t="s">
         <v>735</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="G26" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="I26" s="18">
+      <c r="H26" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I26" s="17">
         <v>44985</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J26" s="17">
         <v>42614</v>
       </c>
+      <c r="K26" s="3" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="87">
-      <c r="A27" s="15">
+      <c r="A27" s="8">
         <v>27</v>
       </c>
       <c r="B27" s="14">
@@ -3812,23 +4188,26 @@
       <c r="D27" s="14">
         <v>39</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>766</v>
+      <c r="E27" s="15" t="s">
+        <v>792</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="I27" s="18">
+        <v>735</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="I27" s="17">
         <v>43799</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J27" s="17">
         <v>43770</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>793</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="87">
@@ -3844,23 +4223,26 @@
       <c r="D28" s="14">
         <v>78</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>767</v>
+      <c r="E28" s="15" t="s">
+        <v>794</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I28" s="18">
+        <v>735</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I28" s="17">
         <v>44985</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="17">
         <v>42614</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>795</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="114">
@@ -3876,23 +4258,26 @@
       <c r="D29" s="14">
         <v>78</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>768</v>
+      <c r="E29" s="3" t="s">
+        <v>796</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>769</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I29" s="18">
+        <v>735</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>797</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I29" s="17">
         <v>44985</v>
       </c>
-      <c r="J29" s="18">
+      <c r="J29" s="17">
         <v>42614</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>798</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
@@ -3905,26 +4290,29 @@
       <c r="C30" s="14">
         <v>54</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="8">
         <v>78</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>770</v>
+      <c r="E30" s="15" t="s">
+        <v>799</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>743</v>
+        <v>735</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>747</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="I30" s="18">
+        <v>751</v>
+      </c>
+      <c r="I30" s="17">
         <v>44985</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="17">
         <v>44228</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>800</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -3934,36 +4322,39 @@
       <c r="B31" s="14">
         <v>8</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="8">
         <v>33</v>
       </c>
       <c r="D31" s="14">
         <v>33</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>771</v>
+      <c r="E31" s="15" t="s">
+        <v>801</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I31" s="18">
+        <v>735</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I31" s="17">
         <v>43616</v>
       </c>
-      <c r="J31" s="18">
+      <c r="J31" s="17">
         <v>43586</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>802</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="14">
         <v>32</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="8">
         <v>8</v>
       </c>
       <c r="C32" s="14">
@@ -3973,24 +4364,27 @@
         <v>78</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>772</v>
+        <v>803</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>769</v>
+        <v>735</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>797</v>
       </c>
       <c r="H32" s="14"/>
-      <c r="I32" s="18">
+      <c r="I32" s="17">
         <v>44985</v>
       </c>
-      <c r="J32" s="18">
+      <c r="J32" s="17">
         <v>44470</v>
       </c>
+      <c r="K32" s="3" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="15">
+      <c r="A33" s="8">
         <v>33</v>
       </c>
       <c r="B33" s="14">
@@ -4002,21 +4396,24 @@
       <c r="D33" s="14">
         <v>78</v>
       </c>
-      <c r="E33" s="16" t="s">
-        <v>773</v>
+      <c r="E33" s="15" t="s">
+        <v>805</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>769</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="18">
+        <v>735</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>797</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="17">
         <v>44985</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J33" s="17">
         <v>44470</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>806</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
@@ -4032,23 +4429,26 @@
       <c r="D34" s="14">
         <v>52</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>774</v>
+      <c r="E34" s="15" t="s">
+        <v>807</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I34" s="18">
+        <v>735</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I34" s="17">
         <v>44196</v>
       </c>
-      <c r="J34" s="18">
+      <c r="J34" s="17">
         <v>42614</v>
+      </c>
+      <c r="K34" s="18" t="s">
+        <v>739</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
@@ -4064,21 +4464,24 @@
       <c r="D35" s="14">
         <v>63</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>775</v>
+      <c r="E35" s="3" t="s">
+        <v>808</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>743</v>
+        <v>735</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>747</v>
       </c>
       <c r="H35" s="14"/>
-      <c r="I35" s="18">
+      <c r="I35" s="17">
         <v>44530</v>
       </c>
-      <c r="J35" s="18">
+      <c r="J35" s="17">
         <v>44501</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>809</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
@@ -4091,26 +4494,29 @@
       <c r="C36" s="14">
         <v>30</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="8">
         <v>42</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>776</v>
+      <c r="E36" s="15" t="s">
+        <v>810</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="I36" s="18">
+        <v>751</v>
+      </c>
+      <c r="I36" s="17">
         <v>43890</v>
       </c>
-      <c r="J36" s="18">
+      <c r="J36" s="17">
         <v>43497</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>811</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
@@ -4120,36 +4526,39 @@
       <c r="B37" s="14">
         <v>6</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="8">
         <v>54</v>
       </c>
       <c r="D37" s="14">
         <v>54</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>777</v>
+      <c r="E37" s="15" t="s">
+        <v>812</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I37" s="18">
+        <v>735</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I37" s="17">
         <v>44255</v>
       </c>
-      <c r="J37" s="18">
+      <c r="J37" s="17">
         <v>44228</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>813</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="14">
         <v>38</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="8">
         <v>6</v>
       </c>
       <c r="C38" s="14">
@@ -4159,26 +4568,29 @@
         <v>78</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>778</v>
+        <v>814</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I38" s="18">
+        <v>735</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I38" s="17">
         <v>44985</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="17">
         <v>43891</v>
       </c>
+      <c r="K38" s="3" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="15">
+      <c r="A39" s="8">
         <v>39</v>
       </c>
       <c r="B39" s="14">
@@ -4190,23 +4602,26 @@
       <c r="D39" s="14">
         <v>70</v>
       </c>
-      <c r="E39" s="16" t="s">
-        <v>779</v>
+      <c r="E39" s="15" t="s">
+        <v>816</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="I39" s="18">
+        <v>735</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="I39" s="17">
         <v>44742</v>
       </c>
-      <c r="J39" s="18">
+      <c r="J39" s="17">
         <v>43891</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>817</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
@@ -4222,23 +4637,26 @@
       <c r="D40" s="14">
         <v>49</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="15" t="s">
+        <v>818</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I40" s="18">
+      <c r="H40" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I40" s="17">
         <v>44104</v>
       </c>
-      <c r="J40" s="18">
+      <c r="J40" s="17">
         <v>43891</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>819</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
@@ -4254,23 +4672,26 @@
       <c r="D41" s="14">
         <v>78</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>781</v>
+      <c r="E41" s="3" t="s">
+        <v>820</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I41" s="18">
+        <v>735</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I41" s="17">
         <v>44985</v>
       </c>
-      <c r="J41" s="18">
+      <c r="J41" s="17">
         <v>44256</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>821</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
@@ -4283,26 +4704,29 @@
       <c r="C42" s="14">
         <v>67</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="8">
         <v>78</v>
       </c>
-      <c r="E42" s="16" t="s">
-        <v>782</v>
+      <c r="E42" s="15" t="s">
+        <v>822</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>743</v>
+        <v>735</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>747</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="I42" s="18">
+        <v>737</v>
+      </c>
+      <c r="I42" s="17">
         <v>44985</v>
       </c>
-      <c r="J42" s="18">
+      <c r="J42" s="17">
         <v>44621</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>823</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
@@ -4312,36 +4736,39 @@
       <c r="B43" s="14">
         <v>2</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="8">
         <v>55</v>
       </c>
       <c r="D43" s="14">
         <v>55</v>
       </c>
-      <c r="E43" s="16" t="s">
-        <v>783</v>
+      <c r="E43" s="15" t="s">
+        <v>824</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I43" s="18">
+        <v>735</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I43" s="17">
         <v>44286</v>
       </c>
-      <c r="J43" s="18">
+      <c r="J43" s="17">
         <v>44256</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>825</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="14">
         <v>44</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="8">
         <v>2</v>
       </c>
       <c r="C44" s="14">
@@ -4351,26 +4778,29 @@
         <v>78</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>784</v>
+        <v>826</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G44" s="16" t="s">
+        <v>735</v>
+      </c>
+      <c r="G44" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="H44" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I44" s="18">
+      <c r="H44" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I44" s="17">
         <v>44985</v>
       </c>
-      <c r="J44" s="18">
+      <c r="J44" s="17">
         <v>44440</v>
       </c>
+      <c r="K44" s="3" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="15">
+      <c r="A45" s="8">
         <v>45</v>
       </c>
       <c r="B45" s="14">
@@ -4382,23 +4812,26 @@
       <c r="D45" s="14">
         <v>78</v>
       </c>
-      <c r="E45" s="16" t="s">
-        <v>785</v>
+      <c r="E45" s="15" t="s">
+        <v>828</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G45" s="16" t="s">
         <v>735</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="G45" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="I45" s="18">
+      <c r="H45" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="I45" s="17">
         <v>44985</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J45" s="17">
         <v>43221</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>829</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -4414,23 +4847,26 @@
       <c r="D46" s="14">
         <v>78</v>
       </c>
-      <c r="E46" s="16" t="s">
-        <v>786</v>
+      <c r="E46" s="15" t="s">
+        <v>830</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G46" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="G46" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="I46" s="18">
+      <c r="H46" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I46" s="17">
         <v>44985</v>
       </c>
-      <c r="J46" s="18">
+      <c r="J46" s="17">
         <v>43831</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>831</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
@@ -4446,23 +4882,26 @@
       <c r="D47" s="14">
         <v>56</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>787</v>
+      <c r="E47" s="3" t="s">
+        <v>832</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I47" s="18">
+        <v>735</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I47" s="17">
         <v>44316</v>
       </c>
-      <c r="J47" s="18">
+      <c r="J47" s="17">
         <v>44287</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>833</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -4475,26 +4914,29 @@
       <c r="C48" s="14">
         <v>65</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D48" s="8">
         <v>78</v>
       </c>
-      <c r="E48" s="16" t="s">
-        <v>788</v>
+      <c r="E48" s="15" t="s">
+        <v>834</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="I48" s="18">
+        <v>737</v>
+      </c>
+      <c r="I48" s="17">
         <v>44985</v>
       </c>
-      <c r="J48" s="18">
+      <c r="J48" s="17">
         <v>44562</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>835</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -4504,36 +4946,39 @@
       <c r="B49" s="14">
         <v>2</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="8">
         <v>64</v>
       </c>
       <c r="D49" s="14">
         <v>64</v>
       </c>
-      <c r="E49" s="16" t="s">
-        <v>789</v>
+      <c r="E49" s="15" t="s">
+        <v>836</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H49" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I49" s="18">
+        <v>735</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I49" s="17">
         <v>44561</v>
       </c>
-      <c r="J49" s="18">
+      <c r="J49" s="17">
         <v>44531</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>837</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="14">
         <v>50</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="8">
         <v>4</v>
       </c>
       <c r="C50" s="14">
@@ -4543,26 +4988,29 @@
         <v>68</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>790</v>
+        <v>838</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I50" s="18">
+        <v>735</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I50" s="17">
         <v>44681</v>
       </c>
-      <c r="J50" s="18">
+      <c r="J50" s="17">
         <v>44652</v>
       </c>
+      <c r="K50" s="3" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="15">
+      <c r="A51" s="8">
         <v>51</v>
       </c>
       <c r="B51" s="14">
@@ -4574,26 +5022,29 @@
       <c r="D51" s="14">
         <v>2</v>
       </c>
-      <c r="E51" s="16" t="s">
-        <v>791</v>
+      <c r="E51" s="15" t="s">
+        <v>840</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G51" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="I51" s="18">
+        <v>735</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="I51" s="17">
         <v>42674</v>
       </c>
-      <c r="J51" s="18">
+      <c r="J51" s="17">
         <v>42644</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+      <c r="K51" s="3" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="14">
         <v>52</v>
       </c>
@@ -4606,26 +5057,29 @@
       <c r="D52" s="14">
         <v>14</v>
       </c>
-      <c r="E52" s="16" t="s">
-        <v>792</v>
+      <c r="E52" s="15" t="s">
+        <v>842</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I52" s="18">
+        <v>735</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I52" s="17">
         <v>43039</v>
       </c>
-      <c r="J52" s="18">
+      <c r="J52" s="17">
         <v>43009</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="K52" s="3" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="409.6000000000001">
       <c r="A53" s="14">
         <v>53</v>
       </c>
@@ -4638,26 +5092,29 @@
       <c r="D53" s="14">
         <v>18</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>793</v>
+      <c r="E53" s="3" t="s">
+        <v>844</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H53" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I53" s="18">
+        <v>735</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I53" s="17">
         <v>43159</v>
       </c>
-      <c r="J53" s="18">
+      <c r="J53" s="17">
         <v>43132</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="131.25">
+      <c r="K53" s="3" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="100.5">
       <c r="A54" s="14">
         <v>54</v>
       </c>
@@ -4667,65 +5124,71 @@
       <c r="C54" s="14">
         <v>20</v>
       </c>
-      <c r="D54" s="15">
+      <c r="D54" s="8">
         <v>20</v>
       </c>
-      <c r="E54" s="16" t="s">
-        <v>794</v>
+      <c r="E54" s="15" t="s">
+        <v>846</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G54" s="16" t="s">
-        <v>743</v>
+        <v>735</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>747</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="I54" s="18">
+        <v>737</v>
+      </c>
+      <c r="I54" s="17">
         <v>43220</v>
       </c>
-      <c r="J54" s="18">
+      <c r="J54" s="17">
         <v>43191</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="K54" s="3" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="14">
         <v>55</v>
       </c>
       <c r="B55" s="14">
         <v>8</v>
       </c>
-      <c r="C55" s="15">
+      <c r="C55" s="8">
         <v>26</v>
       </c>
       <c r="D55" s="14">
         <v>26</v>
       </c>
-      <c r="E55" s="16" t="s">
-        <v>795</v>
+      <c r="E55" s="15" t="s">
+        <v>848</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>736</v>
-      </c>
-      <c r="I55" s="18">
+        <v>735</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="I55" s="17">
         <v>43404</v>
       </c>
-      <c r="J55" s="18">
+      <c r="J55" s="17">
         <v>43374</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="K55" s="3" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="14">
         <v>56</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="8">
         <v>6</v>
       </c>
       <c r="C56" s="14">
@@ -4735,26 +5198,29 @@
         <v>78</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>796</v>
+        <v>850</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G56" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H56" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I56" s="18">
+        <v>735</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I56" s="17">
         <v>44985</v>
       </c>
-      <c r="J56" s="18">
+      <c r="J56" s="17">
         <v>44562</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="15">
+      <c r="K56" s="3" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+      <c r="A57" s="8">
         <v>57</v>
       </c>
       <c r="B57" s="14">
@@ -4766,26 +5232,29 @@
       <c r="D57" s="14">
         <v>78</v>
       </c>
-      <c r="E57" s="16" t="s">
-        <v>797</v>
+      <c r="E57" s="15" t="s">
+        <v>852</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="I57" s="18">
+        <v>735</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="I57" s="17">
         <v>44985</v>
       </c>
-      <c r="J57" s="18">
+      <c r="J57" s="17">
         <v>44409</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="K57" s="3" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="14">
         <v>58</v>
       </c>
@@ -4798,26 +5267,29 @@
       <c r="D58" s="14">
         <v>60</v>
       </c>
-      <c r="E58" s="16" t="s">
-        <v>798</v>
+      <c r="E58" s="15" t="s">
+        <v>854</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="H58" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I58" s="18">
+        <v>735</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I58" s="17">
         <v>44439</v>
       </c>
-      <c r="J58" s="18">
+      <c r="J58" s="17">
         <v>44348</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="K58" s="3" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="409.6000000000001">
       <c r="A59" s="14">
         <v>59</v>
       </c>
@@ -4830,26 +5302,29 @@
       <c r="D59" s="14">
         <v>58</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>799</v>
+      <c r="E59" s="3" t="s">
+        <v>856</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I59" s="18">
+        <v>735</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I59" s="17">
         <v>44377</v>
       </c>
-      <c r="J59" s="18">
+      <c r="J59" s="17">
         <v>44287</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="K59" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="14">
         <v>60</v>
       </c>
@@ -4859,86 +5334,95 @@
       <c r="C60" s="14">
         <v>53</v>
       </c>
-      <c r="D60" s="15">
+      <c r="D60" s="8">
         <v>78</v>
       </c>
-      <c r="E60" s="16" t="s">
-        <v>800</v>
+      <c r="E60" s="15" t="s">
+        <v>858</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I60" s="18">
+        <v>744</v>
+      </c>
+      <c r="I60" s="17">
         <v>44985</v>
       </c>
-      <c r="J60" s="18">
+      <c r="J60" s="17">
         <v>44197</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="K60" s="3" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="14">
         <v>61</v>
       </c>
       <c r="B61" s="14">
         <v>6</v>
       </c>
-      <c r="C61" s="15">
+      <c r="C61" s="8">
         <v>30</v>
       </c>
       <c r="D61" s="14">
         <v>42</v>
       </c>
-      <c r="E61" s="16" t="s">
-        <v>776</v>
+      <c r="E61" s="15" t="s">
+        <v>810</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H61" s="14"/>
-      <c r="I61" s="18">
+      <c r="I61" s="17">
         <v>43890</v>
       </c>
-      <c r="J61" s="18">
+      <c r="J61" s="17">
         <v>43497</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="K61" s="3" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="14">
         <v>62</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="8">
         <v>6</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="2" t="s">
-        <v>801</v>
+        <v>861</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G62" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H62" s="14"/>
-      <c r="I62" s="18" t="s">
-        <v>802</v>
-      </c>
-      <c r="J62" s="18" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="15">
+      <c r="I62" s="17" t="s">
+        <v>862</v>
+      </c>
+      <c r="J62" s="17" t="s">
+        <v>862</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+      <c r="A63" s="8">
         <v>63</v>
       </c>
       <c r="B63" s="14">
@@ -4950,24 +5434,27 @@
       <c r="D63" s="14">
         <v>52</v>
       </c>
-      <c r="E63" s="16" t="s">
-        <v>803</v>
+      <c r="E63" s="15" t="s">
+        <v>864</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>760</v>
-      </c>
-      <c r="H63" s="1"/>
-      <c r="I63" s="18">
+        <v>735</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="H63" s="3"/>
+      <c r="I63" s="17">
         <v>44196</v>
       </c>
-      <c r="J63" s="18">
+      <c r="J63" s="17">
         <v>43160</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+      <c r="K63" s="3" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="14">
         <v>64</v>
       </c>
@@ -4980,26 +5467,29 @@
       <c r="D64" s="14">
         <v>66</v>
       </c>
-      <c r="E64" s="16" t="s">
-        <v>804</v>
+      <c r="E64" s="15" t="s">
+        <v>866</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I64" s="18">
+        <v>735</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I64" s="17">
         <v>44620</v>
       </c>
-      <c r="J64" s="18">
+      <c r="J64" s="17">
         <v>43983</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="K64" s="3" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="262.5">
       <c r="A65" s="14">
         <v>65</v>
       </c>
@@ -5012,24 +5502,27 @@
       <c r="D65" s="14">
         <v>62</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>805</v>
+      <c r="E65" s="3" t="s">
+        <v>868</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>743</v>
       </c>
       <c r="H65" s="14"/>
-      <c r="I65" s="18">
+      <c r="I65" s="17">
         <v>44500</v>
       </c>
-      <c r="J65" s="18">
+      <c r="J65" s="17">
         <v>44105</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+      <c r="K65" s="3" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="14">
         <v>66</v>
       </c>
@@ -5039,65 +5532,71 @@
       <c r="C66" s="14">
         <v>67</v>
       </c>
-      <c r="D66" s="15">
+      <c r="D66" s="8">
         <v>68</v>
       </c>
-      <c r="E66" s="16" t="s">
-        <v>806</v>
+      <c r="E66" s="15" t="s">
+        <v>870</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G66" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="I66" s="18">
+        <v>737</v>
+      </c>
+      <c r="I66" s="17">
         <v>44681</v>
       </c>
-      <c r="J66" s="18">
+      <c r="J66" s="17">
         <v>44621</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="K66" s="3" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="14">
         <v>67</v>
       </c>
       <c r="B67" s="14">
         <v>5</v>
       </c>
-      <c r="C67" s="15">
+      <c r="C67" s="8">
         <v>14</v>
       </c>
       <c r="D67" s="14">
         <v>35</v>
       </c>
-      <c r="E67" s="16" t="s">
-        <v>807</v>
+      <c r="E67" s="15" t="s">
+        <v>872</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>740</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I67" s="18">
+        <v>735</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I67" s="17">
         <v>43677</v>
       </c>
-      <c r="J67" s="18">
+      <c r="J67" s="17">
         <v>43009</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="K67" s="3" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="14">
         <v>68</v>
       </c>
-      <c r="B68" s="15">
+      <c r="B68" s="8">
         <v>5</v>
       </c>
       <c r="C68" s="14">
@@ -5107,26 +5606,29 @@
         <v>49</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>808</v>
+        <v>874</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>740</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I68" s="18">
+        <v>735</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I68" s="17">
         <v>44104</v>
       </c>
-      <c r="J68" s="18">
+      <c r="J68" s="17">
         <v>43678</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="15">
+      <c r="K68" s="3" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
+      <c r="A69" s="8">
         <v>69</v>
       </c>
       <c r="B69" s="14">
@@ -5138,26 +5640,29 @@
       <c r="D69" s="14">
         <v>58</v>
       </c>
-      <c r="E69" s="16" t="s">
-        <v>809</v>
+      <c r="E69" s="15" t="s">
+        <v>876</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>740</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="I69" s="18">
+        <v>735</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="I69" s="17">
         <v>44377</v>
       </c>
-      <c r="J69" s="18">
+      <c r="J69" s="17">
         <v>44105</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+      <c r="K69" s="3" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="14">
         <v>70</v>
       </c>
@@ -5170,26 +5675,29 @@
       <c r="D70" s="14">
         <v>64</v>
       </c>
-      <c r="E70" s="16" t="s">
-        <v>810</v>
+      <c r="E70" s="15" t="s">
+        <v>878</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I70" s="18">
+        <v>735</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="H70" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I70" s="17">
         <v>44561</v>
       </c>
-      <c r="J70" s="18">
+      <c r="J70" s="17">
         <v>44378</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+      <c r="K70" s="3" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="114">
       <c r="A71" s="14">
         <v>71</v>
       </c>
@@ -5202,26 +5710,29 @@
       <c r="D71" s="14">
         <v>74</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>811</v>
+      <c r="E71" s="3" t="s">
+        <v>880</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G71" s="16" t="s">
-        <v>740</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="I71" s="18">
+        <v>735</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="H71" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="I71" s="17">
         <v>44865</v>
       </c>
-      <c r="J71" s="18">
+      <c r="J71" s="17">
         <v>44562</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="37.5">
+      <c r="K71" s="3" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="14">
         <v>72</v>
       </c>
@@ -5231,65 +5742,71 @@
       <c r="C72" s="14">
         <v>6</v>
       </c>
-      <c r="D72" s="15">
+      <c r="D72" s="8">
         <v>9</v>
       </c>
-      <c r="E72" s="16" t="s">
-        <v>812</v>
+      <c r="E72" s="15" t="s">
+        <v>882</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G72" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I72" s="18">
+        <v>744</v>
+      </c>
+      <c r="I72" s="17">
         <v>42886</v>
       </c>
-      <c r="J72" s="18">
+      <c r="J72" s="17">
         <v>42767</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="37.5">
+      <c r="K72" s="3" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="14">
         <v>73</v>
       </c>
       <c r="B73" s="14">
         <v>1</v>
       </c>
-      <c r="C73" s="15">
+      <c r="C73" s="8">
         <v>6</v>
       </c>
       <c r="D73" s="14">
         <v>9</v>
       </c>
-      <c r="E73" s="16" t="s">
-        <v>814</v>
+      <c r="E73" s="15" t="s">
+        <v>885</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H73" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I73" s="18">
+        <v>735</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H73" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I73" s="17">
         <v>42886</v>
       </c>
-      <c r="J73" s="18">
+      <c r="J73" s="17">
         <v>42767</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>886</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="37.5">
       <c r="A74" s="14">
         <v>74</v>
       </c>
-      <c r="B74" s="15">
+      <c r="B74" s="8">
         <v>1</v>
       </c>
       <c r="C74" s="14">
@@ -5299,26 +5816,29 @@
         <v>9</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>815</v>
+        <v>887</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G74" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H74" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I74" s="18">
+        <v>735</v>
+      </c>
+      <c r="G74" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I74" s="17">
         <v>42886</v>
       </c>
-      <c r="J74" s="18">
+      <c r="J74" s="17">
         <v>42767</v>
       </c>
+      <c r="K74" s="3" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="37.5">
-      <c r="A75" s="15">
+      <c r="A75" s="8">
         <v>75</v>
       </c>
       <c r="B75" s="14">
@@ -5330,23 +5850,26 @@
       <c r="D75" s="14">
         <v>9</v>
       </c>
-      <c r="E75" s="16" t="s">
-        <v>816</v>
+      <c r="E75" s="15" t="s">
+        <v>889</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G75" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="I75" s="18">
+        <v>735</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="I75" s="17">
         <v>42886</v>
       </c>
-      <c r="J75" s="18">
+      <c r="J75" s="17">
         <v>42767</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>890</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
@@ -5362,23 +5885,26 @@
       <c r="D76" s="14">
         <v>11</v>
       </c>
-      <c r="E76" s="16" t="s">
-        <v>817</v>
+      <c r="E76" s="15" t="s">
+        <v>891</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="H76" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I76" s="18">
+        <v>735</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I76" s="17">
         <v>42947</v>
       </c>
-      <c r="J76" s="18">
+      <c r="J76" s="17">
         <v>42856</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>892</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="37.5">
@@ -5394,23 +5920,26 @@
       <c r="D77" s="14">
         <v>13</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>818</v>
+      <c r="E77" s="3" t="s">
+        <v>893</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G77" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H77" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I77" s="18">
+        <v>735</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H77" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I77" s="17">
         <v>43008</v>
       </c>
-      <c r="J77" s="18">
+      <c r="J77" s="17">
         <v>42948</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>894</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
@@ -5423,26 +5952,29 @@
       <c r="C78" s="14">
         <v>1</v>
       </c>
-      <c r="D78" s="15">
+      <c r="D78" s="8">
         <v>3</v>
       </c>
-      <c r="E78" s="16" t="s">
-        <v>819</v>
+      <c r="E78" s="15" t="s">
+        <v>895</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G78" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G78" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I78" s="18">
+        <v>744</v>
+      </c>
+      <c r="I78" s="17">
         <v>42704</v>
       </c>
-      <c r="J78" s="18">
+      <c r="J78" s="17">
         <v>42614</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>896</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
@@ -5452,36 +5984,39 @@
       <c r="B79" s="14">
         <v>1</v>
       </c>
-      <c r="C79" s="15">
+      <c r="C79" s="8">
         <v>21</v>
       </c>
       <c r="D79" s="14">
         <v>22</v>
       </c>
-      <c r="E79" s="16" t="s">
-        <v>820</v>
+      <c r="E79" s="15" t="s">
+        <v>897</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G79" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H79" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I79" s="18">
+        <v>735</v>
+      </c>
+      <c r="G79" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H79" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I79" s="17">
         <v>43281</v>
       </c>
-      <c r="J79" s="18">
+      <c r="J79" s="17">
         <v>43221</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>898</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="37.5">
       <c r="A80" s="14">
         <v>80</v>
       </c>
-      <c r="B80" s="15">
+      <c r="B80" s="8">
         <v>1</v>
       </c>
       <c r="C80" s="14">
@@ -5491,26 +6026,29 @@
         <v>14</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>821</v>
+        <v>899</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G80" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H80" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I80" s="18">
+        <v>735</v>
+      </c>
+      <c r="G80" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H80" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I80" s="17">
         <v>43039</v>
       </c>
-      <c r="J80" s="18">
+      <c r="J80" s="17">
         <v>42948</v>
       </c>
+      <c r="K80" s="3" t="s">
+        <v>900</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
-      <c r="A81" s="15">
+      <c r="A81" s="8">
         <v>81</v>
       </c>
       <c r="B81" s="14">
@@ -5522,23 +6060,26 @@
       <c r="D81" s="14">
         <v>47</v>
       </c>
-      <c r="E81" s="16" t="s">
-        <v>822</v>
+      <c r="E81" s="15" t="s">
+        <v>901</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G81" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="I81" s="18">
+        <v>735</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="I81" s="17">
         <v>44043</v>
       </c>
-      <c r="J81" s="18">
+      <c r="J81" s="17">
         <v>43952</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>902</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
@@ -5554,23 +6095,26 @@
       <c r="D82" s="14">
         <v>43</v>
       </c>
-      <c r="E82" s="16" t="s">
-        <v>823</v>
+      <c r="E82" s="15" t="s">
+        <v>903</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="H82" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I82" s="18">
+        <v>735</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="H82" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I82" s="17">
         <v>43921</v>
       </c>
-      <c r="J82" s="18">
+      <c r="J82" s="17">
         <v>43831</v>
+      </c>
+      <c r="K82" s="3" t="s">
+        <v>904</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
@@ -5586,23 +6130,26 @@
       <c r="D83" s="14">
         <v>44</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>824</v>
+      <c r="E83" s="3" t="s">
+        <v>905</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G83" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="H83" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I83" s="18">
+        <v>735</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="I83" s="17">
         <v>43951</v>
       </c>
-      <c r="J83" s="18">
+      <c r="J83" s="17">
         <v>43891</v>
+      </c>
+      <c r="K83" s="3" t="s">
+        <v>906</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="37.5">
@@ -5615,26 +6162,29 @@
       <c r="C84" s="14">
         <v>31</v>
       </c>
-      <c r="D84" s="15">
+      <c r="D84" s="8">
         <v>64</v>
       </c>
-      <c r="E84" s="16" t="s">
-        <v>825</v>
+      <c r="E84" s="15" t="s">
+        <v>907</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G84" s="16" t="s">
-        <v>740</v>
+        <v>735</v>
+      </c>
+      <c r="G84" s="15" t="s">
+        <v>743</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="I84" s="18">
+        <v>751</v>
+      </c>
+      <c r="I84" s="17">
         <v>44561</v>
       </c>
-      <c r="J84" s="18">
+      <c r="J84" s="17">
         <v>43525</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>908</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
@@ -5644,29 +6194,32 @@
       <c r="B85" s="14">
         <v>2</v>
       </c>
-      <c r="C85" s="15">
+      <c r="C85" s="8">
         <v>65</v>
       </c>
       <c r="D85" s="14">
         <v>78</v>
       </c>
-      <c r="E85" s="16" t="s">
-        <v>826</v>
+      <c r="E85" s="15" t="s">
+        <v>909</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G85" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G85" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="I85" s="18">
+        <v>737</v>
+      </c>
+      <c r="I85" s="17">
         <v>44985</v>
       </c>
-      <c r="J85" s="18">
+      <c r="J85" s="17">
         <v>44562</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>910</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
@@ -5683,22 +6236,25 @@
         <v>78</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>827</v>
+        <v>911</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G86" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G86" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I86" s="18">
+        <v>744</v>
+      </c>
+      <c r="I86" s="17">
         <v>44985</v>
       </c>
-      <c r="J86" s="18">
+      <c r="J86" s="17">
         <v>44562</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>912</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -5715,22 +6271,25 @@
         <v>57</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>828</v>
+        <v>913</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G87" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G87" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="I87" s="18">
+        <v>737</v>
+      </c>
+      <c r="I87" s="17">
         <v>44347</v>
       </c>
-      <c r="J87" s="18">
+      <c r="J87" s="17">
         <v>44287</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>914</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
@@ -5747,22 +6306,25 @@
         <v>71</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>829</v>
+        <v>915</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G88" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="I88" s="18">
+        <v>737</v>
+      </c>
+      <c r="I88" s="17">
         <v>44773</v>
       </c>
-      <c r="J88" s="18">
+      <c r="J88" s="17">
         <v>44682</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>916</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
@@ -5780,17 +6342,20 @@
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G89" s="16" t="s">
-        <v>743</v>
+        <v>735</v>
+      </c>
+      <c r="G89" s="15" t="s">
+        <v>747</v>
       </c>
       <c r="H89" s="2"/>
-      <c r="I89" s="18">
+      <c r="I89" s="17">
         <v>44865</v>
       </c>
-      <c r="J89" s="18">
+      <c r="J89" s="17">
         <v>44835</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>917</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
@@ -5808,17 +6373,20 @@
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G90" s="16" t="s">
-        <v>743</v>
+        <v>735</v>
+      </c>
+      <c r="G90" s="15" t="s">
+        <v>747</v>
       </c>
       <c r="H90" s="2"/>
-      <c r="I90" s="18">
+      <c r="I90" s="17">
         <v>44865</v>
       </c>
-      <c r="J90" s="18">
+      <c r="J90" s="17">
         <v>44835</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>918</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
@@ -5834,17 +6402,20 @@
       <c r="D91" s="14"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G91" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G91" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H91" s="2"/>
-      <c r="I91" s="18" t="s">
-        <v>802</v>
-      </c>
-      <c r="J91" s="18">
+      <c r="I91" s="17" t="s">
+        <v>862</v>
+      </c>
+      <c r="J91" s="17">
         <v>44652</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>919</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
@@ -5861,20 +6432,23 @@
         <v>44</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>830</v>
+        <v>920</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G92" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G92" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H92" s="2"/>
-      <c r="I92" s="18">
+      <c r="I92" s="17">
         <v>43951</v>
       </c>
-      <c r="J92" s="18">
+      <c r="J92" s="17">
         <v>43070</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>921</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
@@ -5892,17 +6466,20 @@
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G93" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G93" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H93" s="2"/>
-      <c r="I93" s="18">
+      <c r="I93" s="17">
         <v>43373</v>
       </c>
-      <c r="J93" s="18">
+      <c r="J93" s="17">
         <v>43344</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>922</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="37.5">
@@ -5919,22 +6496,25 @@
         <v>20</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>831</v>
+        <v>923</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G94" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G94" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I94" s="18">
+        <v>744</v>
+      </c>
+      <c r="I94" s="17">
         <v>43220</v>
       </c>
-      <c r="J94" s="18">
+      <c r="J94" s="17">
         <v>43040</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>924</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="37.5">
@@ -5951,22 +6531,25 @@
         <v>25</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>832</v>
+        <v>925</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G95" s="16" t="s">
-        <v>833</v>
+        <v>735</v>
+      </c>
+      <c r="G95" s="15" t="s">
+        <v>926</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I95" s="18">
+        <v>744</v>
+      </c>
+      <c r="I95" s="17">
         <v>43373</v>
       </c>
-      <c r="J95" s="18">
+      <c r="J95" s="17">
         <v>43344</v>
+      </c>
+      <c r="K95" s="3" t="s">
+        <v>927</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
@@ -5983,20 +6566,23 @@
         <v>78</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>834</v>
+        <v>928</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G96" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G96" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H96" s="2"/>
-      <c r="I96" s="18">
+      <c r="I96" s="17">
         <v>44985</v>
       </c>
-      <c r="J96" s="18">
+      <c r="J96" s="17">
         <v>44866</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>929</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
@@ -6013,22 +6599,25 @@
         <v>75</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>835</v>
+        <v>930</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G97" s="16" t="s">
-        <v>760</v>
+        <v>735</v>
+      </c>
+      <c r="G97" s="15" t="s">
+        <v>780</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>836</v>
-      </c>
-      <c r="I97" s="18">
+        <v>931</v>
+      </c>
+      <c r="I97" s="17">
         <v>44895</v>
       </c>
-      <c r="J97" s="18">
+      <c r="J97" s="17">
         <v>43344</v>
+      </c>
+      <c r="K97" s="3" t="s">
+        <v>932</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
@@ -6046,17 +6635,20 @@
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G98" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H98" s="2"/>
-      <c r="I98" s="18">
+      <c r="I98" s="17">
         <v>43281</v>
       </c>
-      <c r="J98" s="18">
+      <c r="J98" s="17">
         <v>43252</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>933</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
@@ -6074,17 +6666,20 @@
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="G99" s="16" t="s">
-        <v>813</v>
+        <v>735</v>
+      </c>
+      <c r="G99" s="15" t="s">
+        <v>883</v>
       </c>
       <c r="H99" s="2"/>
-      <c r="I99" s="18">
+      <c r="I99" s="17">
         <v>42916</v>
       </c>
-      <c r="J99" s="18">
+      <c r="J99" s="17">
         <v>42887</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>934</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
@@ -6106,15 +6701,18 @@
       <c r="F100" s="2" t="s">
         <v>729</v>
       </c>
-      <c r="G100" s="16" t="s">
+      <c r="G100" s="15" t="s">
         <v>729</v>
       </c>
       <c r="H100" s="2"/>
-      <c r="I100" s="18">
+      <c r="I100" s="17">
         <v>42794</v>
       </c>
-      <c r="J100" s="18">
+      <c r="J100" s="17">
         <v>42675</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added config validator+compiler,need to integrate
</commit_message>
<xml_diff>
--- a/src/data/activity_data.xlsx
+++ b/src/data/activity_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4426" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4424" uniqueCount="935">
   <si>
     <t>S_ID</t>
   </si>
@@ -2233,9 +2233,6 @@
   </si>
   <si>
     <t>Transdisciplinary</t>
-  </si>
-  <si>
-    <t>2019-05-31</t>
   </si>
   <si>
     <t/>
@@ -2611,175 +2608,175 @@
     <t>Assessment and quantification of the water use efficiency and management on resource use in participating schools</t>
   </si>
   <si>
+    <t>2,1,14</t>
+  </si>
+  <si>
+    <t>Study investigating how future worst-case scenario climate change will impact on the timing and quantity of streamflow at 130 catchment accross the UK and Ireland (currently England, Wales, Ireland &amp; Northern Ireland), and the knock-on implications of such changes for water abstraction at 420 hydropower locations.</t>
+  </si>
+  <si>
+    <t>13,5,25</t>
+  </si>
+  <si>
+    <t>Journal article based upon a conference paper presented at IPDMC 2020.  Describe and reflect on the actions undertaken by a network of stakeholders to co-generate learning from green process innovation.</t>
+  </si>
+  <si>
+    <t>2,16,22</t>
+  </si>
+  <si>
+    <t>Study investigating cost-effectiveness and emissions savings from replacing conventional heating systems (gas, oil, electricity, LPG and coal) to low-carbon heating systems (ASHP, GSHP, biomass boilers solar PV)</t>
+  </si>
+  <si>
+    <t>1,2,12</t>
+  </si>
+  <si>
+    <t>We carried out a focus group with a gropu of transition year students to develop the materials for the hackathon porgamme</t>
+  </si>
+  <si>
+    <t>3,4,15</t>
+  </si>
+  <si>
+    <t>Journal article investigating economic and environmental efficiency of water and sewage companes, with a focus on appropriate methodologies and the factors affecting performance</t>
+  </si>
+  <si>
+    <t>2,6,7,8,18</t>
+  </si>
+  <si>
+    <t>Journal article investigating energy and economic efficiency across water and sewage and water-only companies. Additional focus on assessing how common proxy indicators performed vs. best available</t>
+  </si>
+  <si>
+    <t>1,3,4,5,15</t>
+  </si>
+  <si>
+    <t>Journal article investigating the productivity of the UK water sector over a 6 year period using metrics based on a wider sustainability perspective.</t>
+  </si>
+  <si>
+    <t>2,1,15</t>
+  </si>
+  <si>
+    <t>Journal article evaluating the energy consumption of wastewater utilities across the globe</t>
+  </si>
+  <si>
+    <t>13,5,26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal article investigating the efficiency of water and sewage, communication, and energy utilties </t>
+  </si>
+  <si>
+    <t>2,16,23</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Ballacolla GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>1,2,13</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Blackstairs GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>3,4,16</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Ballinabrannagh GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>2,6,7,8,19</t>
+  </si>
+  <si>
+    <t>Analysis of the water network operated by the Kilanerin GWS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>1,3,4,5,16</t>
+  </si>
+  <si>
+    <t>Analysis of three water networks operated by EPS to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>2,1,16</t>
+  </si>
+  <si>
+    <t>Analysis of a series of water networks and roadside culverts owned by the Blaenau Gwent municipality to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>13,5,27</t>
+  </si>
+  <si>
+    <t>Analysis of the outfall of the Five Fords WWTP operated by Welsh Water to assess the potential for hydro energy recovery and produce a preliminary design of the hydro site</t>
+  </si>
+  <si>
+    <t>2,16,24</t>
+  </si>
+  <si>
+    <t>Analysis of the Dodder water supply line operated by Dublin City Council on behalf of Irish Water to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>1,2,14</t>
+  </si>
+  <si>
+    <t>Preliminary design of a picoturbine at the inlet of a storage tank in the Blackstairs GWS</t>
+  </si>
+  <si>
+    <t>3,4,17</t>
+  </si>
+  <si>
+    <t>Analysis of a pressure reducing station at Boliden Tara Mines to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>2,6,7,8,20</t>
+  </si>
+  <si>
+    <t>Analysis of the outfall of the Dairygold WWTP to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>1,3,4,5,17</t>
+  </si>
+  <si>
+    <t>Analysis of the inlet of the Fethard WTP to assess the potential for hydro energy recovery</t>
+  </si>
+  <si>
+    <t>2,1,17</t>
+  </si>
+  <si>
+    <t>Publication of the research on the development of a heat recovery toolkit for commercial kitchen owners (pubs, restaurants, cafes, canteens etc.) whcich enables them to get an estimate on their individual heat recovery potential from drain water, environmental and cost savings (or trade-offs).</t>
+  </si>
+  <si>
+    <t>13,5,28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assess the feasibility of installaing a DWHR system at the Imperial Hotel, Llandudno </t>
+  </si>
+  <si>
+    <t>2,16,25</t>
+  </si>
+  <si>
+    <t>Study investigating the impact of variation in abstraction licence conditions between England, Wales, Scotland, Northern Ireland, and Ireland on water abstraction for run-of-river hydropower. Study looks at the lost abstraction, and therefore power generation both historically (1985-2015) and for future worst-cast scenario climate change (RCP8.5) affected flows (2021-2080)</t>
+  </si>
+  <si>
+    <t>1,2,15</t>
+  </si>
+  <si>
+    <t>Hydrological modelling work completed for the Talybont Community Flood Group to identify sub-catchments upstream of the village that are contributing the most to peak flows. Also studied was the impact of tree planting on reducing these peak flood flows.</t>
+  </si>
+  <si>
+    <t>3,4,18</t>
+  </si>
+  <si>
+    <t>Consultation work for Aber Falls distillery on how to lower their environmental footprint with focus on energy, water use and by-product use.</t>
+  </si>
+  <si>
+    <t>2,6,7,8,21</t>
+  </si>
+  <si>
+    <t>1,3,4,5,18</t>
+  </si>
+  <si>
+    <t>2,1,18</t>
+  </si>
+  <si>
     <t>undefined</t>
-  </si>
-  <si>
-    <t>2,1,14</t>
-  </si>
-  <si>
-    <t>Study investigating how future worst-case scenario climate change will impact on the timing and quantity of streamflow at 130 catchment accross the UK and Ireland (currently England, Wales, Ireland &amp; Northern Ireland), and the knock-on implications of such changes for water abstraction at 420 hydropower locations.</t>
-  </si>
-  <si>
-    <t>13,5,25</t>
-  </si>
-  <si>
-    <t>Journal article based upon a conference paper presented at IPDMC 2020.  Describe and reflect on the actions undertaken by a network of stakeholders to co-generate learning from green process innovation.</t>
-  </si>
-  <si>
-    <t>2,16,22</t>
-  </si>
-  <si>
-    <t>Study investigating cost-effectiveness and emissions savings from replacing conventional heating systems (gas, oil, electricity, LPG and coal) to low-carbon heating systems (ASHP, GSHP, biomass boilers solar PV)</t>
-  </si>
-  <si>
-    <t>1,2,12</t>
-  </si>
-  <si>
-    <t>We carried out a focus group with a gropu of transition year students to develop the materials for the hackathon porgamme</t>
-  </si>
-  <si>
-    <t>3,4,15</t>
-  </si>
-  <si>
-    <t>Journal article investigating economic and environmental efficiency of water and sewage companes, with a focus on appropriate methodologies and the factors affecting performance</t>
-  </si>
-  <si>
-    <t>2,6,7,8,18</t>
-  </si>
-  <si>
-    <t>Journal article investigating energy and economic efficiency across water and sewage and water-only companies. Additional focus on assessing how common proxy indicators performed vs. best available</t>
-  </si>
-  <si>
-    <t>1,3,4,5,15</t>
-  </si>
-  <si>
-    <t>Journal article investigating the productivity of the UK water sector over a 6 year period using metrics based on a wider sustainability perspective.</t>
-  </si>
-  <si>
-    <t>2,1,15</t>
-  </si>
-  <si>
-    <t>Journal article evaluating the energy consumption of wastewater utilities across the globe</t>
-  </si>
-  <si>
-    <t>13,5,26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journal article investigating the efficiency of water and sewage, communication, and energy utilties </t>
-  </si>
-  <si>
-    <t>2,16,23</t>
-  </si>
-  <si>
-    <t>Analysis of the water network operated by the Ballacolla GWS to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>Study</t>
-  </si>
-  <si>
-    <t>1,2,13</t>
-  </si>
-  <si>
-    <t>Analysis of the water network operated by the Blackstairs GWS to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>3,4,16</t>
-  </si>
-  <si>
-    <t>Analysis of the water network operated by the Ballinabrannagh GWS to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>2,6,7,8,19</t>
-  </si>
-  <si>
-    <t>Analysis of the water network operated by the Kilanerin GWS to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>1,3,4,5,16</t>
-  </si>
-  <si>
-    <t>Analysis of three water networks operated by EPS to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>2,1,16</t>
-  </si>
-  <si>
-    <t>Analysis of a series of water networks and roadside culverts owned by the Blaenau Gwent municipality to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>13,5,27</t>
-  </si>
-  <si>
-    <t>Analysis of the outfall of the Five Fords WWTP operated by Welsh Water to assess the potential for hydro energy recovery and produce a preliminary design of the hydro site</t>
-  </si>
-  <si>
-    <t>2,16,24</t>
-  </si>
-  <si>
-    <t>Analysis of the Dodder water supply line operated by Dublin City Council on behalf of Irish Water to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>1,2,14</t>
-  </si>
-  <si>
-    <t>Preliminary design of a picoturbine at the inlet of a storage tank in the Blackstairs GWS</t>
-  </si>
-  <si>
-    <t>3,4,17</t>
-  </si>
-  <si>
-    <t>Analysis of a pressure reducing station at Boliden Tara Mines to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>2,6,7,8,20</t>
-  </si>
-  <si>
-    <t>Analysis of the outfall of the Dairygold WWTP to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>1,3,4,5,17</t>
-  </si>
-  <si>
-    <t>Analysis of the inlet of the Fethard WTP to assess the potential for hydro energy recovery</t>
-  </si>
-  <si>
-    <t>2,1,17</t>
-  </si>
-  <si>
-    <t>Publication of the research on the development of a heat recovery toolkit for commercial kitchen owners (pubs, restaurants, cafes, canteens etc.) whcich enables them to get an estimate on their individual heat recovery potential from drain water, environmental and cost savings (or trade-offs).</t>
-  </si>
-  <si>
-    <t>13,5,28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assess the feasibility of installaing a DWHR system at the Imperial Hotel, Llandudno </t>
-  </si>
-  <si>
-    <t>2,16,25</t>
-  </si>
-  <si>
-    <t>Study investigating the impact of variation in abstraction licence conditions between England, Wales, Scotland, Northern Ireland, and Ireland on water abstraction for run-of-river hydropower. Study looks at the lost abstraction, and therefore power generation both historically (1985-2015) and for future worst-cast scenario climate change (RCP8.5) affected flows (2021-2080)</t>
-  </si>
-  <si>
-    <t>1,2,15</t>
-  </si>
-  <si>
-    <t>Hydrological modelling work completed for the Talybont Community Flood Group to identify sub-catchments upstream of the village that are contributing the most to peak flows. Also studied was the impact of tree planting on reducing these peak flood flows.</t>
-  </si>
-  <si>
-    <t>3,4,18</t>
-  </si>
-  <si>
-    <t>Consultation work for Aber Falls distillery on how to lower their environmental footprint with focus on energy, water use and by-product use.</t>
-  </si>
-  <si>
-    <t>2,6,7,8,21</t>
-  </si>
-  <si>
-    <t>1,3,4,5,18</t>
-  </si>
-  <si>
-    <t>2,1,18</t>
   </si>
   <si>
     <t>13,5,29</t>
@@ -2939,10 +2936,10 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -3338,12 +3335,10 @@
       <c r="I2" s="17" t="s">
         <v>738</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="18">
         <v>42614</v>
       </c>
-      <c r="K2" s="18" t="s">
-        <v>739</v>
-      </c>
+      <c r="K2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="8">
@@ -3359,7 +3354,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>735</v>
@@ -3370,14 +3365,14 @@
       <c r="H3" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="18">
         <v>43799</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="18">
         <v>42614</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -3394,25 +3389,25 @@
         <v>26</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>743</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="18">
+        <v>43404</v>
+      </c>
+      <c r="J4" s="18">
+        <v>42614</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>744</v>
-      </c>
-      <c r="I4" s="17">
-        <v>43404</v>
-      </c>
-      <c r="J4" s="17">
-        <v>42614</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>745</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -3429,25 +3424,25 @@
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="18">
         <v>44561</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="18">
         <v>44317</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -3464,25 +3459,25 @@
         <v>33</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G6" s="15" t="s">
+        <v>742</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I6" s="17">
+      <c r="I6" s="18">
         <v>43616</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="18">
         <v>42614</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -3499,25 +3494,25 @@
         <v>54</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H7" s="15" t="s">
+        <v>750</v>
+      </c>
+      <c r="I7" s="18">
+        <v>44255</v>
+      </c>
+      <c r="J7" s="18">
+        <v>44228</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>751</v>
-      </c>
-      <c r="I7" s="17">
-        <v>44255</v>
-      </c>
-      <c r="J7" s="17">
-        <v>44228</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>752</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -3534,23 +3529,23 @@
         <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H8" s="14"/>
-      <c r="I8" s="17">
+      <c r="I8" s="18">
         <v>44500</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="18">
         <v>43739</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -3567,7 +3562,7 @@
         <v>78</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>735</v>
@@ -3576,14 +3571,14 @@
         <v>736</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="17">
+      <c r="I9" s="18">
         <v>44985</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="18">
         <v>43586</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -3600,23 +3595,23 @@
         <v>29</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H10" s="14"/>
-      <c r="I10" s="17">
+      <c r="I10" s="18">
         <v>43496</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="18">
         <v>42614</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -3633,26 +3628,26 @@
         <v>35</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H11" s="14"/>
-      <c r="I11" s="17">
+      <c r="I11" s="18">
         <v>43677</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="18">
         <v>42614</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="37.5">
+        <v>758</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -3666,26 +3661,26 @@
         <v>40</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="17">
+      <c r="I12" s="18">
         <v>43830</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="18">
         <v>42614</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="87">
+        <v>760</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -3699,7 +3694,7 @@
         <v>42</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>735</v>
@@ -3710,17 +3705,17 @@
       <c r="H13" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="18">
         <v>43890</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="18">
         <v>42614</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="114">
+        <v>762</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -3734,7 +3729,7 @@
         <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>735</v>
@@ -3743,19 +3738,19 @@
         <v>736</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I14" s="17">
+        <v>750</v>
+      </c>
+      <c r="I14" s="18">
         <v>44985</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="18">
         <v>43862</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="181.5">
+        <v>764</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -3769,25 +3764,25 @@
         <v>55</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="I15" s="17">
+        <v>750</v>
+      </c>
+      <c r="I15" s="18">
         <v>44286</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="18">
         <v>44256</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33">
@@ -3804,25 +3799,25 @@
         <v>55</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>750</v>
+      </c>
+      <c r="I16" s="18">
+        <v>44286</v>
+      </c>
+      <c r="J16" s="18">
+        <v>43525</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>769</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I16" s="17">
-        <v>44286</v>
-      </c>
-      <c r="J16" s="17">
-        <v>43525</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>770</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="37.5">
@@ -3839,25 +3834,25 @@
         <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I17" s="17">
+        <v>750</v>
+      </c>
+      <c r="I17" s="18">
         <v>44043</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="18">
         <v>43282</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="100.5">
@@ -3874,25 +3869,25 @@
         <v>64</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G18" s="15" t="s">
+        <v>742</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I18" s="17">
+      <c r="I18" s="18">
         <v>44561</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="18">
         <v>43647</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="37.5">
@@ -3909,25 +3904,25 @@
         <v>74</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I19" s="17">
+        <v>750</v>
+      </c>
+      <c r="I19" s="18">
         <v>44865</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="18">
         <v>43525</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="141">
@@ -3944,25 +3939,25 @@
         <v>62</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H20" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="18">
         <v>44500</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="18">
         <v>44470</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="114">
@@ -3979,25 +3974,25 @@
         <v>78</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G21" s="15" t="s">
+        <v>779</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="I21" s="18">
+        <v>44985</v>
+      </c>
+      <c r="J21" s="18">
+        <v>44197</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>780</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="I21" s="17">
-        <v>44985</v>
-      </c>
-      <c r="J21" s="17">
-        <v>44197</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>781</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="100.5">
@@ -4014,25 +4009,25 @@
         <v>18</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I22" s="17">
+        <v>743</v>
+      </c>
+      <c r="I22" s="18">
         <v>43159</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="18">
         <v>42614</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="127.5">
@@ -4049,25 +4044,25 @@
         <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I23" s="17">
+        <v>743</v>
+      </c>
+      <c r="I23" s="18">
         <v>44196</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="18">
         <v>43160</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="168">
@@ -4084,25 +4079,25 @@
         <v>47</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I24" s="17">
+        <v>743</v>
+      </c>
+      <c r="I24" s="18">
         <v>44043</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="18">
         <v>43132</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="60">
@@ -4119,25 +4114,25 @@
         <v>64</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="18">
         <v>44561</v>
       </c>
-      <c r="J25" s="17">
+      <c r="J25" s="18">
         <v>44317</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="168">
@@ -4154,7 +4149,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>735</v>
@@ -4165,14 +4160,14 @@
       <c r="H26" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="18">
         <v>44985</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="18">
         <v>42614</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="87">
@@ -4189,25 +4184,25 @@
         <v>39</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="18">
         <v>43799</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J27" s="18">
         <v>43770</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="87">
@@ -4224,25 +4219,25 @@
         <v>78</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H28" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I28" s="17">
+      <c r="I28" s="18">
         <v>44985</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="18">
         <v>42614</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="114">
@@ -4259,25 +4254,25 @@
         <v>78</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G29" s="15" t="s">
+        <v>796</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>750</v>
+      </c>
+      <c r="I29" s="18">
+        <v>44985</v>
+      </c>
+      <c r="J29" s="18">
+        <v>42614</v>
+      </c>
+      <c r="K29" s="3" t="s">
         <v>797</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I29" s="17">
-        <v>44985</v>
-      </c>
-      <c r="J29" s="17">
-        <v>42614</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>798</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
@@ -4294,25 +4289,25 @@
         <v>78</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="I30" s="17">
+        <v>750</v>
+      </c>
+      <c r="I30" s="18">
         <v>44985</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30" s="18">
         <v>44228</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -4329,25 +4324,25 @@
         <v>33</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H31" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I31" s="17">
+      <c r="I31" s="18">
         <v>43616</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="18">
         <v>43586</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
@@ -4364,23 +4359,23 @@
         <v>78</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H32" s="14"/>
-      <c r="I32" s="17">
+      <c r="I32" s="18">
         <v>44985</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J32" s="18">
         <v>44470</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
@@ -4397,23 +4392,23 @@
         <v>78</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="17">
+      <c r="I33" s="18">
         <v>44985</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J33" s="18">
         <v>44470</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
@@ -4430,26 +4425,24 @@
         <v>52</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I34" s="17">
+        <v>750</v>
+      </c>
+      <c r="I34" s="18">
         <v>44196</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="18">
         <v>42614</v>
       </c>
-      <c r="K34" s="18" t="s">
-        <v>739</v>
-      </c>
+      <c r="K34" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="14">
@@ -4465,23 +4458,23 @@
         <v>63</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H35" s="14"/>
-      <c r="I35" s="17">
+      <c r="I35" s="18">
         <v>44530</v>
       </c>
-      <c r="J35" s="17">
+      <c r="J35" s="18">
         <v>44501</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
@@ -4498,25 +4491,25 @@
         <v>42</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="I36" s="17">
+        <v>750</v>
+      </c>
+      <c r="I36" s="18">
         <v>43890</v>
       </c>
-      <c r="J36" s="17">
+      <c r="J36" s="18">
         <v>43497</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
@@ -4533,25 +4526,25 @@
         <v>54</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H37" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I37" s="17">
+      <c r="I37" s="18">
         <v>44255</v>
       </c>
-      <c r="J37" s="17">
+      <c r="J37" s="18">
         <v>44228</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
@@ -4568,25 +4561,25 @@
         <v>78</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I38" s="17">
+        <v>750</v>
+      </c>
+      <c r="I38" s="18">
         <v>44985</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J38" s="18">
         <v>43891</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
@@ -4603,25 +4596,25 @@
         <v>70</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I39" s="18">
         <v>44742</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="18">
         <v>43891</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
@@ -4638,25 +4631,25 @@
         <v>49</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I40" s="17">
+        <v>750</v>
+      </c>
+      <c r="I40" s="18">
         <v>44104</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="18">
         <v>43891</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
@@ -4673,25 +4666,25 @@
         <v>78</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I41" s="17">
+        <v>750</v>
+      </c>
+      <c r="I41" s="18">
         <v>44985</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J41" s="18">
         <v>44256</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
@@ -4708,25 +4701,25 @@
         <v>78</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="I42" s="17">
+      <c r="I42" s="18">
         <v>44985</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J42" s="18">
         <v>44621</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
@@ -4743,25 +4736,25 @@
         <v>55</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H43" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I43" s="17">
+      <c r="I43" s="18">
         <v>44286</v>
       </c>
-      <c r="J43" s="17">
+      <c r="J43" s="18">
         <v>44256</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
@@ -4778,7 +4771,7 @@
         <v>78</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>735</v>
@@ -4787,16 +4780,16 @@
         <v>120</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I44" s="17">
+        <v>743</v>
+      </c>
+      <c r="I44" s="18">
         <v>44985</v>
       </c>
-      <c r="J44" s="17">
+      <c r="J44" s="18">
         <v>44440</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
@@ -4813,7 +4806,7 @@
         <v>78</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>735</v>
@@ -4824,14 +4817,14 @@
       <c r="H45" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="I45" s="17">
+      <c r="I45" s="18">
         <v>44985</v>
       </c>
-      <c r="J45" s="17">
+      <c r="J45" s="18">
         <v>43221</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -4848,7 +4841,7 @@
         <v>78</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>735</v>
@@ -4859,14 +4852,14 @@
       <c r="H46" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I46" s="17">
+      <c r="I46" s="18">
         <v>44985</v>
       </c>
-      <c r="J46" s="17">
+      <c r="J46" s="18">
         <v>43831</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
@@ -4883,25 +4876,25 @@
         <v>56</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I47" s="17">
+        <v>750</v>
+      </c>
+      <c r="I47" s="18">
         <v>44316</v>
       </c>
-      <c r="J47" s="17">
+      <c r="J47" s="18">
         <v>44287</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -4918,25 +4911,25 @@
         <v>78</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="I48" s="17">
+      <c r="I48" s="18">
         <v>44985</v>
       </c>
-      <c r="J48" s="17">
+      <c r="J48" s="18">
         <v>44562</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -4953,25 +4946,25 @@
         <v>64</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H49" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I49" s="17">
+      <c r="I49" s="18">
         <v>44561</v>
       </c>
-      <c r="J49" s="17">
+      <c r="J49" s="18">
         <v>44531</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -4988,25 +4981,25 @@
         <v>68</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I50" s="17">
+        <v>750</v>
+      </c>
+      <c r="I50" s="18">
         <v>44681</v>
       </c>
-      <c r="J50" s="17">
+      <c r="J50" s="18">
         <v>44652</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
@@ -5023,25 +5016,25 @@
         <v>2</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="I51" s="17">
+      <c r="I51" s="18">
         <v>42674</v>
       </c>
-      <c r="J51" s="17">
+      <c r="J51" s="18">
         <v>42644</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
@@ -5058,25 +5051,25 @@
         <v>14</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H52" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I52" s="17">
+      <c r="I52" s="18">
         <v>43039</v>
       </c>
-      <c r="J52" s="17">
+      <c r="J52" s="18">
         <v>43009</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="409.6000000000001">
@@ -5093,25 +5086,25 @@
         <v>18</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H53" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I53" s="17">
+      <c r="I53" s="18">
         <v>43159</v>
       </c>
-      <c r="J53" s="17">
+      <c r="J53" s="18">
         <v>43132</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="100.5">
@@ -5128,25 +5121,25 @@
         <v>20</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="I54" s="17">
+      <c r="I54" s="18">
         <v>43220</v>
       </c>
-      <c r="J54" s="17">
+      <c r="J54" s="18">
         <v>43191</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
@@ -5163,25 +5156,25 @@
         <v>26</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H55" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="I55" s="17">
+      <c r="I55" s="18">
         <v>43404</v>
       </c>
-      <c r="J55" s="17">
+      <c r="J55" s="18">
         <v>43374</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
@@ -5198,25 +5191,25 @@
         <v>78</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I56" s="17">
+        <v>750</v>
+      </c>
+      <c r="I56" s="18">
         <v>44985</v>
       </c>
-      <c r="J56" s="17">
+      <c r="J56" s="18">
         <v>44562</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
@@ -5233,25 +5226,25 @@
         <v>78</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="I57" s="17">
+        <v>750</v>
+      </c>
+      <c r="I57" s="18">
         <v>44985</v>
       </c>
-      <c r="J57" s="17">
+      <c r="J57" s="18">
         <v>44409</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
@@ -5268,25 +5261,25 @@
         <v>60</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I58" s="17">
+        <v>750</v>
+      </c>
+      <c r="I58" s="18">
         <v>44439</v>
       </c>
-      <c r="J58" s="17">
+      <c r="J58" s="18">
         <v>44348</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="409.6000000000001">
@@ -5303,25 +5296,25 @@
         <v>58</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I59" s="17">
+        <v>750</v>
+      </c>
+      <c r="I59" s="18">
         <v>44377</v>
       </c>
-      <c r="J59" s="17">
+      <c r="J59" s="18">
         <v>44287</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
@@ -5338,25 +5331,25 @@
         <v>78</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I60" s="17">
+        <v>743</v>
+      </c>
+      <c r="I60" s="18">
         <v>44985</v>
       </c>
-      <c r="J60" s="17">
+      <c r="J60" s="18">
         <v>44197</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
@@ -5373,23 +5366,23 @@
         <v>42</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H61" s="14"/>
-      <c r="I61" s="17">
+      <c r="I61" s="18">
         <v>43890</v>
       </c>
-      <c r="J61" s="17">
+      <c r="J61" s="18">
         <v>43497</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
@@ -5402,23 +5395,23 @@
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H62" s="14"/>
       <c r="I62" s="17" t="s">
-        <v>862</v>
+        <v>738</v>
       </c>
       <c r="J62" s="17" t="s">
-        <v>862</v>
+        <v>738</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
@@ -5435,23 +5428,23 @@
         <v>52</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H63" s="3"/>
-      <c r="I63" s="17">
+      <c r="I63" s="18">
         <v>44196</v>
       </c>
-      <c r="J63" s="17">
+      <c r="J63" s="18">
         <v>43160</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
@@ -5468,25 +5461,25 @@
         <v>66</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I64" s="17">
+        <v>750</v>
+      </c>
+      <c r="I64" s="18">
         <v>44620</v>
       </c>
-      <c r="J64" s="17">
+      <c r="J64" s="18">
         <v>43983</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="262.5">
@@ -5503,23 +5496,23 @@
         <v>62</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H65" s="14"/>
-      <c r="I65" s="17">
+      <c r="I65" s="18">
         <v>44500</v>
       </c>
-      <c r="J65" s="17">
+      <c r="J65" s="18">
         <v>44105</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
@@ -5536,25 +5529,25 @@
         <v>68</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="I66" s="17">
+      <c r="I66" s="18">
         <v>44681</v>
       </c>
-      <c r="J66" s="17">
+      <c r="J66" s="18">
         <v>44621</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
@@ -5571,25 +5564,25 @@
         <v>35</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I67" s="17">
+        <v>750</v>
+      </c>
+      <c r="I67" s="18">
         <v>43677</v>
       </c>
-      <c r="J67" s="17">
+      <c r="J67" s="18">
         <v>43009</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
@@ -5606,25 +5599,25 @@
         <v>49</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I68" s="17">
+        <v>750</v>
+      </c>
+      <c r="I68" s="18">
         <v>44104</v>
       </c>
-      <c r="J68" s="17">
+      <c r="J68" s="18">
         <v>43678</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
@@ -5641,25 +5634,25 @@
         <v>58</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="I69" s="17">
+        <v>750</v>
+      </c>
+      <c r="I69" s="18">
         <v>44377</v>
       </c>
-      <c r="J69" s="17">
+      <c r="J69" s="18">
         <v>44105</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
@@ -5676,25 +5669,25 @@
         <v>64</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G70" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="H70" s="15" t="s">
         <v>743</v>
       </c>
-      <c r="H70" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I70" s="17">
+      <c r="I70" s="18">
         <v>44561</v>
       </c>
-      <c r="J70" s="17">
+      <c r="J70" s="18">
         <v>44378</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="114">
@@ -5711,25 +5704,25 @@
         <v>74</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="I71" s="17">
+        <v>750</v>
+      </c>
+      <c r="I71" s="18">
         <v>44865</v>
       </c>
-      <c r="J71" s="17">
+      <c r="J71" s="18">
         <v>44562</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
@@ -5746,25 +5739,25 @@
         <v>9</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I72" s="17">
+        <v>743</v>
+      </c>
+      <c r="I72" s="18">
         <v>42886</v>
       </c>
-      <c r="J72" s="17">
+      <c r="J72" s="18">
         <v>42767</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
@@ -5781,25 +5774,25 @@
         <v>9</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I73" s="17">
+        <v>743</v>
+      </c>
+      <c r="I73" s="18">
         <v>42886</v>
       </c>
-      <c r="J73" s="17">
+      <c r="J73" s="18">
         <v>42767</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="37.5">
@@ -5816,25 +5809,25 @@
         <v>9</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I74" s="17">
+        <v>743</v>
+      </c>
+      <c r="I74" s="18">
         <v>42886</v>
       </c>
-      <c r="J74" s="17">
+      <c r="J74" s="18">
         <v>42767</v>
       </c>
       <c r="K74" s="3" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="37.5">
@@ -5851,25 +5844,25 @@
         <v>9</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="I75" s="17">
+        <v>743</v>
+      </c>
+      <c r="I75" s="18">
         <v>42886</v>
       </c>
-      <c r="J75" s="17">
+      <c r="J75" s="18">
         <v>42767</v>
       </c>
       <c r="K75" s="3" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
@@ -5886,25 +5879,25 @@
         <v>11</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I76" s="17">
+        <v>743</v>
+      </c>
+      <c r="I76" s="18">
         <v>42947</v>
       </c>
-      <c r="J76" s="17">
+      <c r="J76" s="18">
         <v>42856</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="37.5">
@@ -5921,25 +5914,25 @@
         <v>13</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I77" s="17">
+        <v>743</v>
+      </c>
+      <c r="I77" s="18">
         <v>43008</v>
       </c>
-      <c r="J77" s="17">
+      <c r="J77" s="18">
         <v>42948</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
@@ -5956,25 +5949,25 @@
         <v>3</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I78" s="17">
+        <v>743</v>
+      </c>
+      <c r="I78" s="18">
         <v>42704</v>
       </c>
-      <c r="J78" s="17">
+      <c r="J78" s="18">
         <v>42614</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
@@ -5991,25 +5984,25 @@
         <v>22</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I79" s="17">
+        <v>743</v>
+      </c>
+      <c r="I79" s="18">
         <v>43281</v>
       </c>
-      <c r="J79" s="17">
+      <c r="J79" s="18">
         <v>43221</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="37.5">
@@ -6026,25 +6019,25 @@
         <v>14</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I80" s="17">
+        <v>743</v>
+      </c>
+      <c r="I80" s="18">
         <v>43039</v>
       </c>
-      <c r="J80" s="17">
+      <c r="J80" s="18">
         <v>42948</v>
       </c>
       <c r="K80" s="3" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
@@ -6061,25 +6054,25 @@
         <v>47</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="I81" s="17">
+        <v>743</v>
+      </c>
+      <c r="I81" s="18">
         <v>44043</v>
       </c>
-      <c r="J81" s="17">
+      <c r="J81" s="18">
         <v>43952</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
@@ -6096,25 +6089,25 @@
         <v>43</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I82" s="17">
+        <v>743</v>
+      </c>
+      <c r="I82" s="18">
         <v>43921</v>
       </c>
-      <c r="J82" s="17">
+      <c r="J82" s="18">
         <v>43831</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
@@ -6131,25 +6124,25 @@
         <v>44</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="I83" s="17">
+        <v>743</v>
+      </c>
+      <c r="I83" s="18">
         <v>43951</v>
       </c>
-      <c r="J83" s="17">
+      <c r="J83" s="18">
         <v>43891</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="37.5">
@@ -6166,25 +6159,25 @@
         <v>64</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G84" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="I84" s="17">
+        <v>750</v>
+      </c>
+      <c r="I84" s="18">
         <v>44561</v>
       </c>
-      <c r="J84" s="17">
+      <c r="J84" s="18">
         <v>43525</v>
       </c>
       <c r="K84" s="3" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
@@ -6201,25 +6194,25 @@
         <v>78</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="I85" s="17">
+      <c r="I85" s="18">
         <v>44985</v>
       </c>
-      <c r="J85" s="17">
+      <c r="J85" s="18">
         <v>44562</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
@@ -6236,25 +6229,25 @@
         <v>78</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G86" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I86" s="17">
+        <v>743</v>
+      </c>
+      <c r="I86" s="18">
         <v>44985</v>
       </c>
-      <c r="J86" s="17">
+      <c r="J86" s="18">
         <v>44562</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -6271,25 +6264,25 @@
         <v>57</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G87" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="I87" s="17">
+      <c r="I87" s="18">
         <v>44347</v>
       </c>
-      <c r="J87" s="17">
+      <c r="J87" s="18">
         <v>44287</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
@@ -6306,25 +6299,25 @@
         <v>71</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G88" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="I88" s="17">
+      <c r="I88" s="18">
         <v>44773</v>
       </c>
-      <c r="J88" s="17">
+      <c r="J88" s="18">
         <v>44682</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
@@ -6345,17 +6338,17 @@
         <v>735</v>
       </c>
       <c r="G89" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H89" s="2"/>
-      <c r="I89" s="17">
+      <c r="I89" s="18">
         <v>44865</v>
       </c>
-      <c r="J89" s="17">
+      <c r="J89" s="18">
         <v>44835</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
@@ -6376,17 +6369,17 @@
         <v>735</v>
       </c>
       <c r="G90" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H90" s="2"/>
-      <c r="I90" s="17">
+      <c r="I90" s="18">
         <v>44865</v>
       </c>
-      <c r="J90" s="17">
+      <c r="J90" s="18">
         <v>44835</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
@@ -6405,17 +6398,17 @@
         <v>735</v>
       </c>
       <c r="G91" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H91" s="2"/>
-      <c r="I91" s="17" t="s">
-        <v>862</v>
-      </c>
-      <c r="J91" s="17">
+      <c r="I91" s="18" t="s">
+        <v>917</v>
+      </c>
+      <c r="J91" s="18">
         <v>44652</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
@@ -6432,23 +6425,23 @@
         <v>44</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G92" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H92" s="2"/>
-      <c r="I92" s="17">
+      <c r="I92" s="18">
         <v>43951</v>
       </c>
-      <c r="J92" s="17">
+      <c r="J92" s="18">
         <v>43070</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
@@ -6469,17 +6462,17 @@
         <v>735</v>
       </c>
       <c r="G93" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H93" s="2"/>
-      <c r="I93" s="17">
+      <c r="I93" s="18">
         <v>43373</v>
       </c>
-      <c r="J93" s="17">
+      <c r="J93" s="18">
         <v>43344</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="37.5">
@@ -6496,25 +6489,25 @@
         <v>20</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G94" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I94" s="17">
+        <v>743</v>
+      </c>
+      <c r="I94" s="18">
         <v>43220</v>
       </c>
-      <c r="J94" s="17">
+      <c r="J94" s="18">
         <v>43040</v>
       </c>
       <c r="K94" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="37.5">
@@ -6531,25 +6524,25 @@
         <v>25</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G95" s="15" t="s">
+        <v>925</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="I95" s="18">
+        <v>43373</v>
+      </c>
+      <c r="J95" s="18">
+        <v>43344</v>
+      </c>
+      <c r="K95" s="3" t="s">
         <v>926</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I95" s="17">
-        <v>43373</v>
-      </c>
-      <c r="J95" s="17">
-        <v>43344</v>
-      </c>
-      <c r="K95" s="3" t="s">
-        <v>927</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
@@ -6566,23 +6559,23 @@
         <v>78</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G96" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H96" s="2"/>
-      <c r="I96" s="17">
+      <c r="I96" s="18">
         <v>44985</v>
       </c>
-      <c r="J96" s="17">
+      <c r="J96" s="18">
         <v>44866</v>
       </c>
       <c r="K96" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
@@ -6599,25 +6592,25 @@
         <v>75</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>735</v>
       </c>
       <c r="G97" s="15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H97" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="I97" s="18">
+        <v>44895</v>
+      </c>
+      <c r="J97" s="18">
+        <v>43344</v>
+      </c>
+      <c r="K97" s="3" t="s">
         <v>931</v>
-      </c>
-      <c r="I97" s="17">
-        <v>44895</v>
-      </c>
-      <c r="J97" s="17">
-        <v>43344</v>
-      </c>
-      <c r="K97" s="3" t="s">
-        <v>932</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
@@ -6638,17 +6631,17 @@
         <v>735</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H98" s="2"/>
-      <c r="I98" s="17">
+      <c r="I98" s="18">
         <v>43281</v>
       </c>
-      <c r="J98" s="17">
+      <c r="J98" s="18">
         <v>43252</v>
       </c>
       <c r="K98" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
@@ -6669,17 +6662,17 @@
         <v>735</v>
       </c>
       <c r="G99" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H99" s="2"/>
-      <c r="I99" s="17">
+      <c r="I99" s="18">
         <v>42916</v>
       </c>
-      <c r="J99" s="17">
+      <c r="J99" s="18">
         <v>42887</v>
       </c>
       <c r="K99" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
@@ -6705,14 +6698,14 @@
         <v>729</v>
       </c>
       <c r="H100" s="2"/>
-      <c r="I100" s="17">
+      <c r="I100" s="18">
         <v>42794</v>
       </c>
-      <c r="J100" s="17">
+      <c r="J100" s="18">
         <v>42675</v>
       </c>
       <c r="K100" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>